<commit_message>
fix bugs in dataset (wrong RBS). Re-run experiments.
</commit_message>
<xml_diff>
--- a/data/First_round_results/Results - First Plate 3 reps.xlsx
+++ b/data/First_round_results/Results - First Plate 3 reps.xlsx
@@ -47,271 +47,271 @@
     <t xml:space="preserve">PERC</t>
   </si>
   <si>
-    <t xml:space="preserve">ATGTATATCTCCTTCTTAAA</t>
+    <t xml:space="preserve">TTTAAGAAGGAGATATACAT</t>
   </si>
   <si>
-    <t xml:space="preserve">ATGTATATCTCCTTCTTAAG</t>
+    <t xml:space="preserve">CTTAAGAAGGAGATATACAT</t>
   </si>
   <si>
-    <t xml:space="preserve">ATGTATATCTCCTTCTTAAC</t>
+    <t xml:space="preserve">GTTAAGAAGGAGATATACAT</t>
   </si>
   <si>
-    <t xml:space="preserve">ATGTATATCTCCTTCTTAAT</t>
+    <t xml:space="preserve">ATTAAGAAGGAGATATACAT</t>
   </si>
   <si>
-    <t xml:space="preserve">ATGTATATCTCCTTCTTAGA</t>
+    <t xml:space="preserve">TCTAAGAAGGAGATATACAT</t>
   </si>
   <si>
-    <t xml:space="preserve">ATGTATATCTCCTTCTTACA</t>
+    <t xml:space="preserve">TGTAAGAAGGAGATATACAT</t>
   </si>
   <si>
-    <t xml:space="preserve">ATGTATATCTCCTTCTTATA</t>
+    <t xml:space="preserve">TATAAGAAGGAGATATACAT</t>
   </si>
   <si>
-    <t xml:space="preserve">ATGTATATCTCCTTCTTCAA</t>
+    <t xml:space="preserve">TTGAAGAAGGAGATATACAT</t>
   </si>
   <si>
-    <t xml:space="preserve">ATGTATATCTCCTTCTTTAA</t>
+    <t xml:space="preserve">TTAAAGAAGGAGATATACAT</t>
   </si>
   <si>
-    <t xml:space="preserve">ATGTATATCTCCTTCTGAAA</t>
+    <t xml:space="preserve">TTTCAGAAGGAGATATACAT</t>
   </si>
   <si>
-    <t xml:space="preserve">ATGTATATCTCCTTCTCAAA</t>
+    <t xml:space="preserve">TTTGAGAAGGAGATATACAT</t>
   </si>
   <si>
-    <t xml:space="preserve">ATGTATATCTCCTTCTAAAA</t>
+    <t xml:space="preserve">TTTTAGAAGGAGATATACAT</t>
   </si>
   <si>
-    <t xml:space="preserve">ATGTATATCTCCTTCGTAAA</t>
+    <t xml:space="preserve">TTTACGAAGGAGATATACAT</t>
   </si>
   <si>
-    <t xml:space="preserve">ATGTATATCTCCTTCCTAAA</t>
+    <t xml:space="preserve">TTTAGGAAGGAGATATACAT</t>
   </si>
   <si>
-    <t xml:space="preserve">ATGTATATCTCCTTCATAAA</t>
+    <t xml:space="preserve">TTTATGAAGGAGATATACAT</t>
   </si>
   <si>
-    <t xml:space="preserve">ATGTATATCTCCTTGTTAAA</t>
+    <t xml:space="preserve">TTTAACAAGGAGATATACAT</t>
   </si>
   <si>
-    <t xml:space="preserve">ATGTATATCTCCTTTTTAAA</t>
+    <t xml:space="preserve">TTTAAAAAGGAGATATACAT</t>
   </si>
   <si>
-    <t xml:space="preserve">ATGTATATCTCCTTATTAAA</t>
+    <t xml:space="preserve">TTTAATAAGGAGATATACAT</t>
   </si>
   <si>
-    <t xml:space="preserve">ATGTATATCTCCTGCTTAAA</t>
+    <t xml:space="preserve">TTTAAGCAGGAGATATACAT</t>
   </si>
   <si>
-    <t xml:space="preserve">ATGTATATCTCCTCCTTAAA</t>
+    <t xml:space="preserve">TTTAAGGAGGAGATATACAT</t>
   </si>
   <si>
-    <t xml:space="preserve">ATGTATATCTCCTACTTAAA</t>
+    <t xml:space="preserve">TTTAAGTAGGAGATATACAT</t>
   </si>
   <si>
-    <t xml:space="preserve">ATGTATATCTCCGTCTTAAA</t>
+    <t xml:space="preserve">TTTAAGACGGAGATATACAT</t>
   </si>
   <si>
-    <t xml:space="preserve">ATGTATATCTCCCTCTTAAA</t>
+    <t xml:space="preserve">TTTAAGAGGGAGATATACAT</t>
   </si>
   <si>
-    <t xml:space="preserve">ATGTATATCTCCATCTTAAA</t>
+    <t xml:space="preserve">TTTAAGATGGAGATATACAT</t>
   </si>
   <si>
-    <t xml:space="preserve">ATGTATATCTCGTTCTTAAA</t>
+    <t xml:space="preserve">TTTAAGAACGAGATATACAT</t>
   </si>
   <si>
-    <t xml:space="preserve">ATGTATATCTCTTTCTTAAA</t>
+    <t xml:space="preserve">TTTAAGAAAGAGATATACAT</t>
   </si>
   <si>
-    <t xml:space="preserve">ATGTATATCTCATTCTTAAA</t>
+    <t xml:space="preserve">TTTAAGAATGAGATATACAT</t>
   </si>
   <si>
-    <t xml:space="preserve">ATGTATATCTGCTTCTTAAA</t>
+    <t xml:space="preserve">TTTAAGAAGCAGATATACAT</t>
   </si>
   <si>
-    <t xml:space="preserve">ATGTATATCTTCTTCTTAAA</t>
+    <t xml:space="preserve">TTTAAGAAGAAGATATACAT</t>
   </si>
   <si>
-    <t xml:space="preserve">ATGTATATCTACTTCTTAAA</t>
+    <t xml:space="preserve">TTTAAGAAGTAGATATACAT</t>
   </si>
   <si>
-    <t xml:space="preserve">ATGTATATCGCCTTCTTAAA</t>
+    <t xml:space="preserve">TTTAAGAAGGCGATATACAT</t>
   </si>
   <si>
-    <t xml:space="preserve">ATGTATATCCCCTTCTTAAA</t>
+    <t xml:space="preserve">TTTAAGAAGGGGATATACAT</t>
   </si>
   <si>
-    <t xml:space="preserve">ATGTATATCACCTTCTTAAA</t>
+    <t xml:space="preserve">TTTAAGAAGGTGATATACAT</t>
   </si>
   <si>
-    <t xml:space="preserve">ATGTATATGTCCTTCTTAAA</t>
+    <t xml:space="preserve">TTTAAGAAGGACATATACAT</t>
   </si>
   <si>
-    <t xml:space="preserve">ATGTATATTTCCTTCTTAAA</t>
+    <t xml:space="preserve">TTTAAGAAGGAAATATACAT</t>
   </si>
   <si>
-    <t xml:space="preserve">ATGTATATATCCTTCTTAAA</t>
+    <t xml:space="preserve">TTTAAGAAGGATATATACAT</t>
   </si>
   <si>
-    <t xml:space="preserve">ATGTATAGCTCCTTCTTAAA</t>
+    <t xml:space="preserve">TTTAAGAAGGAGCTATACAT</t>
   </si>
   <si>
-    <t xml:space="preserve">ATGTATACCTCCTTCTTAAA</t>
+    <t xml:space="preserve">TTTAAGAAGGAGGTATACAT</t>
   </si>
   <si>
-    <t xml:space="preserve">ATGTATAACTCCTTCTTAAA</t>
+    <t xml:space="preserve">TTTAAGAAGGAGTTATACAT</t>
   </si>
   <si>
-    <t xml:space="preserve">ATGTATGTCTCCTTCTTAAA</t>
+    <t xml:space="preserve">TTTAAGAAGGAGACATACAT</t>
   </si>
   <si>
-    <t xml:space="preserve">ATGTATCTCTCCTTCTTAAA</t>
+    <t xml:space="preserve">TTTAAGAAGGAGAGATACAT</t>
   </si>
   <si>
-    <t xml:space="preserve">ATGTATTTCTCCTTCTTAAA</t>
+    <t xml:space="preserve">TTTAAGAAGGAGAAATACAT</t>
   </si>
   <si>
-    <t xml:space="preserve">ATGTAGATCTCCTTCTTAAA</t>
+    <t xml:space="preserve">TTTAAGAAGGAGATCTACAT</t>
   </si>
   <si>
-    <t xml:space="preserve">ATGTACATCTCCTTCTTAAA</t>
+    <t xml:space="preserve">TTTAAGAAGGAGATGTACAT</t>
   </si>
   <si>
-    <t xml:space="preserve">ATGTAAATCTCCTTCTTAAA</t>
+    <t xml:space="preserve">TTTAAGAAGGAGATTTACAT</t>
   </si>
   <si>
-    <t xml:space="preserve">ATGTGTATCTCCTTCTTAAA</t>
+    <t xml:space="preserve">TTTAAGAAGGAGATACACAT</t>
   </si>
   <si>
-    <t xml:space="preserve">ATGTCTATCTCCTTCTTAAA</t>
+    <t xml:space="preserve">TTTAAGAAGGAGATAGACAT</t>
   </si>
   <si>
-    <t xml:space="preserve">ATGTTTATCTCCTTCTTAAA</t>
+    <t xml:space="preserve">TTTAAGAAGGAGATAAACAT</t>
   </si>
   <si>
-    <t xml:space="preserve">ATGGATATCTCCTTCTTAAA</t>
+    <t xml:space="preserve">TTTAAGAAGGAGATATCCAT</t>
   </si>
   <si>
-    <t xml:space="preserve">ATGCATATCTCCTTCTTAAA</t>
+    <t xml:space="preserve">TTTAAGAAGGAGATATGCAT</t>
   </si>
   <si>
-    <t xml:space="preserve">ATGAATATCTCCTTCTTAAA</t>
+    <t xml:space="preserve">TTTAAGAAGGAGATATTCAT</t>
   </si>
   <si>
-    <t xml:space="preserve">ATTTATATCTCCTTCTTAAA</t>
+    <t xml:space="preserve">TTTAAGAAGGAGATATAAAT</t>
   </si>
   <si>
-    <t xml:space="preserve">ATCTATATCTCCTTCTTAAA</t>
+    <t xml:space="preserve">TTTAAGAAGGAGATATAGAT</t>
   </si>
   <si>
-    <t xml:space="preserve">ATATATATCTCCTTCTTAAA</t>
+    <t xml:space="preserve">TTTAAGAAGGAGATATATAT</t>
   </si>
   <si>
-    <t xml:space="preserve">AGGTATATCTCCTTCTTAAA</t>
+    <t xml:space="preserve">TTTAAGAAGGAGATATACCT</t>
   </si>
   <si>
-    <t xml:space="preserve">ACGTATATCTCCTTCTTAAA</t>
+    <t xml:space="preserve">TTTAAGAAGGAGATATACGT</t>
   </si>
   <si>
-    <t xml:space="preserve">AAGTATATCTCCTTCTTAAA</t>
+    <t xml:space="preserve">TTTAAGAAGGAGATATACTT</t>
   </si>
   <si>
-    <t xml:space="preserve">GTGTATATCTCCTTCTTAAA</t>
+    <t xml:space="preserve">TTTAAGAAGGAGATATACAC</t>
   </si>
   <si>
-    <t xml:space="preserve">CTGTATATCTCCTTCTTAAA</t>
+    <t xml:space="preserve">TTTAAGAAGGAGATATACAG</t>
   </si>
   <si>
-    <t xml:space="preserve">TTGTATATCTCCTTCTTAAA</t>
+    <t xml:space="preserve">TTTAAGAAGGAGATATACAA</t>
   </si>
   <si>
-    <t xml:space="preserve">ATGTATAGTCAACTCTTAAA</t>
+    <t xml:space="preserve">TTTAAGAGTTGACTATACAT</t>
   </si>
   <si>
-    <t xml:space="preserve">ATGTATACAGGTATCTTAAA</t>
+    <t xml:space="preserve">TTTAAGATACCTGTATACAT</t>
   </si>
   <si>
-    <t xml:space="preserve">ATGTATACGCTTCTCTTAAA</t>
+    <t xml:space="preserve">TTTAAGAGAAGCGTATACAT</t>
   </si>
   <si>
-    <t xml:space="preserve">ATGTATAGCATACTCTTAAA</t>
+    <t xml:space="preserve">TTTAAGAGTATGCTATACAT</t>
   </si>
   <si>
-    <t xml:space="preserve">ATGTATAAAGTGATCTTAAA</t>
+    <t xml:space="preserve">TTTAAGATCACTTTATACAT</t>
   </si>
   <si>
-    <t xml:space="preserve">ATGTATAGGCTTCTCTTAAA</t>
+    <t xml:space="preserve">TTTAAGAGAAGCCTATACAT</t>
   </si>
   <si>
-    <t xml:space="preserve">ATGTATATTCTATTCTTAAA</t>
+    <t xml:space="preserve">TTTAAGAATAGAATATACAT</t>
   </si>
   <si>
-    <t xml:space="preserve">ATGTATAGTCAGATCTTAAA</t>
+    <t xml:space="preserve">TTTAAGATCTGACTATACAT</t>
   </si>
   <si>
-    <t xml:space="preserve">ATGTATATACTTATCTTAAA</t>
+    <t xml:space="preserve">TTTAAGATAAGTATATACAT</t>
   </si>
   <si>
-    <t xml:space="preserve">ATGTATATTTATCTCTTAAA</t>
+    <t xml:space="preserve">TTTAAGAGATAAATATACAT</t>
   </si>
   <si>
-    <t xml:space="preserve">ATGTATATTGACCTCTTAAA</t>
+    <t xml:space="preserve">TTTAAGAGGTCAATATACAT</t>
   </si>
   <si>
-    <t xml:space="preserve">ATGTATAGGATCGTCTTAAA</t>
+    <t xml:space="preserve">TTTAAGACGATCCTATACAT</t>
   </si>
   <si>
-    <t xml:space="preserve">ATGTATAGTCTGTTCTTAAA</t>
+    <t xml:space="preserve">TTTAAGAACAGACTATACAT</t>
   </si>
   <si>
-    <t xml:space="preserve">ATGTATATATAACTCTTAAA</t>
+    <t xml:space="preserve">TTTAAGAGTTATATATACAT</t>
   </si>
   <si>
-    <t xml:space="preserve">ATGTATATGTTCCTCTTAAA</t>
+    <t xml:space="preserve">TTTAAGAGGAACATATACAT</t>
   </si>
   <si>
-    <t xml:space="preserve">ATGTATATTCGGGTCTTAAA</t>
+    <t xml:space="preserve">TTTAAGACCCGAATATACAT</t>
   </si>
   <si>
-    <t xml:space="preserve">ATGTATAGACATTTCTTAAA</t>
+    <t xml:space="preserve">TTTAAGAAATGTCTATACAT</t>
   </si>
   <si>
-    <t xml:space="preserve">ATGTATAGGTACGTCTTAAA</t>
+    <t xml:space="preserve">TTTAAGACGTACCTATACAT</t>
   </si>
   <si>
-    <t xml:space="preserve">ATGTATACACGGTTCTTAAA</t>
+    <t xml:space="preserve">TTTAAGAACCGTGTATACAT</t>
   </si>
   <si>
-    <t xml:space="preserve">ATGTATAGTGTCCTCTTAAA</t>
+    <t xml:space="preserve">TTTAAGAGGACACTATACAT</t>
   </si>
   <si>
-    <t xml:space="preserve">ATGTATATGGGATTCTTAAA</t>
+    <t xml:space="preserve">TTTAAGAATCCCATATACAT</t>
   </si>
   <si>
-    <t xml:space="preserve">ATGTATATCGCTCTCTTAAA</t>
+    <t xml:space="preserve">TTTAAGAGAGCGATATACAT</t>
   </si>
   <si>
-    <t xml:space="preserve">ATGTATAGCATATTCTTAAA</t>
+    <t xml:space="preserve">TTTAAGAATATGCTATACAT</t>
   </si>
   <si>
-    <t xml:space="preserve">ATGTATAATGTTGTCTTAAA</t>
+    <t xml:space="preserve">TTTAAGACAACATTATACAT</t>
   </si>
   <si>
-    <t xml:space="preserve">ATGTATATGTAGCTCTTAAA</t>
+    <t xml:space="preserve">TTTAAGAGCTACATATACAT</t>
   </si>
   <si>
-    <t xml:space="preserve">ATGTATAGTCTTCTCTTAAA</t>
+    <t xml:space="preserve">TTTAAGAGAAGACTATACAT</t>
   </si>
   <si>
-    <t xml:space="preserve">ATGTATAACGGAGTCTTAAA</t>
+    <t xml:space="preserve">TTTAAGACTCCGTTATACAT</t>
   </si>
   <si>
-    <t xml:space="preserve">ATGTATATAGTAATCTTAAA</t>
+    <t xml:space="preserve">TTTAAGATTACTATATACAT</t>
   </si>
   <si>
-    <t xml:space="preserve">ATGTATAGTCTCGTCTTAAA</t>
+    <t xml:space="preserve">TTTAAGACGAGACTATACAT</t>
   </si>
 </sst>
 </file>
@@ -322,7 +322,7 @@
     <numFmt numFmtId="164" formatCode="General"/>
     <numFmt numFmtId="165" formatCode="0.00%"/>
   </numFmts>
-  <fonts count="6">
+  <fonts count="7">
     <font>
       <sz val="11"/>
       <color rgb="FF000000"/>
@@ -350,6 +350,13 @@
       <sz val="11"/>
       <color rgb="FF000000"/>
       <name val="Calibri"/>
+      <family val="2"/>
+      <charset val="1"/>
+    </font>
+    <font>
+      <sz val="10"/>
+      <color rgb="FF000000"/>
+      <name val="Arial Unicode MS"/>
       <family val="2"/>
       <charset val="1"/>
     </font>
@@ -428,15 +435,15 @@
       <alignment horizontal="center" vertical="top" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="center" vertical="top" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+    <xf numFmtId="164" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
     <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -467,13 +474,13 @@
   </sheetPr>
   <dimension ref="A1:DJ91"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A13" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="A2" activeCellId="0" sqref="A2"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="39.57"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="39.55"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1025" min="2" style="0" width="8.53"/>
   </cols>
   <sheetData>
@@ -496,32 +503,32 @@
       <c r="F1" s="0" t="s">
         <v>5</v>
       </c>
-      <c r="G1" s="3" t="s">
+      <c r="G1" s="2" t="s">
         <v>6</v>
       </c>
       <c r="K1" s="1"/>
       <c r="L1" s="1"/>
       <c r="M1" s="1"/>
       <c r="N1" s="2"/>
-      <c r="P1" s="3"/>
+      <c r="P1" s="2"/>
       <c r="S1" s="1"/>
       <c r="T1" s="1"/>
       <c r="U1" s="1"/>
       <c r="V1" s="2"/>
-      <c r="X1" s="3"/>
+      <c r="X1" s="2"/>
       <c r="AA1" s="1"/>
       <c r="AB1" s="1"/>
       <c r="AC1" s="1"/>
       <c r="AD1" s="2"/>
-      <c r="AF1" s="3"/>
+      <c r="AF1" s="2"/>
       <c r="AI1" s="1"/>
       <c r="AJ1" s="1"/>
       <c r="AK1" s="1"/>
       <c r="AL1" s="2"/>
-      <c r="AN1" s="3"/>
+      <c r="AN1" s="2"/>
     </row>
     <row r="2" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A2" s="1" t="s">
+      <c r="A2" s="3" t="s">
         <v>7</v>
       </c>
       <c r="B2" s="0" t="n">
@@ -563,7 +570,7 @@
       <c r="AN2" s="4"/>
     </row>
     <row r="3" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A3" s="1" t="s">
+      <c r="A3" s="3" t="s">
         <v>8</v>
       </c>
       <c r="B3" s="0" t="n">
@@ -674,7 +681,7 @@
       <c r="DC3" s="6"/>
     </row>
     <row r="4" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A4" s="1" t="s">
+      <c r="A4" s="3" t="s">
         <v>9</v>
       </c>
       <c r="B4" s="0" t="n">
@@ -787,7 +794,7 @@
       <c r="DE4" s="6"/>
     </row>
     <row r="5" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A5" s="1" t="s">
+      <c r="A5" s="3" t="s">
         <v>10</v>
       </c>
       <c r="B5" s="0" t="n">
@@ -904,7 +911,7 @@
       <c r="DJ5" s="6"/>
     </row>
     <row r="6" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A6" s="1" t="s">
+      <c r="A6" s="3" t="s">
         <v>11</v>
       </c>
       <c r="B6" s="0" t="n">
@@ -946,7 +953,7 @@
       <c r="AN6" s="4"/>
     </row>
     <row r="7" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A7" s="1" t="s">
+      <c r="A7" s="3" t="s">
         <v>12</v>
       </c>
       <c r="B7" s="0" t="n">
@@ -1058,7 +1065,7 @@
       <c r="DD7" s="6"/>
     </row>
     <row r="8" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A8" s="1" t="s">
+      <c r="A8" s="3" t="s">
         <v>13</v>
       </c>
       <c r="B8" s="0" t="n">
@@ -1100,7 +1107,7 @@
       <c r="AN8" s="4"/>
     </row>
     <row r="9" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A9" s="1" t="s">
+      <c r="A9" s="3" t="s">
         <v>14</v>
       </c>
       <c r="B9" s="0" t="n">
@@ -1142,7 +1149,7 @@
       <c r="AN9" s="4"/>
     </row>
     <row r="10" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A10" s="1" t="s">
+      <c r="A10" s="3" t="s">
         <v>15</v>
       </c>
       <c r="B10" s="0" t="n">
@@ -1184,7 +1191,7 @@
       <c r="AN10" s="4"/>
     </row>
     <row r="11" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A11" s="1" t="s">
+      <c r="A11" s="3" t="s">
         <v>16</v>
       </c>
       <c r="B11" s="0" t="n">
@@ -1226,7 +1233,7 @@
       <c r="AN11" s="4"/>
     </row>
     <row r="12" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A12" s="1" t="s">
+      <c r="A12" s="3" t="s">
         <v>17</v>
       </c>
       <c r="B12" s="0" t="n">
@@ -1268,7 +1275,7 @@
       <c r="AN12" s="4"/>
     </row>
     <row r="13" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A13" s="1" t="s">
+      <c r="A13" s="3" t="s">
         <v>18</v>
       </c>
       <c r="B13" s="0" t="n">
@@ -1310,7 +1317,7 @@
       <c r="AN13" s="4"/>
     </row>
     <row r="14" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A14" s="1" t="s">
+      <c r="A14" s="3" t="s">
         <v>19</v>
       </c>
       <c r="B14" s="0" t="n">
@@ -1352,7 +1359,7 @@
       <c r="AN14" s="4"/>
     </row>
     <row r="15" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A15" s="1" t="s">
+      <c r="A15" s="3" t="s">
         <v>20</v>
       </c>
       <c r="B15" s="0" t="n">
@@ -1394,7 +1401,7 @@
       <c r="AN15" s="4"/>
     </row>
     <row r="16" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A16" s="1" t="s">
+      <c r="A16" s="3" t="s">
         <v>21</v>
       </c>
       <c r="B16" s="0" t="n">
@@ -1436,7 +1443,7 @@
       <c r="AN16" s="4"/>
     </row>
     <row r="17" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A17" s="1" t="s">
+      <c r="A17" s="3" t="s">
         <v>22</v>
       </c>
       <c r="B17" s="0" t="n">
@@ -1478,7 +1485,7 @@
       <c r="AN17" s="4"/>
     </row>
     <row r="18" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A18" s="1" t="s">
+      <c r="A18" s="3" t="s">
         <v>23</v>
       </c>
       <c r="B18" s="0" t="n">
@@ -1520,7 +1527,7 @@
       <c r="AN18" s="4"/>
     </row>
     <row r="19" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A19" s="1" t="s">
+      <c r="A19" s="3" t="s">
         <v>24</v>
       </c>
       <c r="B19" s="0" t="n">
@@ -1562,7 +1569,7 @@
       <c r="AN19" s="4"/>
     </row>
     <row r="20" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A20" s="1" t="s">
+      <c r="A20" s="3" t="s">
         <v>25</v>
       </c>
       <c r="B20" s="0" t="n">
@@ -1604,7 +1611,7 @@
       <c r="AN20" s="4"/>
     </row>
     <row r="21" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A21" s="1" t="s">
+      <c r="A21" s="3" t="s">
         <v>26</v>
       </c>
       <c r="B21" s="0" t="n">
@@ -1646,7 +1653,7 @@
       <c r="AN21" s="4"/>
     </row>
     <row r="22" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A22" s="1" t="s">
+      <c r="A22" s="3" t="s">
         <v>27</v>
       </c>
       <c r="B22" s="0" t="n">
@@ -1688,7 +1695,7 @@
       <c r="AN22" s="4"/>
     </row>
     <row r="23" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A23" s="1" t="s">
+      <c r="A23" s="3" t="s">
         <v>28</v>
       </c>
       <c r="B23" s="0" t="n">
@@ -1730,7 +1737,7 @@
       <c r="AN23" s="4"/>
     </row>
     <row r="24" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A24" s="1" t="s">
+      <c r="A24" s="3" t="s">
         <v>29</v>
       </c>
       <c r="B24" s="0" t="n">
@@ -1772,7 +1779,7 @@
       <c r="AN24" s="4"/>
     </row>
     <row r="25" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A25" s="1" t="s">
+      <c r="A25" s="3" t="s">
         <v>30</v>
       </c>
       <c r="B25" s="0" t="n">
@@ -1814,7 +1821,7 @@
       <c r="AN25" s="4"/>
     </row>
     <row r="26" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A26" s="1" t="s">
+      <c r="A26" s="3" t="s">
         <v>31</v>
       </c>
       <c r="B26" s="0" t="n">
@@ -1856,7 +1863,7 @@
       <c r="AN26" s="4"/>
     </row>
     <row r="27" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A27" s="1" t="s">
+      <c r="A27" s="3" t="s">
         <v>32</v>
       </c>
       <c r="B27" s="0" t="n">
@@ -1898,7 +1905,7 @@
       <c r="AN27" s="4"/>
     </row>
     <row r="28" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A28" s="1" t="s">
+      <c r="A28" s="3" t="s">
         <v>33</v>
       </c>
       <c r="B28" s="0" t="n">
@@ -1940,7 +1947,7 @@
       <c r="AN28" s="4"/>
     </row>
     <row r="29" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A29" s="1" t="s">
+      <c r="A29" s="3" t="s">
         <v>34</v>
       </c>
       <c r="B29" s="0" t="n">
@@ -1982,7 +1989,7 @@
       <c r="AN29" s="4"/>
     </row>
     <row r="30" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A30" s="1" t="s">
+      <c r="A30" s="3" t="s">
         <v>35</v>
       </c>
       <c r="B30" s="0" t="n">
@@ -2024,7 +2031,7 @@
       <c r="AN30" s="4"/>
     </row>
     <row r="31" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A31" s="1" t="s">
+      <c r="A31" s="3" t="s">
         <v>36</v>
       </c>
       <c r="B31" s="0" t="n">
@@ -2066,7 +2073,7 @@
       <c r="AN31" s="4"/>
     </row>
     <row r="32" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A32" s="1" t="s">
+      <c r="A32" s="3" t="s">
         <v>37</v>
       </c>
       <c r="B32" s="0" t="n">
@@ -2108,7 +2115,7 @@
       <c r="AN32" s="4"/>
     </row>
     <row r="33" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A33" s="1" t="s">
+      <c r="A33" s="3" t="s">
         <v>38</v>
       </c>
       <c r="B33" s="0" t="n">
@@ -2150,7 +2157,7 @@
       <c r="AN33" s="4"/>
     </row>
     <row r="34" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A34" s="1" t="s">
+      <c r="A34" s="3" t="s">
         <v>39</v>
       </c>
       <c r="B34" s="0" t="n">
@@ -2192,7 +2199,7 @@
       <c r="AN34" s="4"/>
     </row>
     <row r="35" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A35" s="1" t="s">
+      <c r="A35" s="3" t="s">
         <v>40</v>
       </c>
       <c r="B35" s="0" t="n">
@@ -2234,7 +2241,7 @@
       <c r="AN35" s="4"/>
     </row>
     <row r="36" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A36" s="1" t="s">
+      <c r="A36" s="3" t="s">
         <v>41</v>
       </c>
       <c r="B36" s="0" t="n">
@@ -2276,7 +2283,7 @@
       <c r="AN36" s="4"/>
     </row>
     <row r="37" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A37" s="1" t="s">
+      <c r="A37" s="3" t="s">
         <v>42</v>
       </c>
       <c r="B37" s="0" t="n">
@@ -2318,7 +2325,7 @@
       <c r="AN37" s="4"/>
     </row>
     <row r="38" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A38" s="1" t="s">
+      <c r="A38" s="3" t="s">
         <v>43</v>
       </c>
       <c r="B38" s="0" t="n">
@@ -2360,7 +2367,7 @@
       <c r="AN38" s="4"/>
     </row>
     <row r="39" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A39" s="1" t="s">
+      <c r="A39" s="3" t="s">
         <v>44</v>
       </c>
       <c r="B39" s="0" t="n">
@@ -2402,7 +2409,7 @@
       <c r="AN39" s="4"/>
     </row>
     <row r="40" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A40" s="1" t="s">
+      <c r="A40" s="3" t="s">
         <v>45</v>
       </c>
       <c r="B40" s="0" t="n">
@@ -2444,7 +2451,7 @@
       <c r="AN40" s="4"/>
     </row>
     <row r="41" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A41" s="1" t="s">
+      <c r="A41" s="3" t="s">
         <v>46</v>
       </c>
       <c r="B41" s="0" t="n">
@@ -2486,7 +2493,7 @@
       <c r="AN41" s="4"/>
     </row>
     <row r="42" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A42" s="1" t="s">
+      <c r="A42" s="3" t="s">
         <v>47</v>
       </c>
       <c r="B42" s="0" t="n">
@@ -2528,7 +2535,7 @@
       <c r="AN42" s="4"/>
     </row>
     <row r="43" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A43" s="1" t="s">
+      <c r="A43" s="3" t="s">
         <v>48</v>
       </c>
       <c r="B43" s="0" t="n">
@@ -2570,7 +2577,7 @@
       <c r="AN43" s="4"/>
     </row>
     <row r="44" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A44" s="1" t="s">
+      <c r="A44" s="3" t="s">
         <v>49</v>
       </c>
       <c r="B44" s="0" t="n">
@@ -2612,7 +2619,7 @@
       <c r="AN44" s="4"/>
     </row>
     <row r="45" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A45" s="1" t="s">
+      <c r="A45" s="3" t="s">
         <v>50</v>
       </c>
       <c r="B45" s="0" t="n">
@@ -2654,7 +2661,7 @@
       <c r="AN45" s="4"/>
     </row>
     <row r="46" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A46" s="1" t="s">
+      <c r="A46" s="3" t="s">
         <v>51</v>
       </c>
       <c r="B46" s="0" t="n">
@@ -2696,7 +2703,7 @@
       <c r="AN46" s="4"/>
     </row>
     <row r="47" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A47" s="1" t="s">
+      <c r="A47" s="3" t="s">
         <v>52</v>
       </c>
       <c r="B47" s="0" t="n">
@@ -2738,7 +2745,7 @@
       <c r="AN47" s="4"/>
     </row>
     <row r="48" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A48" s="1" t="s">
+      <c r="A48" s="3" t="s">
         <v>53</v>
       </c>
       <c r="B48" s="0" t="n">
@@ -2780,7 +2787,7 @@
       <c r="AN48" s="4"/>
     </row>
     <row r="49" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A49" s="1" t="s">
+      <c r="A49" s="3" t="s">
         <v>54</v>
       </c>
       <c r="B49" s="0" t="n">
@@ -2822,7 +2829,7 @@
       <c r="AN49" s="4"/>
     </row>
     <row r="50" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A50" s="1" t="s">
+      <c r="A50" s="3" t="s">
         <v>55</v>
       </c>
       <c r="B50" s="0" t="n">
@@ -2864,7 +2871,7 @@
       <c r="AN50" s="4"/>
     </row>
     <row r="51" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A51" s="1" t="s">
+      <c r="A51" s="3" t="s">
         <v>56</v>
       </c>
       <c r="B51" s="0" t="n">
@@ -2906,7 +2913,7 @@
       <c r="AN51" s="4"/>
     </row>
     <row r="52" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A52" s="1" t="s">
+      <c r="A52" s="3" t="s">
         <v>57</v>
       </c>
       <c r="B52" s="0" t="n">
@@ -2948,7 +2955,7 @@
       <c r="AN52" s="4"/>
     </row>
     <row r="53" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A53" s="1" t="s">
+      <c r="A53" s="3" t="s">
         <v>58</v>
       </c>
       <c r="B53" s="0" t="n">
@@ -2990,7 +2997,7 @@
       <c r="AN53" s="4"/>
     </row>
     <row r="54" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A54" s="1" t="s">
+      <c r="A54" s="3" t="s">
         <v>59</v>
       </c>
       <c r="B54" s="0" t="n">
@@ -3032,7 +3039,7 @@
       <c r="AN54" s="4"/>
     </row>
     <row r="55" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A55" s="1" t="s">
+      <c r="A55" s="3" t="s">
         <v>60</v>
       </c>
       <c r="B55" s="0" t="n">
@@ -3074,7 +3081,7 @@
       <c r="AN55" s="4"/>
     </row>
     <row r="56" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A56" s="1" t="s">
+      <c r="A56" s="3" t="s">
         <v>61</v>
       </c>
       <c r="B56" s="0" t="n">
@@ -3116,7 +3123,7 @@
       <c r="AN56" s="4"/>
     </row>
     <row r="57" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A57" s="1" t="s">
+      <c r="A57" s="3" t="s">
         <v>62</v>
       </c>
       <c r="B57" s="0" t="n">
@@ -3158,7 +3165,7 @@
       <c r="AN57" s="4"/>
     </row>
     <row r="58" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A58" s="1" t="s">
+      <c r="A58" s="3" t="s">
         <v>63</v>
       </c>
       <c r="B58" s="0" t="n">
@@ -3200,7 +3207,7 @@
       <c r="AN58" s="4"/>
     </row>
     <row r="59" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A59" s="1" t="s">
+      <c r="A59" s="3" t="s">
         <v>64</v>
       </c>
       <c r="B59" s="0" t="n">
@@ -3242,7 +3249,7 @@
       <c r="AN59" s="4"/>
     </row>
     <row r="60" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A60" s="1" t="s">
+      <c r="A60" s="3" t="s">
         <v>65</v>
       </c>
       <c r="B60" s="0" t="n">
@@ -3284,7 +3291,7 @@
       <c r="AN60" s="4"/>
     </row>
     <row r="61" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A61" s="1" t="s">
+      <c r="A61" s="3" t="s">
         <v>66</v>
       </c>
       <c r="B61" s="0" t="n">
@@ -3326,7 +3333,7 @@
       <c r="AN61" s="4"/>
     </row>
     <row r="62" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A62" s="1" t="s">
+      <c r="A62" s="3" t="s">
         <v>67</v>
       </c>
       <c r="B62" s="0" t="n">
@@ -3368,7 +3375,7 @@
       <c r="AN62" s="4"/>
     </row>
     <row r="63" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A63" s="1" t="s">
+      <c r="A63" s="3" t="s">
         <v>68</v>
       </c>
       <c r="B63" s="0" t="n">
@@ -3410,7 +3417,7 @@
       <c r="AN63" s="4"/>
     </row>
     <row r="64" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A64" s="1" t="s">
+      <c r="A64" s="3" t="s">
         <v>69</v>
       </c>
       <c r="B64" s="0" t="n">
@@ -3452,7 +3459,7 @@
       <c r="AN64" s="4"/>
     </row>
     <row r="65" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A65" s="1" t="s">
+      <c r="A65" s="3" t="s">
         <v>70</v>
       </c>
       <c r="B65" s="0" t="n">
@@ -3494,7 +3501,7 @@
       <c r="AN65" s="4"/>
     </row>
     <row r="66" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A66" s="1" t="s">
+      <c r="A66" s="3" t="s">
         <v>71</v>
       </c>
       <c r="B66" s="0" t="n">
@@ -3536,7 +3543,7 @@
       <c r="AN66" s="4"/>
     </row>
     <row r="67" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A67" s="1" t="s">
+      <c r="A67" s="3" t="s">
         <v>72</v>
       </c>
       <c r="B67" s="0" t="n">
@@ -3578,7 +3585,7 @@
       <c r="AN67" s="4"/>
     </row>
     <row r="68" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A68" s="1" t="s">
+      <c r="A68" s="3" t="s">
         <v>73</v>
       </c>
       <c r="B68" s="0" t="n">
@@ -3620,7 +3627,7 @@
       <c r="AN68" s="4"/>
     </row>
     <row r="69" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A69" s="1" t="s">
+      <c r="A69" s="3" t="s">
         <v>74</v>
       </c>
       <c r="B69" s="0" t="n">
@@ -3662,7 +3669,7 @@
       <c r="AN69" s="4"/>
     </row>
     <row r="70" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A70" s="1" t="s">
+      <c r="A70" s="3" t="s">
         <v>75</v>
       </c>
       <c r="B70" s="0" t="n">
@@ -3704,7 +3711,7 @@
       <c r="AN70" s="4"/>
     </row>
     <row r="71" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A71" s="1" t="s">
+      <c r="A71" s="3" t="s">
         <v>76</v>
       </c>
       <c r="B71" s="0" t="n">
@@ -3746,7 +3753,7 @@
       <c r="AN71" s="4"/>
     </row>
     <row r="72" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A72" s="1" t="s">
+      <c r="A72" s="3" t="s">
         <v>77</v>
       </c>
       <c r="B72" s="0" t="n">
@@ -3788,7 +3795,7 @@
       <c r="AN72" s="4"/>
     </row>
     <row r="73" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A73" s="1" t="s">
+      <c r="A73" s="3" t="s">
         <v>78</v>
       </c>
       <c r="B73" s="0" t="n">
@@ -3830,7 +3837,7 @@
       <c r="AN73" s="4"/>
     </row>
     <row r="74" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A74" s="1" t="s">
+      <c r="A74" s="3" t="s">
         <v>79</v>
       </c>
       <c r="B74" s="0" t="n">
@@ -3872,7 +3879,7 @@
       <c r="AN74" s="4"/>
     </row>
     <row r="75" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A75" s="1" t="s">
+      <c r="A75" s="3" t="s">
         <v>80</v>
       </c>
       <c r="B75" s="0" t="n">
@@ -3914,7 +3921,7 @@
       <c r="AN75" s="4"/>
     </row>
     <row r="76" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A76" s="1" t="s">
+      <c r="A76" s="3" t="s">
         <v>81</v>
       </c>
       <c r="B76" s="0" t="n">
@@ -3956,7 +3963,7 @@
       <c r="AN76" s="4"/>
     </row>
     <row r="77" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A77" s="1" t="s">
+      <c r="A77" s="3" t="s">
         <v>82</v>
       </c>
       <c r="B77" s="0" t="n">
@@ -3998,7 +4005,7 @@
       <c r="AN77" s="4"/>
     </row>
     <row r="78" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A78" s="1" t="s">
+      <c r="A78" s="3" t="s">
         <v>83</v>
       </c>
       <c r="B78" s="0" t="n">
@@ -4040,7 +4047,7 @@
       <c r="AN78" s="4"/>
     </row>
     <row r="79" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A79" s="1" t="s">
+      <c r="A79" s="3" t="s">
         <v>84</v>
       </c>
       <c r="B79" s="0" t="n">
@@ -4082,7 +4089,7 @@
       <c r="AN79" s="4"/>
     </row>
     <row r="80" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A80" s="1" t="s">
+      <c r="A80" s="3" t="s">
         <v>85</v>
       </c>
       <c r="B80" s="0" t="n">
@@ -4124,7 +4131,7 @@
       <c r="AN80" s="4"/>
     </row>
     <row r="81" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A81" s="1" t="s">
+      <c r="A81" s="3" t="s">
         <v>86</v>
       </c>
       <c r="B81" s="0" t="n">
@@ -4166,7 +4173,7 @@
       <c r="AN81" s="4"/>
     </row>
     <row r="82" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A82" s="1" t="s">
+      <c r="A82" s="3" t="s">
         <v>87</v>
       </c>
       <c r="B82" s="0" t="n">
@@ -4208,7 +4215,7 @@
       <c r="AN82" s="4"/>
     </row>
     <row r="83" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A83" s="1" t="s">
+      <c r="A83" s="3" t="s">
         <v>88</v>
       </c>
       <c r="B83" s="0" t="n">
@@ -4250,7 +4257,7 @@
       <c r="AN83" s="4"/>
     </row>
     <row r="84" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A84" s="1" t="s">
+      <c r="A84" s="3" t="s">
         <v>89</v>
       </c>
       <c r="B84" s="0" t="n">
@@ -4292,7 +4299,7 @@
       <c r="AN84" s="4"/>
     </row>
     <row r="85" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A85" s="1" t="s">
+      <c r="A85" s="3" t="s">
         <v>90</v>
       </c>
       <c r="B85" s="0" t="n">
@@ -4334,7 +4341,7 @@
       <c r="AN85" s="4"/>
     </row>
     <row r="86" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A86" s="1" t="s">
+      <c r="A86" s="3" t="s">
         <v>91</v>
       </c>
       <c r="B86" s="0" t="n">
@@ -4376,7 +4383,7 @@
       <c r="AN86" s="4"/>
     </row>
     <row r="87" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A87" s="1" t="s">
+      <c r="A87" s="3" t="s">
         <v>92</v>
       </c>
       <c r="B87" s="0" t="n">
@@ -4418,7 +4425,7 @@
       <c r="AN87" s="4"/>
     </row>
     <row r="88" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A88" s="1" t="s">
+      <c r="A88" s="3" t="s">
         <v>93</v>
       </c>
       <c r="B88" s="0" t="n">
@@ -4460,7 +4467,7 @@
       <c r="AN88" s="4"/>
     </row>
     <row r="89" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A89" s="1" t="s">
+      <c r="A89" s="3" t="s">
         <v>94</v>
       </c>
       <c r="B89" s="0" t="n">
@@ -4502,7 +4509,7 @@
       <c r="AN89" s="4"/>
     </row>
     <row r="90" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A90" s="1" t="s">
+      <c r="A90" s="3" t="s">
         <v>95</v>
       </c>
       <c r="B90" s="0" t="n">
@@ -4581,7 +4588,7 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="25.5"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="39.55"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="7" min="2" style="0" width="8.53"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1025" min="8" style="0" width="9.14"/>
   </cols>
@@ -4605,12 +4612,12 @@
       <c r="F1" s="0" t="s">
         <v>5</v>
       </c>
-      <c r="G1" s="3" t="s">
+      <c r="G1" s="2" t="s">
         <v>6</v>
       </c>
     </row>
     <row r="2" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A2" s="1" t="s">
+      <c r="A2" s="3" t="s">
         <v>7</v>
       </c>
       <c r="B2" s="5" t="n">
@@ -4636,7 +4643,7 @@
       </c>
     </row>
     <row r="3" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A3" s="1" t="s">
+      <c r="A3" s="3" t="s">
         <v>8</v>
       </c>
       <c r="B3" s="5" t="n">
@@ -4662,7 +4669,7 @@
       </c>
     </row>
     <row r="4" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A4" s="1" t="s">
+      <c r="A4" s="3" t="s">
         <v>9</v>
       </c>
       <c r="B4" s="5" t="n">
@@ -4688,7 +4695,7 @@
       </c>
     </row>
     <row r="5" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A5" s="1" t="s">
+      <c r="A5" s="3" t="s">
         <v>10</v>
       </c>
       <c r="B5" s="5" t="n">
@@ -4714,7 +4721,7 @@
       </c>
     </row>
     <row r="6" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A6" s="1" t="s">
+      <c r="A6" s="3" t="s">
         <v>11</v>
       </c>
       <c r="B6" s="5" t="n">
@@ -4740,7 +4747,7 @@
       </c>
     </row>
     <row r="7" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A7" s="1" t="s">
+      <c r="A7" s="3" t="s">
         <v>12</v>
       </c>
       <c r="B7" s="5" t="n">
@@ -4766,7 +4773,7 @@
       </c>
     </row>
     <row r="8" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A8" s="1" t="s">
+      <c r="A8" s="3" t="s">
         <v>13</v>
       </c>
       <c r="B8" s="5" t="n">
@@ -4792,7 +4799,7 @@
       </c>
     </row>
     <row r="9" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A9" s="1" t="s">
+      <c r="A9" s="3" t="s">
         <v>14</v>
       </c>
       <c r="B9" s="5" t="n">
@@ -4818,7 +4825,7 @@
       </c>
     </row>
     <row r="10" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A10" s="1" t="s">
+      <c r="A10" s="3" t="s">
         <v>15</v>
       </c>
       <c r="B10" s="5" t="n">
@@ -4844,7 +4851,7 @@
       </c>
     </row>
     <row r="11" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A11" s="1" t="s">
+      <c r="A11" s="3" t="s">
         <v>16</v>
       </c>
       <c r="B11" s="5" t="n">
@@ -4870,7 +4877,7 @@
       </c>
     </row>
     <row r="12" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A12" s="1" t="s">
+      <c r="A12" s="3" t="s">
         <v>17</v>
       </c>
       <c r="B12" s="5" t="n">
@@ -4896,7 +4903,7 @@
       </c>
     </row>
     <row r="13" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A13" s="1" t="s">
+      <c r="A13" s="3" t="s">
         <v>18</v>
       </c>
       <c r="B13" s="5" t="n">
@@ -4922,7 +4929,7 @@
       </c>
     </row>
     <row r="14" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A14" s="1" t="s">
+      <c r="A14" s="3" t="s">
         <v>19</v>
       </c>
       <c r="B14" s="5" t="n">
@@ -4948,7 +4955,7 @@
       </c>
     </row>
     <row r="15" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A15" s="1" t="s">
+      <c r="A15" s="3" t="s">
         <v>20</v>
       </c>
       <c r="B15" s="5" t="n">
@@ -4974,7 +4981,7 @@
       </c>
     </row>
     <row r="16" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A16" s="1" t="s">
+      <c r="A16" s="3" t="s">
         <v>21</v>
       </c>
       <c r="B16" s="5" t="n">
@@ -5000,7 +5007,7 @@
       </c>
     </row>
     <row r="17" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A17" s="1" t="s">
+      <c r="A17" s="3" t="s">
         <v>22</v>
       </c>
       <c r="B17" s="5" t="n">
@@ -5026,7 +5033,7 @@
       </c>
     </row>
     <row r="18" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A18" s="1" t="s">
+      <c r="A18" s="3" t="s">
         <v>23</v>
       </c>
       <c r="B18" s="5" t="n">
@@ -5052,7 +5059,7 @@
       </c>
     </row>
     <row r="19" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A19" s="1" t="s">
+      <c r="A19" s="3" t="s">
         <v>24</v>
       </c>
       <c r="B19" s="5" t="n">
@@ -5078,7 +5085,7 @@
       </c>
     </row>
     <row r="20" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A20" s="1" t="s">
+      <c r="A20" s="3" t="s">
         <v>25</v>
       </c>
       <c r="B20" s="5" t="n">
@@ -5104,7 +5111,7 @@
       </c>
     </row>
     <row r="21" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A21" s="1" t="s">
+      <c r="A21" s="3" t="s">
         <v>26</v>
       </c>
       <c r="B21" s="5" t="n">
@@ -5130,7 +5137,7 @@
       </c>
     </row>
     <row r="22" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A22" s="1" t="s">
+      <c r="A22" s="3" t="s">
         <v>27</v>
       </c>
       <c r="B22" s="5" t="n">
@@ -5156,7 +5163,7 @@
       </c>
     </row>
     <row r="23" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A23" s="1" t="s">
+      <c r="A23" s="3" t="s">
         <v>28</v>
       </c>
       <c r="B23" s="5" t="n">
@@ -5182,7 +5189,7 @@
       </c>
     </row>
     <row r="24" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A24" s="1" t="s">
+      <c r="A24" s="3" t="s">
         <v>29</v>
       </c>
       <c r="B24" s="5" t="n">
@@ -5208,7 +5215,7 @@
       </c>
     </row>
     <row r="25" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A25" s="1" t="s">
+      <c r="A25" s="3" t="s">
         <v>30</v>
       </c>
       <c r="B25" s="5" t="n">
@@ -5234,7 +5241,7 @@
       </c>
     </row>
     <row r="26" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A26" s="1" t="s">
+      <c r="A26" s="3" t="s">
         <v>31</v>
       </c>
       <c r="B26" s="5" t="n">
@@ -5260,7 +5267,7 @@
       </c>
     </row>
     <row r="27" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A27" s="1" t="s">
+      <c r="A27" s="3" t="s">
         <v>32</v>
       </c>
       <c r="B27" s="5" t="n">
@@ -5286,7 +5293,7 @@
       </c>
     </row>
     <row r="28" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A28" s="1" t="s">
+      <c r="A28" s="3" t="s">
         <v>33</v>
       </c>
       <c r="B28" s="5" t="n">
@@ -5312,7 +5319,7 @@
       </c>
     </row>
     <row r="29" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A29" s="1" t="s">
+      <c r="A29" s="3" t="s">
         <v>34</v>
       </c>
       <c r="B29" s="5" t="n">
@@ -5338,7 +5345,7 @@
       </c>
     </row>
     <row r="30" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A30" s="1" t="s">
+      <c r="A30" s="3" t="s">
         <v>35</v>
       </c>
       <c r="B30" s="5" t="n">
@@ -5364,7 +5371,7 @@
       </c>
     </row>
     <row r="31" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A31" s="1" t="s">
+      <c r="A31" s="3" t="s">
         <v>36</v>
       </c>
       <c r="B31" s="5" t="n">
@@ -5390,7 +5397,7 @@
       </c>
     </row>
     <row r="32" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A32" s="1" t="s">
+      <c r="A32" s="3" t="s">
         <v>37</v>
       </c>
       <c r="B32" s="5" t="n">
@@ -5416,7 +5423,7 @@
       </c>
     </row>
     <row r="33" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A33" s="1" t="s">
+      <c r="A33" s="3" t="s">
         <v>38</v>
       </c>
       <c r="B33" s="5" t="n">
@@ -5442,7 +5449,7 @@
       </c>
     </row>
     <row r="34" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A34" s="1" t="s">
+      <c r="A34" s="3" t="s">
         <v>39</v>
       </c>
       <c r="B34" s="5" t="n">
@@ -5468,7 +5475,7 @@
       </c>
     </row>
     <row r="35" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A35" s="1" t="s">
+      <c r="A35" s="3" t="s">
         <v>40</v>
       </c>
       <c r="B35" s="5" t="n">
@@ -5494,7 +5501,7 @@
       </c>
     </row>
     <row r="36" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A36" s="1" t="s">
+      <c r="A36" s="3" t="s">
         <v>41</v>
       </c>
       <c r="B36" s="5" t="n">
@@ -5520,7 +5527,7 @@
       </c>
     </row>
     <row r="37" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A37" s="1" t="s">
+      <c r="A37" s="3" t="s">
         <v>42</v>
       </c>
       <c r="B37" s="5" t="n">
@@ -5546,7 +5553,7 @@
       </c>
     </row>
     <row r="38" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A38" s="1" t="s">
+      <c r="A38" s="3" t="s">
         <v>43</v>
       </c>
       <c r="B38" s="5" t="n">
@@ -5572,7 +5579,7 @@
       </c>
     </row>
     <row r="39" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A39" s="1" t="s">
+      <c r="A39" s="3" t="s">
         <v>44</v>
       </c>
       <c r="B39" s="5" t="n">
@@ -5598,7 +5605,7 @@
       </c>
     </row>
     <row r="40" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A40" s="1" t="s">
+      <c r="A40" s="3" t="s">
         <v>45</v>
       </c>
       <c r="B40" s="5" t="n">
@@ -5624,7 +5631,7 @@
       </c>
     </row>
     <row r="41" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A41" s="1" t="s">
+      <c r="A41" s="3" t="s">
         <v>46</v>
       </c>
       <c r="B41" s="5" t="n">
@@ -5650,7 +5657,7 @@
       </c>
     </row>
     <row r="42" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A42" s="1" t="s">
+      <c r="A42" s="3" t="s">
         <v>47</v>
       </c>
       <c r="B42" s="5" t="n">
@@ -5676,7 +5683,7 @@
       </c>
     </row>
     <row r="43" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A43" s="1" t="s">
+      <c r="A43" s="3" t="s">
         <v>48</v>
       </c>
       <c r="B43" s="5" t="n">
@@ -5702,7 +5709,7 @@
       </c>
     </row>
     <row r="44" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A44" s="1" t="s">
+      <c r="A44" s="3" t="s">
         <v>49</v>
       </c>
       <c r="B44" s="5" t="n">
@@ -5728,7 +5735,7 @@
       </c>
     </row>
     <row r="45" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A45" s="1" t="s">
+      <c r="A45" s="3" t="s">
         <v>50</v>
       </c>
       <c r="B45" s="5" t="n">
@@ -5754,7 +5761,7 @@
       </c>
     </row>
     <row r="46" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A46" s="1" t="s">
+      <c r="A46" s="3" t="s">
         <v>51</v>
       </c>
       <c r="B46" s="5" t="n">
@@ -5780,7 +5787,7 @@
       </c>
     </row>
     <row r="47" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A47" s="1" t="s">
+      <c r="A47" s="3" t="s">
         <v>52</v>
       </c>
       <c r="B47" s="5" t="n">
@@ -5806,7 +5813,7 @@
       </c>
     </row>
     <row r="48" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A48" s="1" t="s">
+      <c r="A48" s="3" t="s">
         <v>53</v>
       </c>
       <c r="B48" s="5" t="n">
@@ -5832,7 +5839,7 @@
       </c>
     </row>
     <row r="49" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A49" s="1" t="s">
+      <c r="A49" s="3" t="s">
         <v>54</v>
       </c>
       <c r="B49" s="5" t="n">
@@ -5858,7 +5865,7 @@
       </c>
     </row>
     <row r="50" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A50" s="1" t="s">
+      <c r="A50" s="3" t="s">
         <v>55</v>
       </c>
       <c r="B50" s="5" t="n">
@@ -5884,7 +5891,7 @@
       </c>
     </row>
     <row r="51" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A51" s="1" t="s">
+      <c r="A51" s="3" t="s">
         <v>56</v>
       </c>
       <c r="B51" s="5" t="n">
@@ -5910,7 +5917,7 @@
       </c>
     </row>
     <row r="52" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A52" s="1" t="s">
+      <c r="A52" s="3" t="s">
         <v>57</v>
       </c>
       <c r="B52" s="5" t="n">
@@ -5936,7 +5943,7 @@
       </c>
     </row>
     <row r="53" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A53" s="1" t="s">
+      <c r="A53" s="3" t="s">
         <v>58</v>
       </c>
       <c r="B53" s="5" t="n">
@@ -5962,7 +5969,7 @@
       </c>
     </row>
     <row r="54" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A54" s="1" t="s">
+      <c r="A54" s="3" t="s">
         <v>59</v>
       </c>
       <c r="B54" s="5" t="n">
@@ -5988,7 +5995,7 @@
       </c>
     </row>
     <row r="55" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A55" s="1" t="s">
+      <c r="A55" s="3" t="s">
         <v>60</v>
       </c>
       <c r="B55" s="5" t="n">
@@ -6014,7 +6021,7 @@
       </c>
     </row>
     <row r="56" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A56" s="1" t="s">
+      <c r="A56" s="3" t="s">
         <v>61</v>
       </c>
       <c r="B56" s="5" t="n">
@@ -6040,7 +6047,7 @@
       </c>
     </row>
     <row r="57" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A57" s="1" t="s">
+      <c r="A57" s="3" t="s">
         <v>62</v>
       </c>
       <c r="B57" s="5" t="n">
@@ -6066,7 +6073,7 @@
       </c>
     </row>
     <row r="58" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A58" s="1" t="s">
+      <c r="A58" s="3" t="s">
         <v>63</v>
       </c>
       <c r="B58" s="5" t="n">
@@ -6092,7 +6099,7 @@
       </c>
     </row>
     <row r="59" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A59" s="1" t="s">
+      <c r="A59" s="3" t="s">
         <v>64</v>
       </c>
       <c r="B59" s="5" t="n">
@@ -6118,7 +6125,7 @@
       </c>
     </row>
     <row r="60" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A60" s="1" t="s">
+      <c r="A60" s="3" t="s">
         <v>65</v>
       </c>
       <c r="B60" s="5" t="n">
@@ -6144,7 +6151,7 @@
       </c>
     </row>
     <row r="61" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A61" s="1" t="s">
+      <c r="A61" s="3" t="s">
         <v>66</v>
       </c>
       <c r="B61" s="5" t="n">
@@ -6170,7 +6177,7 @@
       </c>
     </row>
     <row r="62" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A62" s="1" t="s">
+      <c r="A62" s="3" t="s">
         <v>67</v>
       </c>
       <c r="B62" s="5" t="n">
@@ -6196,7 +6203,7 @@
       </c>
     </row>
     <row r="63" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A63" s="1" t="s">
+      <c r="A63" s="3" t="s">
         <v>68</v>
       </c>
       <c r="B63" s="5" t="n">
@@ -6222,7 +6229,7 @@
       </c>
     </row>
     <row r="64" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A64" s="1" t="s">
+      <c r="A64" s="3" t="s">
         <v>69</v>
       </c>
       <c r="B64" s="5" t="n">
@@ -6248,7 +6255,7 @@
       </c>
     </row>
     <row r="65" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A65" s="1" t="s">
+      <c r="A65" s="3" t="s">
         <v>70</v>
       </c>
       <c r="B65" s="5" t="n">
@@ -6274,7 +6281,7 @@
       </c>
     </row>
     <row r="66" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A66" s="1" t="s">
+      <c r="A66" s="3" t="s">
         <v>71</v>
       </c>
       <c r="B66" s="5" t="n">
@@ -6300,7 +6307,7 @@
       </c>
     </row>
     <row r="67" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A67" s="1" t="s">
+      <c r="A67" s="3" t="s">
         <v>72</v>
       </c>
       <c r="B67" s="5" t="n">
@@ -6326,7 +6333,7 @@
       </c>
     </row>
     <row r="68" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A68" s="1" t="s">
+      <c r="A68" s="3" t="s">
         <v>73</v>
       </c>
       <c r="B68" s="5" t="n">
@@ -6352,7 +6359,7 @@
       </c>
     </row>
     <row r="69" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A69" s="1" t="s">
+      <c r="A69" s="3" t="s">
         <v>74</v>
       </c>
       <c r="B69" s="5" t="n">
@@ -6378,7 +6385,7 @@
       </c>
     </row>
     <row r="70" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A70" s="1" t="s">
+      <c r="A70" s="3" t="s">
         <v>75</v>
       </c>
       <c r="B70" s="5" t="n">
@@ -6404,7 +6411,7 @@
       </c>
     </row>
     <row r="71" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A71" s="1" t="s">
+      <c r="A71" s="3" t="s">
         <v>76</v>
       </c>
       <c r="B71" s="5" t="n">
@@ -6430,7 +6437,7 @@
       </c>
     </row>
     <row r="72" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A72" s="1" t="s">
+      <c r="A72" s="3" t="s">
         <v>77</v>
       </c>
       <c r="B72" s="5" t="n">
@@ -6456,7 +6463,7 @@
       </c>
     </row>
     <row r="73" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A73" s="1" t="s">
+      <c r="A73" s="3" t="s">
         <v>78</v>
       </c>
       <c r="B73" s="5" t="n">
@@ -6482,7 +6489,7 @@
       </c>
     </row>
     <row r="74" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A74" s="1" t="s">
+      <c r="A74" s="3" t="s">
         <v>79</v>
       </c>
       <c r="B74" s="5" t="n">
@@ -6508,7 +6515,7 @@
       </c>
     </row>
     <row r="75" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A75" s="1" t="s">
+      <c r="A75" s="3" t="s">
         <v>80</v>
       </c>
       <c r="B75" s="5" t="n">
@@ -6534,7 +6541,7 @@
       </c>
     </row>
     <row r="76" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A76" s="1" t="s">
+      <c r="A76" s="3" t="s">
         <v>81</v>
       </c>
       <c r="B76" s="5" t="n">
@@ -6560,7 +6567,7 @@
       </c>
     </row>
     <row r="77" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A77" s="1" t="s">
+      <c r="A77" s="3" t="s">
         <v>82</v>
       </c>
       <c r="B77" s="5" t="n">
@@ -6586,7 +6593,7 @@
       </c>
     </row>
     <row r="78" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A78" s="1" t="s">
+      <c r="A78" s="3" t="s">
         <v>83</v>
       </c>
       <c r="B78" s="5" t="n">
@@ -6612,7 +6619,7 @@
       </c>
     </row>
     <row r="79" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A79" s="1" t="s">
+      <c r="A79" s="3" t="s">
         <v>84</v>
       </c>
       <c r="B79" s="5" t="n">
@@ -6638,7 +6645,7 @@
       </c>
     </row>
     <row r="80" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A80" s="1" t="s">
+      <c r="A80" s="3" t="s">
         <v>85</v>
       </c>
       <c r="B80" s="5" t="n">
@@ -6664,7 +6671,7 @@
       </c>
     </row>
     <row r="81" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A81" s="1" t="s">
+      <c r="A81" s="3" t="s">
         <v>86</v>
       </c>
       <c r="B81" s="5" t="n">
@@ -6690,7 +6697,7 @@
       </c>
     </row>
     <row r="82" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A82" s="1" t="s">
+      <c r="A82" s="3" t="s">
         <v>87</v>
       </c>
       <c r="B82" s="5" t="n">
@@ -6716,7 +6723,7 @@
       </c>
     </row>
     <row r="83" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A83" s="1" t="s">
+      <c r="A83" s="3" t="s">
         <v>88</v>
       </c>
       <c r="B83" s="5" t="n">
@@ -6742,7 +6749,7 @@
       </c>
     </row>
     <row r="84" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A84" s="1" t="s">
+      <c r="A84" s="3" t="s">
         <v>89</v>
       </c>
       <c r="B84" s="5" t="n">
@@ -6768,7 +6775,7 @@
       </c>
     </row>
     <row r="85" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A85" s="1" t="s">
+      <c r="A85" s="3" t="s">
         <v>90</v>
       </c>
       <c r="B85" s="5" t="n">
@@ -6794,7 +6801,7 @@
       </c>
     </row>
     <row r="86" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A86" s="1" t="s">
+      <c r="A86" s="3" t="s">
         <v>91</v>
       </c>
       <c r="B86" s="5" t="n">
@@ -6820,7 +6827,7 @@
       </c>
     </row>
     <row r="87" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A87" s="1" t="s">
+      <c r="A87" s="3" t="s">
         <v>92</v>
       </c>
       <c r="B87" s="5" t="n">
@@ -6846,7 +6853,7 @@
       </c>
     </row>
     <row r="88" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A88" s="1" t="s">
+      <c r="A88" s="3" t="s">
         <v>93</v>
       </c>
       <c r="B88" s="5" t="n">
@@ -6872,7 +6879,7 @@
       </c>
     </row>
     <row r="89" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A89" s="1" t="s">
+      <c r="A89" s="3" t="s">
         <v>94</v>
       </c>
       <c r="B89" s="5" t="n">
@@ -6898,7 +6905,7 @@
       </c>
     </row>
     <row r="90" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A90" s="1" t="s">
+      <c r="A90" s="3" t="s">
         <v>95</v>
       </c>
       <c r="B90" s="5" t="n">
@@ -6954,7 +6961,7 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="25.5"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="39.55"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1023" min="2" style="0" width="8.53"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1025" min="1024" style="0" width="9.14"/>
   </cols>
@@ -6978,12 +6985,12 @@
       <c r="F1" s="0" t="s">
         <v>5</v>
       </c>
-      <c r="G1" s="3" t="s">
+      <c r="G1" s="2" t="s">
         <v>6</v>
       </c>
     </row>
     <row r="2" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A2" s="1" t="s">
+      <c r="A2" s="3" t="s">
         <v>7</v>
       </c>
       <c r="B2" s="5" t="n">
@@ -7009,7 +7016,7 @@
       </c>
     </row>
     <row r="3" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A3" s="1" t="s">
+      <c r="A3" s="3" t="s">
         <v>8</v>
       </c>
       <c r="B3" s="5" t="n">
@@ -7035,7 +7042,7 @@
       </c>
     </row>
     <row r="4" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A4" s="1" t="s">
+      <c r="A4" s="3" t="s">
         <v>9</v>
       </c>
       <c r="B4" s="5" t="n">
@@ -7061,7 +7068,7 @@
       </c>
     </row>
     <row r="5" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A5" s="1" t="s">
+      <c r="A5" s="3" t="s">
         <v>10</v>
       </c>
       <c r="B5" s="5" t="n">
@@ -7087,7 +7094,7 @@
       </c>
     </row>
     <row r="6" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A6" s="1" t="s">
+      <c r="A6" s="3" t="s">
         <v>11</v>
       </c>
       <c r="B6" s="5" t="n">
@@ -7113,7 +7120,7 @@
       </c>
     </row>
     <row r="7" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A7" s="1" t="s">
+      <c r="A7" s="3" t="s">
         <v>12</v>
       </c>
       <c r="B7" s="5" t="n">
@@ -7139,7 +7146,7 @@
       </c>
     </row>
     <row r="8" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A8" s="1" t="s">
+      <c r="A8" s="3" t="s">
         <v>13</v>
       </c>
       <c r="B8" s="5" t="n">
@@ -7165,7 +7172,7 @@
       </c>
     </row>
     <row r="9" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A9" s="1" t="s">
+      <c r="A9" s="3" t="s">
         <v>14</v>
       </c>
       <c r="B9" s="5" t="n">
@@ -7191,7 +7198,7 @@
       </c>
     </row>
     <row r="10" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A10" s="1" t="s">
+      <c r="A10" s="3" t="s">
         <v>15</v>
       </c>
       <c r="B10" s="5" t="n">
@@ -7217,7 +7224,7 @@
       </c>
     </row>
     <row r="11" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A11" s="1" t="s">
+      <c r="A11" s="3" t="s">
         <v>16</v>
       </c>
       <c r="B11" s="5" t="n">
@@ -7243,7 +7250,7 @@
       </c>
     </row>
     <row r="12" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A12" s="1" t="s">
+      <c r="A12" s="3" t="s">
         <v>17</v>
       </c>
       <c r="B12" s="5" t="n">
@@ -7269,7 +7276,7 @@
       </c>
     </row>
     <row r="13" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A13" s="1" t="s">
+      <c r="A13" s="3" t="s">
         <v>18</v>
       </c>
       <c r="B13" s="5" t="n">
@@ -7295,7 +7302,7 @@
       </c>
     </row>
     <row r="14" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A14" s="1" t="s">
+      <c r="A14" s="3" t="s">
         <v>19</v>
       </c>
       <c r="B14" s="5" t="n">
@@ -7321,7 +7328,7 @@
       </c>
     </row>
     <row r="15" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A15" s="1" t="s">
+      <c r="A15" s="3" t="s">
         <v>20</v>
       </c>
       <c r="B15" s="5" t="n">
@@ -7347,7 +7354,7 @@
       </c>
     </row>
     <row r="16" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A16" s="1" t="s">
+      <c r="A16" s="3" t="s">
         <v>21</v>
       </c>
       <c r="B16" s="5" t="n">
@@ -7373,7 +7380,7 @@
       </c>
     </row>
     <row r="17" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A17" s="1" t="s">
+      <c r="A17" s="3" t="s">
         <v>22</v>
       </c>
       <c r="B17" s="5" t="n">
@@ -7399,7 +7406,7 @@
       </c>
     </row>
     <row r="18" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A18" s="1" t="s">
+      <c r="A18" s="3" t="s">
         <v>23</v>
       </c>
       <c r="B18" s="5" t="n">
@@ -7425,7 +7432,7 @@
       </c>
     </row>
     <row r="19" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A19" s="1" t="s">
+      <c r="A19" s="3" t="s">
         <v>24</v>
       </c>
       <c r="B19" s="5" t="n">
@@ -7451,7 +7458,7 @@
       </c>
     </row>
     <row r="20" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A20" s="1" t="s">
+      <c r="A20" s="3" t="s">
         <v>25</v>
       </c>
       <c r="B20" s="5" t="n">
@@ -7477,7 +7484,7 @@
       </c>
     </row>
     <row r="21" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A21" s="1" t="s">
+      <c r="A21" s="3" t="s">
         <v>26</v>
       </c>
       <c r="B21" s="5" t="n">
@@ -7503,7 +7510,7 @@
       </c>
     </row>
     <row r="22" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A22" s="1" t="s">
+      <c r="A22" s="3" t="s">
         <v>27</v>
       </c>
       <c r="B22" s="5" t="n">
@@ -7529,7 +7536,7 @@
       </c>
     </row>
     <row r="23" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A23" s="1" t="s">
+      <c r="A23" s="3" t="s">
         <v>28</v>
       </c>
       <c r="B23" s="5" t="n">
@@ -7555,7 +7562,7 @@
       </c>
     </row>
     <row r="24" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A24" s="1" t="s">
+      <c r="A24" s="3" t="s">
         <v>29</v>
       </c>
       <c r="B24" s="5" t="n">
@@ -7581,7 +7588,7 @@
       </c>
     </row>
     <row r="25" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A25" s="1" t="s">
+      <c r="A25" s="3" t="s">
         <v>30</v>
       </c>
       <c r="B25" s="5" t="n">
@@ -7607,7 +7614,7 @@
       </c>
     </row>
     <row r="26" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A26" s="1" t="s">
+      <c r="A26" s="3" t="s">
         <v>31</v>
       </c>
       <c r="B26" s="5" t="n">
@@ -7633,7 +7640,7 @@
       </c>
     </row>
     <row r="27" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A27" s="1" t="s">
+      <c r="A27" s="3" t="s">
         <v>32</v>
       </c>
       <c r="B27" s="5" t="n">
@@ -7659,7 +7666,7 @@
       </c>
     </row>
     <row r="28" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A28" s="1" t="s">
+      <c r="A28" s="3" t="s">
         <v>33</v>
       </c>
       <c r="B28" s="5" t="n">
@@ -7685,7 +7692,7 @@
       </c>
     </row>
     <row r="29" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A29" s="1" t="s">
+      <c r="A29" s="3" t="s">
         <v>34</v>
       </c>
       <c r="B29" s="5" t="n">
@@ -7711,7 +7718,7 @@
       </c>
     </row>
     <row r="30" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A30" s="1" t="s">
+      <c r="A30" s="3" t="s">
         <v>35</v>
       </c>
       <c r="B30" s="5" t="n">
@@ -7737,7 +7744,7 @@
       </c>
     </row>
     <row r="31" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A31" s="1" t="s">
+      <c r="A31" s="3" t="s">
         <v>36</v>
       </c>
       <c r="B31" s="5" t="n">
@@ -7763,7 +7770,7 @@
       </c>
     </row>
     <row r="32" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A32" s="1" t="s">
+      <c r="A32" s="3" t="s">
         <v>37</v>
       </c>
       <c r="B32" s="5" t="n">
@@ -7789,7 +7796,7 @@
       </c>
     </row>
     <row r="33" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A33" s="1" t="s">
+      <c r="A33" s="3" t="s">
         <v>38</v>
       </c>
       <c r="B33" s="5" t="n">
@@ -7815,7 +7822,7 @@
       </c>
     </row>
     <row r="34" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A34" s="1" t="s">
+      <c r="A34" s="3" t="s">
         <v>39</v>
       </c>
       <c r="B34" s="5" t="n">
@@ -7841,7 +7848,7 @@
       </c>
     </row>
     <row r="35" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A35" s="1" t="s">
+      <c r="A35" s="3" t="s">
         <v>40</v>
       </c>
       <c r="B35" s="5" t="n">
@@ -7867,7 +7874,7 @@
       </c>
     </row>
     <row r="36" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A36" s="1" t="s">
+      <c r="A36" s="3" t="s">
         <v>41</v>
       </c>
       <c r="B36" s="5" t="n">
@@ -7893,7 +7900,7 @@
       </c>
     </row>
     <row r="37" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A37" s="1" t="s">
+      <c r="A37" s="3" t="s">
         <v>42</v>
       </c>
       <c r="B37" s="5" t="n">
@@ -7919,7 +7926,7 @@
       </c>
     </row>
     <row r="38" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A38" s="1" t="s">
+      <c r="A38" s="3" t="s">
         <v>43</v>
       </c>
       <c r="B38" s="5" t="n">
@@ -7945,7 +7952,7 @@
       </c>
     </row>
     <row r="39" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A39" s="1" t="s">
+      <c r="A39" s="3" t="s">
         <v>44</v>
       </c>
       <c r="B39" s="5" t="n">
@@ -7971,7 +7978,7 @@
       </c>
     </row>
     <row r="40" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A40" s="1" t="s">
+      <c r="A40" s="3" t="s">
         <v>45</v>
       </c>
       <c r="B40" s="5" t="n">
@@ -7997,7 +8004,7 @@
       </c>
     </row>
     <row r="41" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A41" s="1" t="s">
+      <c r="A41" s="3" t="s">
         <v>46</v>
       </c>
       <c r="B41" s="5" t="n">
@@ -8023,7 +8030,7 @@
       </c>
     </row>
     <row r="42" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A42" s="1" t="s">
+      <c r="A42" s="3" t="s">
         <v>47</v>
       </c>
       <c r="B42" s="5" t="n">
@@ -8049,7 +8056,7 @@
       </c>
     </row>
     <row r="43" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A43" s="1" t="s">
+      <c r="A43" s="3" t="s">
         <v>48</v>
       </c>
       <c r="B43" s="5" t="n">
@@ -8075,7 +8082,7 @@
       </c>
     </row>
     <row r="44" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A44" s="1" t="s">
+      <c r="A44" s="3" t="s">
         <v>49</v>
       </c>
       <c r="B44" s="5" t="n">
@@ -8101,7 +8108,7 @@
       </c>
     </row>
     <row r="45" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A45" s="1" t="s">
+      <c r="A45" s="3" t="s">
         <v>50</v>
       </c>
       <c r="B45" s="5" t="n">
@@ -8127,7 +8134,7 @@
       </c>
     </row>
     <row r="46" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A46" s="1" t="s">
+      <c r="A46" s="3" t="s">
         <v>51</v>
       </c>
       <c r="B46" s="5" t="n">
@@ -8153,7 +8160,7 @@
       </c>
     </row>
     <row r="47" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A47" s="1" t="s">
+      <c r="A47" s="3" t="s">
         <v>52</v>
       </c>
       <c r="B47" s="5" t="n">
@@ -8179,7 +8186,7 @@
       </c>
     </row>
     <row r="48" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A48" s="1" t="s">
+      <c r="A48" s="3" t="s">
         <v>53</v>
       </c>
       <c r="B48" s="5" t="n">
@@ -8205,7 +8212,7 @@
       </c>
     </row>
     <row r="49" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A49" s="1" t="s">
+      <c r="A49" s="3" t="s">
         <v>54</v>
       </c>
       <c r="B49" s="5" t="n">
@@ -8231,7 +8238,7 @@
       </c>
     </row>
     <row r="50" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A50" s="1" t="s">
+      <c r="A50" s="3" t="s">
         <v>55</v>
       </c>
       <c r="B50" s="5" t="n">
@@ -8257,7 +8264,7 @@
       </c>
     </row>
     <row r="51" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A51" s="1" t="s">
+      <c r="A51" s="3" t="s">
         <v>56</v>
       </c>
       <c r="B51" s="5" t="n">
@@ -8283,7 +8290,7 @@
       </c>
     </row>
     <row r="52" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A52" s="1" t="s">
+      <c r="A52" s="3" t="s">
         <v>57</v>
       </c>
       <c r="B52" s="5" t="n">
@@ -8309,7 +8316,7 @@
       </c>
     </row>
     <row r="53" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A53" s="1" t="s">
+      <c r="A53" s="3" t="s">
         <v>58</v>
       </c>
       <c r="B53" s="5" t="n">
@@ -8335,7 +8342,7 @@
       </c>
     </row>
     <row r="54" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A54" s="1" t="s">
+      <c r="A54" s="3" t="s">
         <v>59</v>
       </c>
       <c r="B54" s="5" t="n">
@@ -8361,7 +8368,7 @@
       </c>
     </row>
     <row r="55" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A55" s="1" t="s">
+      <c r="A55" s="3" t="s">
         <v>60</v>
       </c>
       <c r="B55" s="5" t="n">
@@ -8387,7 +8394,7 @@
       </c>
     </row>
     <row r="56" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A56" s="1" t="s">
+      <c r="A56" s="3" t="s">
         <v>61</v>
       </c>
       <c r="B56" s="5" t="n">
@@ -8413,7 +8420,7 @@
       </c>
     </row>
     <row r="57" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A57" s="1" t="s">
+      <c r="A57" s="3" t="s">
         <v>62</v>
       </c>
       <c r="B57" s="5" t="n">
@@ -8439,7 +8446,7 @@
       </c>
     </row>
     <row r="58" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A58" s="1" t="s">
+      <c r="A58" s="3" t="s">
         <v>63</v>
       </c>
       <c r="B58" s="5" t="n">
@@ -8465,7 +8472,7 @@
       </c>
     </row>
     <row r="59" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A59" s="1" t="s">
+      <c r="A59" s="3" t="s">
         <v>64</v>
       </c>
       <c r="B59" s="5" t="n">
@@ -8491,7 +8498,7 @@
       </c>
     </row>
     <row r="60" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A60" s="1" t="s">
+      <c r="A60" s="3" t="s">
         <v>65</v>
       </c>
       <c r="B60" s="5" t="n">
@@ -8517,7 +8524,7 @@
       </c>
     </row>
     <row r="61" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A61" s="1" t="s">
+      <c r="A61" s="3" t="s">
         <v>66</v>
       </c>
       <c r="B61" s="5" t="n">
@@ -8543,7 +8550,7 @@
       </c>
     </row>
     <row r="62" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A62" s="1" t="s">
+      <c r="A62" s="3" t="s">
         <v>67</v>
       </c>
       <c r="B62" s="5" t="n">
@@ -8569,7 +8576,7 @@
       </c>
     </row>
     <row r="63" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A63" s="1" t="s">
+      <c r="A63" s="3" t="s">
         <v>68</v>
       </c>
       <c r="B63" s="5" t="n">
@@ -8595,7 +8602,7 @@
       </c>
     </row>
     <row r="64" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A64" s="1" t="s">
+      <c r="A64" s="3" t="s">
         <v>69</v>
       </c>
       <c r="B64" s="5" t="n">
@@ -8621,7 +8628,7 @@
       </c>
     </row>
     <row r="65" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A65" s="1" t="s">
+      <c r="A65" s="3" t="s">
         <v>70</v>
       </c>
       <c r="B65" s="5" t="n">
@@ -8647,7 +8654,7 @@
       </c>
     </row>
     <row r="66" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A66" s="1" t="s">
+      <c r="A66" s="3" t="s">
         <v>71</v>
       </c>
       <c r="B66" s="5" t="n">
@@ -8673,7 +8680,7 @@
       </c>
     </row>
     <row r="67" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A67" s="1" t="s">
+      <c r="A67" s="3" t="s">
         <v>72</v>
       </c>
       <c r="B67" s="5" t="n">
@@ -8699,7 +8706,7 @@
       </c>
     </row>
     <row r="68" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A68" s="1" t="s">
+      <c r="A68" s="3" t="s">
         <v>73</v>
       </c>
       <c r="B68" s="5" t="n">
@@ -8725,7 +8732,7 @@
       </c>
     </row>
     <row r="69" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A69" s="1" t="s">
+      <c r="A69" s="3" t="s">
         <v>74</v>
       </c>
       <c r="B69" s="5" t="n">
@@ -8751,7 +8758,7 @@
       </c>
     </row>
     <row r="70" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A70" s="1" t="s">
+      <c r="A70" s="3" t="s">
         <v>75</v>
       </c>
       <c r="B70" s="5" t="n">
@@ -8777,7 +8784,7 @@
       </c>
     </row>
     <row r="71" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A71" s="1" t="s">
+      <c r="A71" s="3" t="s">
         <v>76</v>
       </c>
       <c r="B71" s="5" t="n">
@@ -8803,7 +8810,7 @@
       </c>
     </row>
     <row r="72" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A72" s="1" t="s">
+      <c r="A72" s="3" t="s">
         <v>77</v>
       </c>
       <c r="B72" s="5" t="n">
@@ -8829,7 +8836,7 @@
       </c>
     </row>
     <row r="73" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A73" s="1" t="s">
+      <c r="A73" s="3" t="s">
         <v>78</v>
       </c>
       <c r="B73" s="5" t="n">
@@ -8855,7 +8862,7 @@
       </c>
     </row>
     <row r="74" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A74" s="1" t="s">
+      <c r="A74" s="3" t="s">
         <v>79</v>
       </c>
       <c r="B74" s="5" t="n">
@@ -8881,7 +8888,7 @@
       </c>
     </row>
     <row r="75" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A75" s="1" t="s">
+      <c r="A75" s="3" t="s">
         <v>80</v>
       </c>
       <c r="B75" s="5" t="n">
@@ -8907,7 +8914,7 @@
       </c>
     </row>
     <row r="76" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A76" s="1" t="s">
+      <c r="A76" s="3" t="s">
         <v>81</v>
       </c>
       <c r="B76" s="5" t="n">
@@ -8933,7 +8940,7 @@
       </c>
     </row>
     <row r="77" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A77" s="1" t="s">
+      <c r="A77" s="3" t="s">
         <v>82</v>
       </c>
       <c r="B77" s="5" t="n">
@@ -8959,7 +8966,7 @@
       </c>
     </row>
     <row r="78" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A78" s="1" t="s">
+      <c r="A78" s="3" t="s">
         <v>83</v>
       </c>
       <c r="B78" s="5" t="n">
@@ -8985,7 +8992,7 @@
       </c>
     </row>
     <row r="79" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A79" s="1" t="s">
+      <c r="A79" s="3" t="s">
         <v>84</v>
       </c>
       <c r="B79" s="5" t="n">
@@ -9011,7 +9018,7 @@
       </c>
     </row>
     <row r="80" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A80" s="1" t="s">
+      <c r="A80" s="3" t="s">
         <v>85</v>
       </c>
       <c r="B80" s="5" t="n">
@@ -9037,7 +9044,7 @@
       </c>
     </row>
     <row r="81" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A81" s="1" t="s">
+      <c r="A81" s="3" t="s">
         <v>86</v>
       </c>
       <c r="B81" s="5" t="n">
@@ -9063,7 +9070,7 @@
       </c>
     </row>
     <row r="82" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A82" s="1" t="s">
+      <c r="A82" s="3" t="s">
         <v>87</v>
       </c>
       <c r="B82" s="5" t="n">
@@ -9089,7 +9096,7 @@
       </c>
     </row>
     <row r="83" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A83" s="1" t="s">
+      <c r="A83" s="3" t="s">
         <v>88</v>
       </c>
       <c r="B83" s="5" t="n">
@@ -9115,7 +9122,7 @@
       </c>
     </row>
     <row r="84" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A84" s="1" t="s">
+      <c r="A84" s="3" t="s">
         <v>89</v>
       </c>
       <c r="B84" s="5" t="n">
@@ -9141,7 +9148,7 @@
       </c>
     </row>
     <row r="85" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A85" s="1" t="s">
+      <c r="A85" s="3" t="s">
         <v>90</v>
       </c>
       <c r="B85" s="5" t="n">
@@ -9167,7 +9174,7 @@
       </c>
     </row>
     <row r="86" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A86" s="1" t="s">
+      <c r="A86" s="3" t="s">
         <v>91</v>
       </c>
       <c r="B86" s="5" t="n">
@@ -9193,7 +9200,7 @@
       </c>
     </row>
     <row r="87" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A87" s="1" t="s">
+      <c r="A87" s="3" t="s">
         <v>92</v>
       </c>
       <c r="B87" s="5" t="n">
@@ -9219,7 +9226,7 @@
       </c>
     </row>
     <row r="88" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A88" s="1" t="s">
+      <c r="A88" s="3" t="s">
         <v>93</v>
       </c>
       <c r="B88" s="5" t="n">
@@ -9245,7 +9252,7 @@
       </c>
     </row>
     <row r="89" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A89" s="1" t="s">
+      <c r="A89" s="3" t="s">
         <v>94</v>
       </c>
       <c r="B89" s="5" t="n">
@@ -9271,7 +9278,7 @@
       </c>
     </row>
     <row r="90" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A90" s="1" t="s">
+      <c r="A90" s="3" t="s">
         <v>95</v>
       </c>
       <c r="B90" s="5" t="n">
@@ -9322,12 +9329,12 @@
   <dimension ref="A1:G91"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="B1" activeCellId="0" sqref="B1"/>
+      <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="25.5"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="39.55"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="7" min="2" style="0" width="8.53"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1025" min="8" style="0" width="9.14"/>
   </cols>
@@ -9351,12 +9358,12 @@
       <c r="F1" s="0" t="s">
         <v>5</v>
       </c>
-      <c r="G1" s="3" t="s">
+      <c r="G1" s="2" t="s">
         <v>6</v>
       </c>
     </row>
     <row r="2" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A2" s="1" t="s">
+      <c r="A2" s="3" t="s">
         <v>7</v>
       </c>
       <c r="B2" s="5" t="n">
@@ -9382,7 +9389,7 @@
       </c>
     </row>
     <row r="3" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A3" s="1" t="s">
+      <c r="A3" s="3" t="s">
         <v>8</v>
       </c>
       <c r="B3" s="5" t="n">
@@ -9408,7 +9415,7 @@
       </c>
     </row>
     <row r="4" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A4" s="1" t="s">
+      <c r="A4" s="3" t="s">
         <v>9</v>
       </c>
       <c r="B4" s="5" t="n">
@@ -9434,7 +9441,7 @@
       </c>
     </row>
     <row r="5" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A5" s="1" t="s">
+      <c r="A5" s="3" t="s">
         <v>10</v>
       </c>
       <c r="B5" s="5" t="n">
@@ -9460,7 +9467,7 @@
       </c>
     </row>
     <row r="6" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A6" s="1" t="s">
+      <c r="A6" s="3" t="s">
         <v>11</v>
       </c>
       <c r="B6" s="5" t="n">
@@ -9486,7 +9493,7 @@
       </c>
     </row>
     <row r="7" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A7" s="1" t="s">
+      <c r="A7" s="3" t="s">
         <v>12</v>
       </c>
       <c r="B7" s="5" t="n">
@@ -9512,7 +9519,7 @@
       </c>
     </row>
     <row r="8" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A8" s="1" t="s">
+      <c r="A8" s="3" t="s">
         <v>13</v>
       </c>
       <c r="B8" s="5" t="n">
@@ -9538,7 +9545,7 @@
       </c>
     </row>
     <row r="9" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A9" s="1" t="s">
+      <c r="A9" s="3" t="s">
         <v>14</v>
       </c>
       <c r="B9" s="5" t="n">
@@ -9564,7 +9571,7 @@
       </c>
     </row>
     <row r="10" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A10" s="1" t="s">
+      <c r="A10" s="3" t="s">
         <v>15</v>
       </c>
       <c r="B10" s="5" t="n">
@@ -9590,7 +9597,7 @@
       </c>
     </row>
     <row r="11" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A11" s="1" t="s">
+      <c r="A11" s="3" t="s">
         <v>16</v>
       </c>
       <c r="B11" s="5" t="n">
@@ -9616,7 +9623,7 @@
       </c>
     </row>
     <row r="12" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A12" s="1" t="s">
+      <c r="A12" s="3" t="s">
         <v>17</v>
       </c>
       <c r="B12" s="5" t="n">
@@ -9642,7 +9649,7 @@
       </c>
     </row>
     <row r="13" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A13" s="1" t="s">
+      <c r="A13" s="3" t="s">
         <v>18</v>
       </c>
       <c r="B13" s="5" t="n">
@@ -9668,7 +9675,7 @@
       </c>
     </row>
     <row r="14" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A14" s="1" t="s">
+      <c r="A14" s="3" t="s">
         <v>19</v>
       </c>
       <c r="B14" s="5" t="n">
@@ -9694,7 +9701,7 @@
       </c>
     </row>
     <row r="15" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A15" s="1" t="s">
+      <c r="A15" s="3" t="s">
         <v>20</v>
       </c>
       <c r="B15" s="5" t="n">
@@ -9720,7 +9727,7 @@
       </c>
     </row>
     <row r="16" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A16" s="1" t="s">
+      <c r="A16" s="3" t="s">
         <v>21</v>
       </c>
       <c r="B16" s="5" t="n">
@@ -9746,7 +9753,7 @@
       </c>
     </row>
     <row r="17" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A17" s="1" t="s">
+      <c r="A17" s="3" t="s">
         <v>22</v>
       </c>
       <c r="B17" s="5" t="n">
@@ -9772,7 +9779,7 @@
       </c>
     </row>
     <row r="18" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A18" s="1" t="s">
+      <c r="A18" s="3" t="s">
         <v>23</v>
       </c>
       <c r="B18" s="5" t="n">
@@ -9798,7 +9805,7 @@
       </c>
     </row>
     <row r="19" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A19" s="1" t="s">
+      <c r="A19" s="3" t="s">
         <v>24</v>
       </c>
       <c r="B19" s="5" t="n">
@@ -9824,7 +9831,7 @@
       </c>
     </row>
     <row r="20" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A20" s="1" t="s">
+      <c r="A20" s="3" t="s">
         <v>25</v>
       </c>
       <c r="B20" s="5" t="n">
@@ -9850,7 +9857,7 @@
       </c>
     </row>
     <row r="21" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A21" s="1" t="s">
+      <c r="A21" s="3" t="s">
         <v>26</v>
       </c>
       <c r="B21" s="5" t="n">
@@ -9876,7 +9883,7 @@
       </c>
     </row>
     <row r="22" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A22" s="1" t="s">
+      <c r="A22" s="3" t="s">
         <v>27</v>
       </c>
       <c r="B22" s="5" t="n">
@@ -9902,7 +9909,7 @@
       </c>
     </row>
     <row r="23" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A23" s="1" t="s">
+      <c r="A23" s="3" t="s">
         <v>28</v>
       </c>
       <c r="B23" s="5" t="n">
@@ -9928,7 +9935,7 @@
       </c>
     </row>
     <row r="24" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A24" s="1" t="s">
+      <c r="A24" s="3" t="s">
         <v>29</v>
       </c>
       <c r="B24" s="5" t="n">
@@ -9954,7 +9961,7 @@
       </c>
     </row>
     <row r="25" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A25" s="1" t="s">
+      <c r="A25" s="3" t="s">
         <v>30</v>
       </c>
       <c r="B25" s="5" t="n">
@@ -9980,7 +9987,7 @@
       </c>
     </row>
     <row r="26" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A26" s="1" t="s">
+      <c r="A26" s="3" t="s">
         <v>31</v>
       </c>
       <c r="B26" s="5" t="n">
@@ -10006,7 +10013,7 @@
       </c>
     </row>
     <row r="27" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A27" s="1" t="s">
+      <c r="A27" s="3" t="s">
         <v>32</v>
       </c>
       <c r="B27" s="5" t="n">
@@ -10032,7 +10039,7 @@
       </c>
     </row>
     <row r="28" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A28" s="1" t="s">
+      <c r="A28" s="3" t="s">
         <v>33</v>
       </c>
       <c r="B28" s="5" t="n">
@@ -10058,7 +10065,7 @@
       </c>
     </row>
     <row r="29" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A29" s="1" t="s">
+      <c r="A29" s="3" t="s">
         <v>34</v>
       </c>
       <c r="B29" s="5" t="n">
@@ -10084,7 +10091,7 @@
       </c>
     </row>
     <row r="30" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A30" s="1" t="s">
+      <c r="A30" s="3" t="s">
         <v>35</v>
       </c>
       <c r="B30" s="5" t="n">
@@ -10110,7 +10117,7 @@
       </c>
     </row>
     <row r="31" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A31" s="1" t="s">
+      <c r="A31" s="3" t="s">
         <v>36</v>
       </c>
       <c r="B31" s="5" t="n">
@@ -10136,7 +10143,7 @@
       </c>
     </row>
     <row r="32" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A32" s="1" t="s">
+      <c r="A32" s="3" t="s">
         <v>37</v>
       </c>
       <c r="B32" s="5" t="n">
@@ -10162,7 +10169,7 @@
       </c>
     </row>
     <row r="33" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A33" s="1" t="s">
+      <c r="A33" s="3" t="s">
         <v>38</v>
       </c>
       <c r="B33" s="5" t="n">
@@ -10188,7 +10195,7 @@
       </c>
     </row>
     <row r="34" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A34" s="1" t="s">
+      <c r="A34" s="3" t="s">
         <v>39</v>
       </c>
       <c r="B34" s="5" t="n">
@@ -10214,7 +10221,7 @@
       </c>
     </row>
     <row r="35" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A35" s="1" t="s">
+      <c r="A35" s="3" t="s">
         <v>40</v>
       </c>
       <c r="B35" s="5" t="n">
@@ -10240,7 +10247,7 @@
       </c>
     </row>
     <row r="36" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A36" s="1" t="s">
+      <c r="A36" s="3" t="s">
         <v>41</v>
       </c>
       <c r="B36" s="5" t="n">
@@ -10266,7 +10273,7 @@
       </c>
     </row>
     <row r="37" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A37" s="1" t="s">
+      <c r="A37" s="3" t="s">
         <v>42</v>
       </c>
       <c r="B37" s="5" t="n">
@@ -10292,7 +10299,7 @@
       </c>
     </row>
     <row r="38" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A38" s="1" t="s">
+      <c r="A38" s="3" t="s">
         <v>43</v>
       </c>
       <c r="B38" s="5" t="n">
@@ -10318,7 +10325,7 @@
       </c>
     </row>
     <row r="39" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A39" s="1" t="s">
+      <c r="A39" s="3" t="s">
         <v>44</v>
       </c>
       <c r="B39" s="5" t="n">
@@ -10344,7 +10351,7 @@
       </c>
     </row>
     <row r="40" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A40" s="1" t="s">
+      <c r="A40" s="3" t="s">
         <v>45</v>
       </c>
       <c r="B40" s="5" t="n">
@@ -10370,7 +10377,7 @@
       </c>
     </row>
     <row r="41" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A41" s="1" t="s">
+      <c r="A41" s="3" t="s">
         <v>46</v>
       </c>
       <c r="B41" s="5" t="n">
@@ -10396,7 +10403,7 @@
       </c>
     </row>
     <row r="42" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A42" s="1" t="s">
+      <c r="A42" s="3" t="s">
         <v>47</v>
       </c>
       <c r="B42" s="5" t="n">
@@ -10422,7 +10429,7 @@
       </c>
     </row>
     <row r="43" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A43" s="1" t="s">
+      <c r="A43" s="3" t="s">
         <v>48</v>
       </c>
       <c r="B43" s="5" t="n">
@@ -10448,7 +10455,7 @@
       </c>
     </row>
     <row r="44" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A44" s="1" t="s">
+      <c r="A44" s="3" t="s">
         <v>49</v>
       </c>
       <c r="B44" s="5" t="n">
@@ -10474,7 +10481,7 @@
       </c>
     </row>
     <row r="45" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A45" s="1" t="s">
+      <c r="A45" s="3" t="s">
         <v>50</v>
       </c>
       <c r="B45" s="5" t="n">
@@ -10500,7 +10507,7 @@
       </c>
     </row>
     <row r="46" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A46" s="1" t="s">
+      <c r="A46" s="3" t="s">
         <v>51</v>
       </c>
       <c r="B46" s="5" t="n">
@@ -10526,7 +10533,7 @@
       </c>
     </row>
     <row r="47" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A47" s="1" t="s">
+      <c r="A47" s="3" t="s">
         <v>52</v>
       </c>
       <c r="B47" s="5" t="n">
@@ -10552,7 +10559,7 @@
       </c>
     </row>
     <row r="48" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A48" s="1" t="s">
+      <c r="A48" s="3" t="s">
         <v>53</v>
       </c>
       <c r="B48" s="5" t="n">
@@ -10578,7 +10585,7 @@
       </c>
     </row>
     <row r="49" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A49" s="1" t="s">
+      <c r="A49" s="3" t="s">
         <v>54</v>
       </c>
       <c r="B49" s="5" t="n">
@@ -10604,7 +10611,7 @@
       </c>
     </row>
     <row r="50" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A50" s="1" t="s">
+      <c r="A50" s="3" t="s">
         <v>55</v>
       </c>
       <c r="B50" s="5" t="n">
@@ -10630,7 +10637,7 @@
       </c>
     </row>
     <row r="51" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A51" s="1" t="s">
+      <c r="A51" s="3" t="s">
         <v>56</v>
       </c>
       <c r="B51" s="5" t="n">
@@ -10656,7 +10663,7 @@
       </c>
     </row>
     <row r="52" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A52" s="1" t="s">
+      <c r="A52" s="3" t="s">
         <v>57</v>
       </c>
       <c r="B52" s="5" t="n">
@@ -10682,7 +10689,7 @@
       </c>
     </row>
     <row r="53" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A53" s="1" t="s">
+      <c r="A53" s="3" t="s">
         <v>58</v>
       </c>
       <c r="B53" s="5" t="n">
@@ -10708,7 +10715,7 @@
       </c>
     </row>
     <row r="54" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A54" s="1" t="s">
+      <c r="A54" s="3" t="s">
         <v>59</v>
       </c>
       <c r="B54" s="5" t="n">
@@ -10734,7 +10741,7 @@
       </c>
     </row>
     <row r="55" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A55" s="1" t="s">
+      <c r="A55" s="3" t="s">
         <v>60</v>
       </c>
       <c r="B55" s="5" t="n">
@@ -10760,7 +10767,7 @@
       </c>
     </row>
     <row r="56" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A56" s="1" t="s">
+      <c r="A56" s="3" t="s">
         <v>61</v>
       </c>
       <c r="B56" s="5" t="n">
@@ -10786,7 +10793,7 @@
       </c>
     </row>
     <row r="57" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A57" s="1" t="s">
+      <c r="A57" s="3" t="s">
         <v>62</v>
       </c>
       <c r="B57" s="5" t="n">
@@ -10812,7 +10819,7 @@
       </c>
     </row>
     <row r="58" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A58" s="1" t="s">
+      <c r="A58" s="3" t="s">
         <v>63</v>
       </c>
       <c r="B58" s="5" t="n">
@@ -10838,7 +10845,7 @@
       </c>
     </row>
     <row r="59" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A59" s="1" t="s">
+      <c r="A59" s="3" t="s">
         <v>64</v>
       </c>
       <c r="B59" s="5" t="n">
@@ -10864,7 +10871,7 @@
       </c>
     </row>
     <row r="60" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A60" s="1" t="s">
+      <c r="A60" s="3" t="s">
         <v>65</v>
       </c>
       <c r="B60" s="5" t="n">
@@ -10890,7 +10897,7 @@
       </c>
     </row>
     <row r="61" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A61" s="1" t="s">
+      <c r="A61" s="3" t="s">
         <v>66</v>
       </c>
       <c r="B61" s="5" t="n">
@@ -10916,7 +10923,7 @@
       </c>
     </row>
     <row r="62" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A62" s="1" t="s">
+      <c r="A62" s="3" t="s">
         <v>67</v>
       </c>
       <c r="B62" s="5" t="n">
@@ -10942,7 +10949,7 @@
       </c>
     </row>
     <row r="63" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A63" s="1" t="s">
+      <c r="A63" s="3" t="s">
         <v>68</v>
       </c>
       <c r="B63" s="5" t="n">
@@ -10968,7 +10975,7 @@
       </c>
     </row>
     <row r="64" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A64" s="1" t="s">
+      <c r="A64" s="3" t="s">
         <v>69</v>
       </c>
       <c r="B64" s="5" t="n">
@@ -10994,7 +11001,7 @@
       </c>
     </row>
     <row r="65" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A65" s="1" t="s">
+      <c r="A65" s="3" t="s">
         <v>70</v>
       </c>
       <c r="B65" s="5" t="n">
@@ -11020,7 +11027,7 @@
       </c>
     </row>
     <row r="66" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A66" s="1" t="s">
+      <c r="A66" s="3" t="s">
         <v>71</v>
       </c>
       <c r="B66" s="5" t="n">
@@ -11046,7 +11053,7 @@
       </c>
     </row>
     <row r="67" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A67" s="1" t="s">
+      <c r="A67" s="3" t="s">
         <v>72</v>
       </c>
       <c r="B67" s="5" t="n">
@@ -11072,7 +11079,7 @@
       </c>
     </row>
     <row r="68" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A68" s="1" t="s">
+      <c r="A68" s="3" t="s">
         <v>73</v>
       </c>
       <c r="B68" s="5" t="n">
@@ -11098,7 +11105,7 @@
       </c>
     </row>
     <row r="69" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A69" s="1" t="s">
+      <c r="A69" s="3" t="s">
         <v>74</v>
       </c>
       <c r="B69" s="5" t="n">
@@ -11124,7 +11131,7 @@
       </c>
     </row>
     <row r="70" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A70" s="1" t="s">
+      <c r="A70" s="3" t="s">
         <v>75</v>
       </c>
       <c r="B70" s="5" t="n">
@@ -11150,7 +11157,7 @@
       </c>
     </row>
     <row r="71" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A71" s="1" t="s">
+      <c r="A71" s="3" t="s">
         <v>76</v>
       </c>
       <c r="B71" s="5" t="n">
@@ -11176,7 +11183,7 @@
       </c>
     </row>
     <row r="72" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A72" s="1" t="s">
+      <c r="A72" s="3" t="s">
         <v>77</v>
       </c>
       <c r="B72" s="5" t="n">
@@ -11202,7 +11209,7 @@
       </c>
     </row>
     <row r="73" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A73" s="1" t="s">
+      <c r="A73" s="3" t="s">
         <v>78</v>
       </c>
       <c r="B73" s="5" t="n">
@@ -11228,7 +11235,7 @@
       </c>
     </row>
     <row r="74" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A74" s="1" t="s">
+      <c r="A74" s="3" t="s">
         <v>79</v>
       </c>
       <c r="B74" s="5" t="n">
@@ -11254,7 +11261,7 @@
       </c>
     </row>
     <row r="75" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A75" s="1" t="s">
+      <c r="A75" s="3" t="s">
         <v>80</v>
       </c>
       <c r="B75" s="5" t="n">
@@ -11280,7 +11287,7 @@
       </c>
     </row>
     <row r="76" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A76" s="1" t="s">
+      <c r="A76" s="3" t="s">
         <v>81</v>
       </c>
       <c r="B76" s="5" t="n">
@@ -11306,7 +11313,7 @@
       </c>
     </row>
     <row r="77" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A77" s="1" t="s">
+      <c r="A77" s="3" t="s">
         <v>82</v>
       </c>
       <c r="B77" s="5" t="n">
@@ -11332,7 +11339,7 @@
       </c>
     </row>
     <row r="78" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A78" s="1" t="s">
+      <c r="A78" s="3" t="s">
         <v>83</v>
       </c>
       <c r="B78" s="5" t="n">
@@ -11358,7 +11365,7 @@
       </c>
     </row>
     <row r="79" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A79" s="1" t="s">
+      <c r="A79" s="3" t="s">
         <v>84</v>
       </c>
       <c r="B79" s="5" t="n">
@@ -11384,7 +11391,7 @@
       </c>
     </row>
     <row r="80" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A80" s="1" t="s">
+      <c r="A80" s="3" t="s">
         <v>85</v>
       </c>
       <c r="B80" s="5" t="n">
@@ -11410,7 +11417,7 @@
       </c>
     </row>
     <row r="81" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A81" s="1" t="s">
+      <c r="A81" s="3" t="s">
         <v>86</v>
       </c>
       <c r="B81" s="5" t="n">
@@ -11436,7 +11443,7 @@
       </c>
     </row>
     <row r="82" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A82" s="1" t="s">
+      <c r="A82" s="3" t="s">
         <v>87</v>
       </c>
       <c r="B82" s="5" t="n">
@@ -11462,7 +11469,7 @@
       </c>
     </row>
     <row r="83" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A83" s="1" t="s">
+      <c r="A83" s="3" t="s">
         <v>88</v>
       </c>
       <c r="B83" s="5" t="n">
@@ -11488,7 +11495,7 @@
       </c>
     </row>
     <row r="84" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A84" s="1" t="s">
+      <c r="A84" s="3" t="s">
         <v>89</v>
       </c>
       <c r="B84" s="5" t="n">
@@ -11514,7 +11521,7 @@
       </c>
     </row>
     <row r="85" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A85" s="1" t="s">
+      <c r="A85" s="3" t="s">
         <v>90</v>
       </c>
       <c r="B85" s="5" t="n">
@@ -11540,7 +11547,7 @@
       </c>
     </row>
     <row r="86" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A86" s="1" t="s">
+      <c r="A86" s="3" t="s">
         <v>91</v>
       </c>
       <c r="B86" s="5" t="n">
@@ -11566,7 +11573,7 @@
       </c>
     </row>
     <row r="87" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A87" s="1" t="s">
+      <c r="A87" s="3" t="s">
         <v>92</v>
       </c>
       <c r="B87" s="5" t="n">
@@ -11592,7 +11599,7 @@
       </c>
     </row>
     <row r="88" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A88" s="1" t="s">
+      <c r="A88" s="3" t="s">
         <v>93</v>
       </c>
       <c r="B88" s="5" t="n">
@@ -11618,7 +11625,7 @@
       </c>
     </row>
     <row r="89" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A89" s="1" t="s">
+      <c r="A89" s="3" t="s">
         <v>94</v>
       </c>
       <c r="B89" s="5" t="n">
@@ -11644,7 +11651,7 @@
       </c>
     </row>
     <row r="90" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A90" s="1" t="s">
+      <c r="A90" s="3" t="s">
         <v>95</v>
       </c>
       <c r="B90" s="5" t="n">
@@ -11694,13 +11701,13 @@
   </sheetPr>
   <dimension ref="A1:G90"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A64" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="O83" activeCellId="0" sqref="O83"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="Q10" activeCellId="0" sqref="Q10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="25.5"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="27.12"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="7" min="2" style="0" width="8.53"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1025" min="8" style="0" width="9.14"/>
   </cols>
@@ -11724,12 +11731,12 @@
       <c r="F1" s="0" t="s">
         <v>5</v>
       </c>
-      <c r="G1" s="3" t="s">
+      <c r="G1" s="2" t="s">
         <v>6</v>
       </c>
     </row>
     <row r="2" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A2" s="1" t="s">
+      <c r="A2" s="3" t="s">
         <v>7</v>
       </c>
       <c r="B2" s="5" t="n">
@@ -11755,7 +11762,7 @@
       </c>
     </row>
     <row r="3" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A3" s="1" t="s">
+      <c r="A3" s="3" t="s">
         <v>8</v>
       </c>
       <c r="B3" s="5" t="n">
@@ -11781,7 +11788,7 @@
       </c>
     </row>
     <row r="4" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A4" s="1" t="s">
+      <c r="A4" s="3" t="s">
         <v>9</v>
       </c>
       <c r="B4" s="5" t="n">
@@ -11807,7 +11814,7 @@
       </c>
     </row>
     <row r="5" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A5" s="1" t="s">
+      <c r="A5" s="3" t="s">
         <v>10</v>
       </c>
       <c r="B5" s="5" t="n">
@@ -11833,7 +11840,7 @@
       </c>
     </row>
     <row r="6" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A6" s="1" t="s">
+      <c r="A6" s="3" t="s">
         <v>11</v>
       </c>
       <c r="B6" s="5" t="n">
@@ -11859,7 +11866,7 @@
       </c>
     </row>
     <row r="7" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A7" s="1" t="s">
+      <c r="A7" s="3" t="s">
         <v>12</v>
       </c>
       <c r="B7" s="5" t="n">
@@ -11885,7 +11892,7 @@
       </c>
     </row>
     <row r="8" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A8" s="1" t="s">
+      <c r="A8" s="3" t="s">
         <v>13</v>
       </c>
       <c r="B8" s="5" t="n">
@@ -11911,7 +11918,7 @@
       </c>
     </row>
     <row r="9" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A9" s="1" t="s">
+      <c r="A9" s="3" t="s">
         <v>14</v>
       </c>
       <c r="B9" s="5" t="n">
@@ -11937,7 +11944,7 @@
       </c>
     </row>
     <row r="10" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A10" s="1" t="s">
+      <c r="A10" s="3" t="s">
         <v>15</v>
       </c>
       <c r="B10" s="5" t="n">
@@ -11963,7 +11970,7 @@
       </c>
     </row>
     <row r="11" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A11" s="1" t="s">
+      <c r="A11" s="3" t="s">
         <v>16</v>
       </c>
       <c r="B11" s="5" t="n">
@@ -11989,7 +11996,7 @@
       </c>
     </row>
     <row r="12" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A12" s="1" t="s">
+      <c r="A12" s="3" t="s">
         <v>17</v>
       </c>
       <c r="B12" s="5" t="n">
@@ -12015,7 +12022,7 @@
       </c>
     </row>
     <row r="13" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A13" s="1" t="s">
+      <c r="A13" s="3" t="s">
         <v>18</v>
       </c>
       <c r="B13" s="5" t="n">
@@ -12041,7 +12048,7 @@
       </c>
     </row>
     <row r="14" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A14" s="1" t="s">
+      <c r="A14" s="3" t="s">
         <v>19</v>
       </c>
       <c r="B14" s="5" t="n">
@@ -12067,7 +12074,7 @@
       </c>
     </row>
     <row r="15" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A15" s="1" t="s">
+      <c r="A15" s="3" t="s">
         <v>20</v>
       </c>
       <c r="B15" s="5" t="n">
@@ -12093,7 +12100,7 @@
       </c>
     </row>
     <row r="16" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A16" s="1" t="s">
+      <c r="A16" s="3" t="s">
         <v>21</v>
       </c>
       <c r="B16" s="5" t="n">
@@ -12119,7 +12126,7 @@
       </c>
     </row>
     <row r="17" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A17" s="1" t="s">
+      <c r="A17" s="3" t="s">
         <v>22</v>
       </c>
       <c r="B17" s="5" t="n">
@@ -12145,7 +12152,7 @@
       </c>
     </row>
     <row r="18" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A18" s="1" t="s">
+      <c r="A18" s="3" t="s">
         <v>23</v>
       </c>
       <c r="B18" s="5" t="n">
@@ -12171,7 +12178,7 @@
       </c>
     </row>
     <row r="19" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A19" s="1" t="s">
+      <c r="A19" s="3" t="s">
         <v>24</v>
       </c>
       <c r="B19" s="5" t="n">
@@ -12197,7 +12204,7 @@
       </c>
     </row>
     <row r="20" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A20" s="1" t="s">
+      <c r="A20" s="3" t="s">
         <v>25</v>
       </c>
       <c r="B20" s="5" t="n">
@@ -12223,7 +12230,7 @@
       </c>
     </row>
     <row r="21" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A21" s="1" t="s">
+      <c r="A21" s="3" t="s">
         <v>26</v>
       </c>
       <c r="B21" s="5" t="n">
@@ -12249,7 +12256,7 @@
       </c>
     </row>
     <row r="22" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A22" s="1" t="s">
+      <c r="A22" s="3" t="s">
         <v>27</v>
       </c>
       <c r="B22" s="5" t="n">
@@ -12275,7 +12282,7 @@
       </c>
     </row>
     <row r="23" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A23" s="1" t="s">
+      <c r="A23" s="3" t="s">
         <v>28</v>
       </c>
       <c r="B23" s="5" t="n">
@@ -12301,7 +12308,7 @@
       </c>
     </row>
     <row r="24" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A24" s="1" t="s">
+      <c r="A24" s="3" t="s">
         <v>29</v>
       </c>
       <c r="B24" s="5" t="n">
@@ -12327,7 +12334,7 @@
       </c>
     </row>
     <row r="25" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A25" s="1" t="s">
+      <c r="A25" s="3" t="s">
         <v>30</v>
       </c>
       <c r="B25" s="5" t="n">
@@ -12353,7 +12360,7 @@
       </c>
     </row>
     <row r="26" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A26" s="1" t="s">
+      <c r="A26" s="3" t="s">
         <v>31</v>
       </c>
       <c r="B26" s="5" t="n">
@@ -12379,7 +12386,7 @@
       </c>
     </row>
     <row r="27" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A27" s="1" t="s">
+      <c r="A27" s="3" t="s">
         <v>32</v>
       </c>
       <c r="B27" s="5" t="n">
@@ -12405,7 +12412,7 @@
       </c>
     </row>
     <row r="28" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A28" s="1" t="s">
+      <c r="A28" s="3" t="s">
         <v>33</v>
       </c>
       <c r="B28" s="5" t="n">
@@ -12431,7 +12438,7 @@
       </c>
     </row>
     <row r="29" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A29" s="1" t="s">
+      <c r="A29" s="3" t="s">
         <v>34</v>
       </c>
       <c r="B29" s="5" t="n">
@@ -12457,7 +12464,7 @@
       </c>
     </row>
     <row r="30" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A30" s="1" t="s">
+      <c r="A30" s="3" t="s">
         <v>35</v>
       </c>
       <c r="B30" s="5" t="n">
@@ -12483,7 +12490,7 @@
       </c>
     </row>
     <row r="31" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A31" s="1" t="s">
+      <c r="A31" s="3" t="s">
         <v>36</v>
       </c>
       <c r="B31" s="5" t="n">
@@ -12509,7 +12516,7 @@
       </c>
     </row>
     <row r="32" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A32" s="1" t="s">
+      <c r="A32" s="3" t="s">
         <v>37</v>
       </c>
       <c r="B32" s="5" t="n">
@@ -12535,7 +12542,7 @@
       </c>
     </row>
     <row r="33" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A33" s="1" t="s">
+      <c r="A33" s="3" t="s">
         <v>38</v>
       </c>
       <c r="B33" s="5" t="n">
@@ -12561,7 +12568,7 @@
       </c>
     </row>
     <row r="34" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A34" s="1" t="s">
+      <c r="A34" s="3" t="s">
         <v>39</v>
       </c>
       <c r="B34" s="5" t="n">
@@ -12587,7 +12594,7 @@
       </c>
     </row>
     <row r="35" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A35" s="1" t="s">
+      <c r="A35" s="3" t="s">
         <v>40</v>
       </c>
       <c r="B35" s="5" t="n">
@@ -12613,7 +12620,7 @@
       </c>
     </row>
     <row r="36" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A36" s="1" t="s">
+      <c r="A36" s="3" t="s">
         <v>41</v>
       </c>
       <c r="B36" s="5" t="n">
@@ -12639,7 +12646,7 @@
       </c>
     </row>
     <row r="37" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A37" s="1" t="s">
+      <c r="A37" s="3" t="s">
         <v>42</v>
       </c>
       <c r="B37" s="5" t="n">
@@ -12665,7 +12672,7 @@
       </c>
     </row>
     <row r="38" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A38" s="1" t="s">
+      <c r="A38" s="3" t="s">
         <v>43</v>
       </c>
       <c r="B38" s="5" t="n">
@@ -12691,7 +12698,7 @@
       </c>
     </row>
     <row r="39" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A39" s="1" t="s">
+      <c r="A39" s="3" t="s">
         <v>44</v>
       </c>
       <c r="B39" s="5" t="n">
@@ -12717,7 +12724,7 @@
       </c>
     </row>
     <row r="40" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A40" s="1" t="s">
+      <c r="A40" s="3" t="s">
         <v>45</v>
       </c>
       <c r="B40" s="5" t="n">
@@ -12743,7 +12750,7 @@
       </c>
     </row>
     <row r="41" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A41" s="1" t="s">
+      <c r="A41" s="3" t="s">
         <v>46</v>
       </c>
       <c r="B41" s="5" t="n">
@@ -12769,7 +12776,7 @@
       </c>
     </row>
     <row r="42" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A42" s="1" t="s">
+      <c r="A42" s="3" t="s">
         <v>47</v>
       </c>
       <c r="B42" s="5" t="n">
@@ -12795,7 +12802,7 @@
       </c>
     </row>
     <row r="43" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A43" s="1" t="s">
+      <c r="A43" s="3" t="s">
         <v>48</v>
       </c>
       <c r="B43" s="5" t="n">
@@ -12821,7 +12828,7 @@
       </c>
     </row>
     <row r="44" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A44" s="1" t="s">
+      <c r="A44" s="3" t="s">
         <v>49</v>
       </c>
       <c r="B44" s="5" t="n">
@@ -12847,7 +12854,7 @@
       </c>
     </row>
     <row r="45" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A45" s="1" t="s">
+      <c r="A45" s="3" t="s">
         <v>50</v>
       </c>
       <c r="B45" s="5" t="n">
@@ -12873,7 +12880,7 @@
       </c>
     </row>
     <row r="46" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A46" s="1" t="s">
+      <c r="A46" s="3" t="s">
         <v>51</v>
       </c>
       <c r="B46" s="5" t="n">
@@ -12899,7 +12906,7 @@
       </c>
     </row>
     <row r="47" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A47" s="1" t="s">
+      <c r="A47" s="3" t="s">
         <v>52</v>
       </c>
       <c r="B47" s="5" t="n">
@@ -12925,7 +12932,7 @@
       </c>
     </row>
     <row r="48" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A48" s="1" t="s">
+      <c r="A48" s="3" t="s">
         <v>53</v>
       </c>
       <c r="B48" s="5" t="n">
@@ -12951,7 +12958,7 @@
       </c>
     </row>
     <row r="49" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A49" s="1" t="s">
+      <c r="A49" s="3" t="s">
         <v>54</v>
       </c>
       <c r="B49" s="5" t="n">
@@ -12977,7 +12984,7 @@
       </c>
     </row>
     <row r="50" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A50" s="1" t="s">
+      <c r="A50" s="3" t="s">
         <v>55</v>
       </c>
       <c r="B50" s="5" t="n">
@@ -13003,7 +13010,7 @@
       </c>
     </row>
     <row r="51" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A51" s="1" t="s">
+      <c r="A51" s="3" t="s">
         <v>56</v>
       </c>
       <c r="B51" s="5" t="n">
@@ -13029,7 +13036,7 @@
       </c>
     </row>
     <row r="52" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A52" s="1" t="s">
+      <c r="A52" s="3" t="s">
         <v>57</v>
       </c>
       <c r="B52" s="5" t="n">
@@ -13055,7 +13062,7 @@
       </c>
     </row>
     <row r="53" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A53" s="1" t="s">
+      <c r="A53" s="3" t="s">
         <v>58</v>
       </c>
       <c r="B53" s="5" t="n">
@@ -13081,7 +13088,7 @@
       </c>
     </row>
     <row r="54" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A54" s="1" t="s">
+      <c r="A54" s="3" t="s">
         <v>59</v>
       </c>
       <c r="B54" s="5" t="n">
@@ -13107,7 +13114,7 @@
       </c>
     </row>
     <row r="55" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A55" s="1" t="s">
+      <c r="A55" s="3" t="s">
         <v>60</v>
       </c>
       <c r="B55" s="5" t="n">
@@ -13133,7 +13140,7 @@
       </c>
     </row>
     <row r="56" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A56" s="1" t="s">
+      <c r="A56" s="3" t="s">
         <v>61</v>
       </c>
       <c r="B56" s="5" t="n">
@@ -13159,7 +13166,7 @@
       </c>
     </row>
     <row r="57" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A57" s="1" t="s">
+      <c r="A57" s="3" t="s">
         <v>62</v>
       </c>
       <c r="B57" s="5" t="n">
@@ -13185,7 +13192,7 @@
       </c>
     </row>
     <row r="58" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A58" s="1" t="s">
+      <c r="A58" s="3" t="s">
         <v>63</v>
       </c>
       <c r="B58" s="5" t="n">
@@ -13211,7 +13218,7 @@
       </c>
     </row>
     <row r="59" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A59" s="1" t="s">
+      <c r="A59" s="3" t="s">
         <v>64</v>
       </c>
       <c r="B59" s="5" t="n">
@@ -13237,7 +13244,7 @@
       </c>
     </row>
     <row r="60" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A60" s="1" t="s">
+      <c r="A60" s="3" t="s">
         <v>65</v>
       </c>
       <c r="B60" s="5" t="n">
@@ -13263,7 +13270,7 @@
       </c>
     </row>
     <row r="61" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A61" s="1" t="s">
+      <c r="A61" s="3" t="s">
         <v>66</v>
       </c>
       <c r="B61" s="5" t="n">
@@ -13289,7 +13296,7 @@
       </c>
     </row>
     <row r="62" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A62" s="1" t="s">
+      <c r="A62" s="3" t="s">
         <v>67</v>
       </c>
       <c r="B62" s="5" t="n">
@@ -13315,7 +13322,7 @@
       </c>
     </row>
     <row r="63" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A63" s="1" t="s">
+      <c r="A63" s="3" t="s">
         <v>68</v>
       </c>
       <c r="B63" s="5" t="n">
@@ -13341,7 +13348,7 @@
       </c>
     </row>
     <row r="64" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A64" s="1" t="s">
+      <c r="A64" s="3" t="s">
         <v>69</v>
       </c>
       <c r="B64" s="5" t="n">
@@ -13367,7 +13374,7 @@
       </c>
     </row>
     <row r="65" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A65" s="1" t="s">
+      <c r="A65" s="3" t="s">
         <v>70</v>
       </c>
       <c r="B65" s="5" t="n">
@@ -13393,7 +13400,7 @@
       </c>
     </row>
     <row r="66" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A66" s="1" t="s">
+      <c r="A66" s="3" t="s">
         <v>71</v>
       </c>
       <c r="B66" s="5" t="n">
@@ -13419,7 +13426,7 @@
       </c>
     </row>
     <row r="67" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A67" s="1" t="s">
+      <c r="A67" s="3" t="s">
         <v>72</v>
       </c>
       <c r="B67" s="5" t="n">
@@ -13445,7 +13452,7 @@
       </c>
     </row>
     <row r="68" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A68" s="1" t="s">
+      <c r="A68" s="3" t="s">
         <v>73</v>
       </c>
       <c r="B68" s="5" t="n">
@@ -13471,7 +13478,7 @@
       </c>
     </row>
     <row r="69" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A69" s="1" t="s">
+      <c r="A69" s="3" t="s">
         <v>74</v>
       </c>
       <c r="B69" s="5" t="n">
@@ -13497,7 +13504,7 @@
       </c>
     </row>
     <row r="70" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A70" s="1" t="s">
+      <c r="A70" s="3" t="s">
         <v>75</v>
       </c>
       <c r="B70" s="5" t="n">
@@ -13523,7 +13530,7 @@
       </c>
     </row>
     <row r="71" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A71" s="1" t="s">
+      <c r="A71" s="3" t="s">
         <v>76</v>
       </c>
       <c r="B71" s="5" t="n">
@@ -13549,7 +13556,7 @@
       </c>
     </row>
     <row r="72" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A72" s="1" t="s">
+      <c r="A72" s="3" t="s">
         <v>77</v>
       </c>
       <c r="B72" s="5" t="n">
@@ -13575,7 +13582,7 @@
       </c>
     </row>
     <row r="73" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A73" s="1" t="s">
+      <c r="A73" s="3" t="s">
         <v>78</v>
       </c>
       <c r="B73" s="5" t="n">
@@ -13601,7 +13608,7 @@
       </c>
     </row>
     <row r="74" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A74" s="1" t="s">
+      <c r="A74" s="3" t="s">
         <v>79</v>
       </c>
       <c r="B74" s="5" t="n">
@@ -13627,7 +13634,7 @@
       </c>
     </row>
     <row r="75" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A75" s="1" t="s">
+      <c r="A75" s="3" t="s">
         <v>80</v>
       </c>
       <c r="B75" s="5" t="n">
@@ -13653,7 +13660,7 @@
       </c>
     </row>
     <row r="76" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A76" s="1" t="s">
+      <c r="A76" s="3" t="s">
         <v>81</v>
       </c>
       <c r="B76" s="5" t="n">
@@ -13679,7 +13686,7 @@
       </c>
     </row>
     <row r="77" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A77" s="1" t="s">
+      <c r="A77" s="3" t="s">
         <v>82</v>
       </c>
       <c r="B77" s="5" t="n">
@@ -13705,7 +13712,7 @@
       </c>
     </row>
     <row r="78" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A78" s="1" t="s">
+      <c r="A78" s="3" t="s">
         <v>83</v>
       </c>
       <c r="B78" s="5" t="n">
@@ -13731,7 +13738,7 @@
       </c>
     </row>
     <row r="79" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A79" s="1" t="s">
+      <c r="A79" s="3" t="s">
         <v>84</v>
       </c>
       <c r="B79" s="5" t="n">
@@ -13757,7 +13764,7 @@
       </c>
     </row>
     <row r="80" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A80" s="1" t="s">
+      <c r="A80" s="3" t="s">
         <v>85</v>
       </c>
       <c r="B80" s="5" t="n">
@@ -13783,7 +13790,7 @@
       </c>
     </row>
     <row r="81" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A81" s="1" t="s">
+      <c r="A81" s="3" t="s">
         <v>86</v>
       </c>
       <c r="B81" s="5" t="n">
@@ -13809,7 +13816,7 @@
       </c>
     </row>
     <row r="82" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A82" s="1" t="s">
+      <c r="A82" s="3" t="s">
         <v>87</v>
       </c>
       <c r="B82" s="5" t="n">
@@ -13835,7 +13842,7 @@
       </c>
     </row>
     <row r="83" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A83" s="1" t="s">
+      <c r="A83" s="3" t="s">
         <v>88</v>
       </c>
       <c r="B83" s="5" t="n">
@@ -13861,7 +13868,7 @@
       </c>
     </row>
     <row r="84" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A84" s="1" t="s">
+      <c r="A84" s="3" t="s">
         <v>89</v>
       </c>
       <c r="B84" s="5" t="n">
@@ -13887,7 +13894,7 @@
       </c>
     </row>
     <row r="85" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A85" s="1" t="s">
+      <c r="A85" s="3" t="s">
         <v>90</v>
       </c>
       <c r="B85" s="5" t="n">
@@ -13913,7 +13920,7 @@
       </c>
     </row>
     <row r="86" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A86" s="1" t="s">
+      <c r="A86" s="3" t="s">
         <v>91</v>
       </c>
       <c r="B86" s="5" t="n">
@@ -13939,7 +13946,7 @@
       </c>
     </row>
     <row r="87" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A87" s="1" t="s">
+      <c r="A87" s="3" t="s">
         <v>92</v>
       </c>
       <c r="B87" s="5" t="n">
@@ -13965,7 +13972,7 @@
       </c>
     </row>
     <row r="88" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A88" s="1" t="s">
+      <c r="A88" s="3" t="s">
         <v>93</v>
       </c>
       <c r="B88" s="5" t="n">
@@ -13991,7 +13998,7 @@
       </c>
     </row>
     <row r="89" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A89" s="1" t="s">
+      <c r="A89" s="3" t="s">
         <v>94</v>
       </c>
       <c r="B89" s="5" t="n">
@@ -14017,7 +14024,7 @@
       </c>
     </row>
     <row r="90" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A90" s="1" t="s">
+      <c r="A90" s="3" t="s">
         <v>95</v>
       </c>
       <c r="B90" s="5" t="n">

</xml_diff>

<commit_message>
add first second part of second plate results
</commit_message>
<xml_diff>
--- a/data/First_round_results/Results - First Plate 3 reps.xlsx
+++ b/data/First_round_results/Results - First Plate 3 reps.xlsx
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="480" uniqueCount="96">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="570" uniqueCount="185">
   <si>
     <t xml:space="preserve">RBS</t>
   </si>
@@ -312,15 +312,283 @@
   </si>
   <si>
     <t xml:space="preserve">TTTAAGACGAGACTATACAT</t>
+  </si>
+  <si>
+    <t xml:space="preserve">tttaagaGAAAGAtatacat</t>
+  </si>
+  <si>
+    <t xml:space="preserve">tttaagaCGGGGGtatacat</t>
+  </si>
+  <si>
+    <t xml:space="preserve">tttaagaTGAGGGtatacat</t>
+  </si>
+  <si>
+    <t xml:space="preserve">tttaagaCCGGGAtatacat</t>
+  </si>
+  <si>
+    <t xml:space="preserve">tttaagaAAGGGTtatacat</t>
+  </si>
+  <si>
+    <t xml:space="preserve">tttaagaCTGTAGtatacat</t>
+  </si>
+  <si>
+    <t xml:space="preserve">tttaagaCTGACAtatacat</t>
+  </si>
+  <si>
+    <t xml:space="preserve">tttaagaCGTGTGtatacat</t>
+  </si>
+  <si>
+    <t xml:space="preserve">tttaagaGAGGGGtatacat</t>
+  </si>
+  <si>
+    <t xml:space="preserve">tttaagaCTAGGAtatacat</t>
+  </si>
+  <si>
+    <t xml:space="preserve">tttaagaATTGGGtatacat</t>
+  </si>
+  <si>
+    <t xml:space="preserve">tttaagaTACTGAtatacat</t>
+  </si>
+  <si>
+    <t xml:space="preserve">tttaagaAGAGCGtatacat</t>
+  </si>
+  <si>
+    <t xml:space="preserve">tttaagaAGGGGTtatacat</t>
+  </si>
+  <si>
+    <t xml:space="preserve">tttaagaCTGGGGtatacat</t>
+  </si>
+  <si>
+    <t xml:space="preserve">tttaagaCAAGCCtatacat</t>
+  </si>
+  <si>
+    <t xml:space="preserve">tttaagaCAATTGtatacat</t>
+  </si>
+  <si>
+    <t xml:space="preserve">tttaagaTATTTTtatacat</t>
+  </si>
+  <si>
+    <t xml:space="preserve">tttaagaTCCGGCtatacat</t>
+  </si>
+  <si>
+    <t xml:space="preserve">tttaagaTGGGAGtatacat</t>
+  </si>
+  <si>
+    <t xml:space="preserve">tttaagaAAAGTGtatacat</t>
+  </si>
+  <si>
+    <t xml:space="preserve">tttaagaCGGGAGtatacat</t>
+  </si>
+  <si>
+    <t xml:space="preserve">tttaagaTAAGAGtatacat</t>
+  </si>
+  <si>
+    <t xml:space="preserve">tttaagaTAAGGGtatacat</t>
+  </si>
+  <si>
+    <t xml:space="preserve">tttaagaTAGTCTtatacat</t>
+  </si>
+  <si>
+    <t xml:space="preserve">tttaagaAAGTAGtatacat</t>
+  </si>
+  <si>
+    <t xml:space="preserve">tttaagaCCACGCtatacat</t>
+  </si>
+  <si>
+    <t xml:space="preserve">tttaagaGTAATGtatacat</t>
+  </si>
+  <si>
+    <t xml:space="preserve">tttaagaCATTGAtatacat</t>
+  </si>
+  <si>
+    <t xml:space="preserve">TTTAAGACGGATTTATACAT</t>
+  </si>
+  <si>
+    <t xml:space="preserve">TTTAAGATTCGGATATACAT</t>
+  </si>
+  <si>
+    <t xml:space="preserve">TTTAAGACTCGGATATACAT</t>
+  </si>
+  <si>
+    <t xml:space="preserve">TTTAAGAACCGGATATACAT</t>
+  </si>
+  <si>
+    <t xml:space="preserve">TTTAAGAGCCGGATATACAT</t>
+  </si>
+  <si>
+    <t xml:space="preserve">TTTAAGAATCGGATATACAT</t>
+  </si>
+  <si>
+    <t xml:space="preserve">TTTAAGACCGGATTATACAT</t>
+  </si>
+  <si>
+    <t xml:space="preserve">TTTAAGATAAAGATATACAT</t>
+  </si>
+  <si>
+    <t xml:space="preserve">TTTAAGACGATAATATACAT</t>
+  </si>
+  <si>
+    <t xml:space="preserve">TTTAAGAACACACTATACAT</t>
+  </si>
+  <si>
+    <t xml:space="preserve">TTTAAGATATATATATACAT</t>
+  </si>
+  <si>
+    <t xml:space="preserve">TTTAAGACTCTCTTATACAT</t>
+  </si>
+  <si>
+    <t xml:space="preserve">TTTAAGAGTGTGTTATACAT</t>
+  </si>
+  <si>
+    <t xml:space="preserve">TTTAAGAATATATTATACAT</t>
+  </si>
+  <si>
+    <t xml:space="preserve">TTTAAGATGTGTGTATACAT</t>
+  </si>
+  <si>
+    <t xml:space="preserve">TTTAAGATCTCTCTATACAT</t>
+  </si>
+  <si>
+    <t xml:space="preserve">TTTAAGACACACATATACAT</t>
+  </si>
+  <si>
+    <t xml:space="preserve">TTTAAGACTAAGATATACAT</t>
+  </si>
+  <si>
+    <t xml:space="preserve">TTTAAGAATAAGATATACAT</t>
+  </si>
+  <si>
+    <t xml:space="preserve">TTTAAGATAAGATTATACAT</t>
+  </si>
+  <si>
+    <t xml:space="preserve">TTTAAGATTAAGATATACAT</t>
+  </si>
+  <si>
+    <t xml:space="preserve">TTTAAGAGGTCGATATACAT</t>
+  </si>
+  <si>
+    <t xml:space="preserve">TTTAAGAGGTAGATATACAT</t>
+  </si>
+  <si>
+    <t xml:space="preserve">TTTAAGAGGAAGATATACAT</t>
+  </si>
+  <si>
+    <t xml:space="preserve">TTTAAGAGGGGGATATACAT</t>
+  </si>
+  <si>
+    <t xml:space="preserve">TTTAAGAGGGGATTATACAT</t>
+  </si>
+  <si>
+    <t xml:space="preserve">TTTAAGAGGGATCTATACAT</t>
+  </si>
+  <si>
+    <t xml:space="preserve">TTTAAGAGGGATTTATACAT</t>
+  </si>
+  <si>
+    <t xml:space="preserve">TTTAAGAGGGATGTATACAT</t>
+  </si>
+  <si>
+    <t xml:space="preserve">TTTAAGAGGGATATATACAT</t>
+  </si>
+  <si>
+    <t xml:space="preserve">TTTAAGAGGATCTTATACAT</t>
+  </si>
+  <si>
+    <t xml:space="preserve">TTTAAGAGGATTTTATACAT</t>
+  </si>
+  <si>
+    <t xml:space="preserve">TTTAAGAGGATAGTATACAT</t>
+  </si>
+  <si>
+    <t xml:space="preserve">TTTAAGAGGATTATATACAT</t>
+  </si>
+  <si>
+    <t xml:space="preserve">TTTAAGAGGATATTATACAT</t>
+  </si>
+  <si>
+    <t xml:space="preserve">TTTAAGAGGATACTATACAT</t>
+  </si>
+  <si>
+    <t xml:space="preserve">TTTAAGAGGATGCTATACAT</t>
+  </si>
+  <si>
+    <t xml:space="preserve">TTTAAGAGGATGTTATACAT</t>
+  </si>
+  <si>
+    <t xml:space="preserve">TTTAAGAGGATTCTATACAT</t>
+  </si>
+  <si>
+    <t xml:space="preserve">TTTAAGAGGATCGTATACAT</t>
+  </si>
+  <si>
+    <t xml:space="preserve">TTTAAGAGGATTGTATACAT</t>
+  </si>
+  <si>
+    <t xml:space="preserve">TTTAAGAGGATCCTATACAT</t>
+  </si>
+  <si>
+    <t xml:space="preserve">TTTAAGAGGATGATATACAT</t>
+  </si>
+  <si>
+    <t xml:space="preserve">TTTAAGAGGATCATATACAT</t>
+  </si>
+  <si>
+    <t xml:space="preserve">TTTAAGACCCCGATATACAT</t>
+  </si>
+  <si>
+    <t xml:space="preserve">TTTAAGATTTTTGTATACAT</t>
+  </si>
+  <si>
+    <t xml:space="preserve">TTTAAGATTTTTATATACAT</t>
+  </si>
+  <si>
+    <t xml:space="preserve">TTTAAGAGTTTTTTATACAT</t>
+  </si>
+  <si>
+    <t xml:space="preserve">TTTAAGACTTTTTTATACAT</t>
+  </si>
+  <si>
+    <t xml:space="preserve">TTTAAGACCCCCTTATACAT</t>
+  </si>
+  <si>
+    <t xml:space="preserve">TTTAAGACCCCCGTATACAT</t>
+  </si>
+  <si>
+    <t xml:space="preserve">TTTAAGACCCCCATATACAT</t>
+  </si>
+  <si>
+    <t xml:space="preserve">TTTAAGATTTTTCTATACAT</t>
+  </si>
+  <si>
+    <t xml:space="preserve">TTTAAGAGCCCCCTATACAT</t>
+  </si>
+  <si>
+    <t xml:space="preserve">TTTAAGAATTTTTTATACAT</t>
+  </si>
+  <si>
+    <t xml:space="preserve">TTTAAGAACCCCCTATACAT</t>
+  </si>
+  <si>
+    <t xml:space="preserve">TTTAAGATCCCCCTATACAT</t>
+  </si>
+  <si>
+    <t xml:space="preserve">TTTAAGAGGATAATATACAT</t>
+  </si>
+  <si>
+    <t xml:space="preserve">TTTAAGACCCCCCTATACAT</t>
+  </si>
+  <si>
+    <t xml:space="preserve">TTTAAGATTTTTTTATACAT</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <numFmts count="2">
+  <numFmts count="3">
     <numFmt numFmtId="164" formatCode="General"/>
     <numFmt numFmtId="165" formatCode="0.00%"/>
+    <numFmt numFmtId="166" formatCode="0.00"/>
   </numFmts>
   <fonts count="7">
     <font>
@@ -367,7 +635,7 @@
       <charset val="1"/>
     </font>
   </fonts>
-  <fills count="3">
+  <fills count="4">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -377,6 +645,12 @@
     <fill>
       <patternFill patternType="solid">
         <fgColor rgb="FFFFFF00"/>
+        <bgColor rgb="FFFFF200"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFF200"/>
         <bgColor rgb="FFFFFF00"/>
       </patternFill>
     </fill>
@@ -422,7 +696,7 @@
     <xf numFmtId="42" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
     <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
   </cellStyleXfs>
-  <cellXfs count="8">
+  <cellXfs count="14">
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
@@ -455,6 +729,30 @@
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="general" vertical="center" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="166" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="general" vertical="center" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="3" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="general" vertical="center" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="165" fontId="0" fillId="3" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="general" vertical="center" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
   </cellXfs>
   <cellStyles count="6">
     <cellStyle name="Normal" xfId="0" builtinId="0" customBuiltin="false"/>
@@ -464,6 +762,66 @@
     <cellStyle name="Currency [0]" xfId="18" builtinId="7" customBuiltin="false"/>
     <cellStyle name="Percent" xfId="19" builtinId="5" customBuiltin="false"/>
   </cellStyles>
+  <colors>
+    <indexedColors>
+      <rgbColor rgb="FF000000"/>
+      <rgbColor rgb="FFFFFFFF"/>
+      <rgbColor rgb="FFFF0000"/>
+      <rgbColor rgb="FF00FF00"/>
+      <rgbColor rgb="FF0000FF"/>
+      <rgbColor rgb="FFFFFF00"/>
+      <rgbColor rgb="FFFF00FF"/>
+      <rgbColor rgb="FF00FFFF"/>
+      <rgbColor rgb="FF800000"/>
+      <rgbColor rgb="FF008000"/>
+      <rgbColor rgb="FF000080"/>
+      <rgbColor rgb="FF808000"/>
+      <rgbColor rgb="FF800080"/>
+      <rgbColor rgb="FF008080"/>
+      <rgbColor rgb="FFC0C0C0"/>
+      <rgbColor rgb="FF808080"/>
+      <rgbColor rgb="FF9999FF"/>
+      <rgbColor rgb="FF993366"/>
+      <rgbColor rgb="FFFFFFCC"/>
+      <rgbColor rgb="FFCCFFFF"/>
+      <rgbColor rgb="FF660066"/>
+      <rgbColor rgb="FFFF8080"/>
+      <rgbColor rgb="FF0066CC"/>
+      <rgbColor rgb="FFCCCCFF"/>
+      <rgbColor rgb="FF000080"/>
+      <rgbColor rgb="FFFF00FF"/>
+      <rgbColor rgb="FFFFF200"/>
+      <rgbColor rgb="FF00FFFF"/>
+      <rgbColor rgb="FF800080"/>
+      <rgbColor rgb="FF800000"/>
+      <rgbColor rgb="FF008080"/>
+      <rgbColor rgb="FF0000FF"/>
+      <rgbColor rgb="FF00CCFF"/>
+      <rgbColor rgb="FFCCFFFF"/>
+      <rgbColor rgb="FFCCFFCC"/>
+      <rgbColor rgb="FFFFFF99"/>
+      <rgbColor rgb="FF99CCFF"/>
+      <rgbColor rgb="FFFF99CC"/>
+      <rgbColor rgb="FFCC99FF"/>
+      <rgbColor rgb="FFFFCC99"/>
+      <rgbColor rgb="FF3366FF"/>
+      <rgbColor rgb="FF33CCCC"/>
+      <rgbColor rgb="FF99CC00"/>
+      <rgbColor rgb="FFFFCC00"/>
+      <rgbColor rgb="FFFF9900"/>
+      <rgbColor rgb="FFFF6600"/>
+      <rgbColor rgb="FF666699"/>
+      <rgbColor rgb="FF969696"/>
+      <rgbColor rgb="FF003366"/>
+      <rgbColor rgb="FF339966"/>
+      <rgbColor rgb="FF003300"/>
+      <rgbColor rgb="FF333300"/>
+      <rgbColor rgb="FF993300"/>
+      <rgbColor rgb="FF993366"/>
+      <rgbColor rgb="FF333399"/>
+      <rgbColor rgb="FF333333"/>
+    </indexedColors>
+  </colors>
 </styleSheet>
 </file>
 
@@ -474,7 +832,7 @@
   </sheetPr>
   <dimension ref="A1:DJ91"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A61" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
       <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
     </sheetView>
   </sheetViews>
@@ -11699,10 +12057,10 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:G90"/>
+  <dimension ref="A1:G180"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="Q10" activeCellId="0" sqref="Q10"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A162" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="G185" activeCellId="0" sqref="G185"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -13366,11 +13724,11 @@
       </c>
       <c r="F64" s="0" t="n">
         <f aca="false">_xlfn.STDEV.P(B64:C64)</f>
-        <v>0.862875000000001</v>
+        <v>0.862875</v>
       </c>
       <c r="G64" s="4" t="n">
         <f aca="false">F64/E64</f>
-        <v>0.0635458179800329</v>
+        <v>0.0635458179800328</v>
       </c>
     </row>
     <row r="65" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -13860,11 +14218,11 @@
       </c>
       <c r="F83" s="0" t="n">
         <f aca="false">_xlfn.STDEV.P(B83:C83)</f>
-        <v>0.919799999999999</v>
+        <v>0.9198</v>
       </c>
       <c r="G83" s="4" t="n">
         <f aca="false">F83/E83</f>
-        <v>0.0527446666127636</v>
+        <v>0.0527446666127637</v>
       </c>
     </row>
     <row r="84" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -14047,6 +14405,2346 @@
       <c r="G90" s="4" t="n">
         <f aca="false">F90/E90</f>
         <v>0.0445642192472993</v>
+      </c>
+    </row>
+    <row r="91" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A91" s="8" t="s">
+        <v>96</v>
+      </c>
+      <c r="B91" s="9" t="n">
+        <v>30.7805316021367</v>
+      </c>
+      <c r="C91" s="9" t="n">
+        <v>30.4426820899785</v>
+      </c>
+      <c r="D91" s="10" t="n">
+        <v>30.0968179564725</v>
+      </c>
+      <c r="E91" s="8" t="n">
+        <f aca="false">AVERAGE(B91:D91)</f>
+        <v>30.4400105495292</v>
+      </c>
+      <c r="F91" s="8" t="n">
+        <f aca="false">_xlfn.STDEV.P(B91:D91)</f>
+        <v>0.279131319350023</v>
+      </c>
+      <c r="G91" s="11" t="n">
+        <f aca="false">F91/E91</f>
+        <v>0.00916988247740078</v>
+      </c>
+    </row>
+    <row r="92" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A92" s="12" t="s">
+        <v>97</v>
+      </c>
+      <c r="B92" s="9" t="n">
+        <v>209.268707482993</v>
+      </c>
+      <c r="C92" s="9" t="n">
+        <v>174.814814814815</v>
+      </c>
+      <c r="D92" s="10" t="n">
+        <v>161.481481481481</v>
+      </c>
+      <c r="E92" s="12" t="n">
+        <f aca="false">AVERAGE(B92:D92)</f>
+        <v>181.855001259763</v>
+      </c>
+      <c r="F92" s="12" t="n">
+        <f aca="false">_xlfn.STDEV.P(B92:D92)</f>
+        <v>20.1341817334704</v>
+      </c>
+      <c r="G92" s="13" t="n">
+        <f aca="false">F92/E92</f>
+        <v>0.110715578862253</v>
+      </c>
+    </row>
+    <row r="93" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A93" s="8" t="s">
+        <v>98</v>
+      </c>
+      <c r="B93" s="9" t="n">
+        <v>23.8595502635998</v>
+      </c>
+      <c r="C93" s="9" t="n">
+        <v>19.5759934373255</v>
+      </c>
+      <c r="D93" s="10" t="n">
+        <v>21.3450622747192</v>
+      </c>
+      <c r="E93" s="8" t="n">
+        <f aca="false">AVERAGE(B93:D93)</f>
+        <v>21.5935353252148</v>
+      </c>
+      <c r="F93" s="8" t="n">
+        <f aca="false">_xlfn.STDEV.P(B93:D93)</f>
+        <v>1.75755870714603</v>
+      </c>
+      <c r="G93" s="11" t="n">
+        <f aca="false">F93/E93</f>
+        <v>0.0813928187615356</v>
+      </c>
+    </row>
+    <row r="94" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A94" s="8" t="s">
+        <v>99</v>
+      </c>
+      <c r="B94" s="9" t="n">
+        <v>21.1668611445581</v>
+      </c>
+      <c r="C94" s="9" t="n">
+        <v>20.0566337062376</v>
+      </c>
+      <c r="D94" s="10" t="n">
+        <v>19.5192351567033</v>
+      </c>
+      <c r="E94" s="8" t="n">
+        <f aca="false">AVERAGE(B94:D94)</f>
+        <v>20.2475766691663</v>
+      </c>
+      <c r="F94" s="8" t="n">
+        <f aca="false">_xlfn.STDEV.P(B94:D94)</f>
+        <v>0.686057461287612</v>
+      </c>
+      <c r="G94" s="11" t="n">
+        <f aca="false">F94/E94</f>
+        <v>0.0338834356573823</v>
+      </c>
+    </row>
+    <row r="95" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A95" s="12" t="s">
+        <v>100</v>
+      </c>
+      <c r="B95" s="9" t="n">
+        <v>225.18115942029</v>
+      </c>
+      <c r="C95" s="9" t="n">
+        <v>173.240740740741</v>
+      </c>
+      <c r="D95" s="10" t="n">
+        <v>162.777777777778</v>
+      </c>
+      <c r="E95" s="12" t="n">
+        <f aca="false">AVERAGE(B95:D95)</f>
+        <v>187.066559312936</v>
+      </c>
+      <c r="F95" s="12" t="n">
+        <f aca="false">_xlfn.STDEV.P(B95:D95)</f>
+        <v>27.2874874194346</v>
+      </c>
+      <c r="G95" s="13" t="n">
+        <f aca="false">F95/E95</f>
+        <v>0.145870472625663</v>
+      </c>
+    </row>
+    <row r="96" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A96" s="8" t="s">
+        <v>101</v>
+      </c>
+      <c r="B96" s="9" t="n">
+        <v>20.149038133154</v>
+      </c>
+      <c r="C96" s="9" t="n">
+        <v>20.6030329668822</v>
+      </c>
+      <c r="D96" s="10" t="n">
+        <v>17.4359417900153</v>
+      </c>
+      <c r="E96" s="8" t="n">
+        <f aca="false">AVERAGE(B96:D96)</f>
+        <v>19.3960042966838</v>
+      </c>
+      <c r="F96" s="8" t="n">
+        <f aca="false">_xlfn.STDEV.P(B96:D96)</f>
+        <v>1.39831126715972</v>
+      </c>
+      <c r="G96" s="11" t="n">
+        <f aca="false">F96/E96</f>
+        <v>0.0720927488863665</v>
+      </c>
+    </row>
+    <row r="97" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A97" s="8" t="s">
+        <v>102</v>
+      </c>
+      <c r="B97" s="9" t="n">
+        <v>18.5718428079613</v>
+      </c>
+      <c r="C97" s="9" t="n">
+        <v>19.0974911579163</v>
+      </c>
+      <c r="D97" s="10" t="n">
+        <v>14.8170368873931</v>
+      </c>
+      <c r="E97" s="8" t="n">
+        <f aca="false">AVERAGE(B97:D97)</f>
+        <v>17.4954569510902</v>
+      </c>
+      <c r="F97" s="8" t="n">
+        <f aca="false">_xlfn.STDEV.P(B97:D97)</f>
+        <v>1.90604775651328</v>
+      </c>
+      <c r="G97" s="11" t="n">
+        <f aca="false">F97/E97</f>
+        <v>0.10894529716153</v>
+      </c>
+    </row>
+    <row r="98" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A98" s="12" t="s">
+        <v>103</v>
+      </c>
+      <c r="B98" s="9" t="n">
+        <v>203.421900161031</v>
+      </c>
+      <c r="C98" s="9" t="n">
+        <v>164.836956521739</v>
+      </c>
+      <c r="D98" s="10" t="n">
+        <v>167.407407407407</v>
+      </c>
+      <c r="E98" s="12" t="n">
+        <f aca="false">AVERAGE(B98:D98)</f>
+        <v>178.555421363392</v>
+      </c>
+      <c r="F98" s="12" t="n">
+        <f aca="false">_xlfn.STDEV.P(B98:D98)</f>
+        <v>17.6145419144514</v>
+      </c>
+      <c r="G98" s="13" t="n">
+        <f aca="false">F98/E98</f>
+        <v>0.0986502777678347</v>
+      </c>
+    </row>
+    <row r="99" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A99" s="8" t="s">
+        <v>104</v>
+      </c>
+      <c r="B99" s="9" t="n">
+        <v>18.9136096838775</v>
+      </c>
+      <c r="C99" s="9" t="n">
+        <v>17.7557818893671</v>
+      </c>
+      <c r="D99" s="10" t="n">
+        <v>13.7937856305341</v>
+      </c>
+      <c r="E99" s="8" t="n">
+        <f aca="false">AVERAGE(B99:D99)</f>
+        <v>16.8210590679262</v>
+      </c>
+      <c r="F99" s="8" t="n">
+        <f aca="false">_xlfn.STDEV.P(B99:D99)</f>
+        <v>2.19217238509963</v>
+      </c>
+      <c r="G99" s="11" t="n">
+        <f aca="false">F99/E99</f>
+        <v>0.130323089423043</v>
+      </c>
+    </row>
+    <row r="100" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A100" s="8" t="s">
+        <v>105</v>
+      </c>
+      <c r="B100" s="9" t="n">
+        <v>17.1505132580184</v>
+      </c>
+      <c r="C100" s="9" t="n">
+        <v>15.9461635698141</v>
+      </c>
+      <c r="D100" s="10" t="n">
+        <v>14.3003078998694</v>
+      </c>
+      <c r="E100" s="8" t="n">
+        <f aca="false">AVERAGE(B100:D100)</f>
+        <v>15.798994909234</v>
+      </c>
+      <c r="F100" s="8" t="n">
+        <f aca="false">_xlfn.STDEV.P(B100:D100)</f>
+        <v>1.16823559464638</v>
+      </c>
+      <c r="G100" s="11" t="n">
+        <f aca="false">F100/E100</f>
+        <v>0.0739436654899851</v>
+      </c>
+    </row>
+    <row r="101" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A101" s="8" t="s">
+        <v>106</v>
+      </c>
+      <c r="B101" s="9" t="n">
+        <v>18.4830085013517</v>
+      </c>
+      <c r="C101" s="9" t="n">
+        <v>15.1669406270928</v>
+      </c>
+      <c r="D101" s="10" t="n">
+        <v>14.5413537960461</v>
+      </c>
+      <c r="E101" s="8" t="n">
+        <f aca="false">AVERAGE(B101:D101)</f>
+        <v>16.0637676414969</v>
+      </c>
+      <c r="F101" s="8" t="n">
+        <f aca="false">_xlfn.STDEV.P(B101:D101)</f>
+        <v>1.72962124452883</v>
+      </c>
+      <c r="G101" s="11" t="n">
+        <f aca="false">F101/E101</f>
+        <v>0.107672202632013</v>
+      </c>
+    </row>
+    <row r="102" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A102" s="8" t="s">
+        <v>107</v>
+      </c>
+      <c r="B102" s="9" t="n">
+        <v>22.9857538082425</v>
+      </c>
+      <c r="C102" s="9" t="n">
+        <v>17.3014393644971</v>
+      </c>
+      <c r="D102" s="10" t="n">
+        <v>18.7596389638528</v>
+      </c>
+      <c r="E102" s="8" t="n">
+        <f aca="false">AVERAGE(B102:D102)</f>
+        <v>19.6822773788641</v>
+      </c>
+      <c r="F102" s="8" t="n">
+        <f aca="false">_xlfn.STDEV.P(B102:D102)</f>
+        <v>2.41057446922016</v>
+      </c>
+      <c r="G102" s="11" t="n">
+        <f aca="false">F102/E102</f>
+        <v>0.122474367311212</v>
+      </c>
+    </row>
+    <row r="103" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A103" s="12" t="s">
+        <v>108</v>
+      </c>
+      <c r="B103" s="9" t="n">
+        <v>227.536231884058</v>
+      </c>
+      <c r="C103" s="9" t="n">
+        <v>216.574074074074</v>
+      </c>
+      <c r="D103" s="10" t="n">
+        <v>172.87037037037</v>
+      </c>
+      <c r="E103" s="12" t="n">
+        <f aca="false">AVERAGE(B103:D103)</f>
+        <v>205.660225442834</v>
+      </c>
+      <c r="F103" s="12" t="n">
+        <f aca="false">_xlfn.STDEV.P(B103:D103)</f>
+        <v>23.6138825371522</v>
+      </c>
+      <c r="G103" s="13" t="n">
+        <f aca="false">F103/E103</f>
+        <v>0.114819880637133</v>
+      </c>
+    </row>
+    <row r="104" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A104" s="8" t="s">
+        <v>109</v>
+      </c>
+      <c r="B104" s="9" t="n">
+        <v>21.0968257431605</v>
+      </c>
+      <c r="C104" s="9" t="n">
+        <v>19.717793843533</v>
+      </c>
+      <c r="D104" s="10" t="n">
+        <v>17.750195391975</v>
+      </c>
+      <c r="E104" s="8" t="n">
+        <f aca="false">AVERAGE(B104:D104)</f>
+        <v>19.5216049928895</v>
+      </c>
+      <c r="F104" s="8" t="n">
+        <f aca="false">_xlfn.STDEV.P(B104:D104)</f>
+        <v>1.3732810408426</v>
+      </c>
+      <c r="G104" s="11" t="n">
+        <f aca="false">F104/E104</f>
+        <v>0.0703467282194675</v>
+      </c>
+    </row>
+    <row r="105" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A105" s="8" t="s">
+        <v>110</v>
+      </c>
+      <c r="B105" s="9" t="n">
+        <v>17.3815840751345</v>
+      </c>
+      <c r="C105" s="9" t="n">
+        <v>13.8441727348063</v>
+      </c>
+      <c r="D105" s="10" t="n">
+        <v>16.2135213755028</v>
+      </c>
+      <c r="E105" s="8" t="n">
+        <f aca="false">AVERAGE(B105:D105)</f>
+        <v>15.8130927284812</v>
+      </c>
+      <c r="F105" s="8" t="n">
+        <f aca="false">_xlfn.STDEV.P(B105:D105)</f>
+        <v>1.47163787975335</v>
+      </c>
+      <c r="G105" s="11" t="n">
+        <f aca="false">F105/E105</f>
+        <v>0.0930645197003593</v>
+      </c>
+    </row>
+    <row r="106" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A106" s="8" t="s">
+        <v>111</v>
+      </c>
+      <c r="B106" s="9" t="n">
+        <v>10.4926175959423</v>
+      </c>
+      <c r="C106" s="9" t="n">
+        <v>15.5397703389723</v>
+      </c>
+      <c r="D106" s="10" t="n">
+        <v>9.97518034155952</v>
+      </c>
+      <c r="E106" s="8" t="n">
+        <f aca="false">AVERAGE(B106:D106)</f>
+        <v>12.0025227588247</v>
+      </c>
+      <c r="F106" s="8" t="n">
+        <f aca="false">_xlfn.STDEV.P(B106:D106)</f>
+        <v>2.51011628688139</v>
+      </c>
+      <c r="G106" s="11" t="n">
+        <f aca="false">F106/E106</f>
+        <v>0.209132391357963</v>
+      </c>
+    </row>
+    <row r="107" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A107" s="8" t="s">
+        <v>112</v>
+      </c>
+      <c r="B107" s="9" t="n">
+        <v>10.1434903215865</v>
+      </c>
+      <c r="C107" s="9" t="n">
+        <v>14.2192880841743</v>
+      </c>
+      <c r="D107" s="10" t="n">
+        <v>6.43946629805588</v>
+      </c>
+      <c r="E107" s="8" t="n">
+        <f aca="false">AVERAGE(B107:D107)</f>
+        <v>10.2674149012722</v>
+      </c>
+      <c r="F107" s="8" t="n">
+        <f aca="false">_xlfn.STDEV.P(B107:D107)</f>
+        <v>3.17730753228039</v>
+      </c>
+      <c r="G107" s="11" t="n">
+        <f aca="false">F107/E107</f>
+        <v>0.309455453279354</v>
+      </c>
+    </row>
+    <row r="108" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A108" s="8" t="s">
+        <v>113</v>
+      </c>
+      <c r="B108" s="9" t="n">
+        <v>8.66776352021093</v>
+      </c>
+      <c r="C108" s="9" t="n">
+        <v>8.79071010929643</v>
+      </c>
+      <c r="D108" s="10" t="n">
+        <v>13.4609427777435</v>
+      </c>
+      <c r="E108" s="8" t="n">
+        <f aca="false">AVERAGE(B108:D108)</f>
+        <v>10.3064721357503</v>
+      </c>
+      <c r="F108" s="8" t="n">
+        <f aca="false">_xlfn.STDEV.P(B108:D108)</f>
+        <v>2.23111223971958</v>
+      </c>
+      <c r="G108" s="11" t="n">
+        <f aca="false">F108/E108</f>
+        <v>0.216476812854369</v>
+      </c>
+    </row>
+    <row r="109" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A109" s="8" t="s">
+        <v>114</v>
+      </c>
+      <c r="B109" s="9" t="n">
+        <v>14.356465420976</v>
+      </c>
+      <c r="C109" s="9" t="n">
+        <v>9.07206281977669</v>
+      </c>
+      <c r="D109" s="10" t="n">
+        <v>7.7126794951582</v>
+      </c>
+      <c r="E109" s="8" t="n">
+        <f aca="false">AVERAGE(B109:D109)</f>
+        <v>10.380402578637</v>
+      </c>
+      <c r="F109" s="8" t="n">
+        <f aca="false">_xlfn.STDEV.P(B109:D109)</f>
+        <v>2.86575034391631</v>
+      </c>
+      <c r="G109" s="11" t="n">
+        <f aca="false">F109/E109</f>
+        <v>0.276073140921728</v>
+      </c>
+    </row>
+    <row r="110" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A110" s="8" t="s">
+        <v>115</v>
+      </c>
+      <c r="B110" s="9" t="n">
+        <v>9.6298471484311</v>
+      </c>
+      <c r="C110" s="9" t="n">
+        <v>8.28354885036655</v>
+      </c>
+      <c r="D110" s="10" t="n">
+        <v>6.50380172451121</v>
+      </c>
+      <c r="E110" s="8" t="n">
+        <f aca="false">AVERAGE(B110:D110)</f>
+        <v>8.13906590776962</v>
+      </c>
+      <c r="F110" s="8" t="n">
+        <f aca="false">_xlfn.STDEV.P(B110:D110)</f>
+        <v>1.2802855120711</v>
+      </c>
+      <c r="G110" s="11" t="n">
+        <f aca="false">F110/E110</f>
+        <v>0.157301283289637</v>
+      </c>
+    </row>
+    <row r="111" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A111" s="8" t="s">
+        <v>116</v>
+      </c>
+      <c r="B111" s="9" t="n">
+        <v>9.80546943431823</v>
+      </c>
+      <c r="C111" s="9" t="n">
+        <v>5.19154895037389</v>
+      </c>
+      <c r="D111" s="10" t="n">
+        <v>11.009068973732</v>
+      </c>
+      <c r="E111" s="8" t="n">
+        <f aca="false">AVERAGE(B111:D111)</f>
+        <v>8.66869578614139</v>
+      </c>
+      <c r="F111" s="8" t="n">
+        <f aca="false">_xlfn.STDEV.P(B111:D111)</f>
+        <v>2.50733265323068</v>
+      </c>
+      <c r="G111" s="11" t="n">
+        <f aca="false">F111/E111</f>
+        <v>0.289239894337871</v>
+      </c>
+    </row>
+    <row r="112" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A112" s="12" t="s">
+        <v>117</v>
+      </c>
+      <c r="B112" s="9" t="n">
+        <v>173.404255319149</v>
+      </c>
+      <c r="C112" s="9" t="n">
+        <v>151.347132284921</v>
+      </c>
+      <c r="D112" s="10" t="n">
+        <v>124.313906876349</v>
+      </c>
+      <c r="E112" s="12" t="n">
+        <f aca="false">AVERAGE(B112:D112)</f>
+        <v>149.688431493473</v>
+      </c>
+      <c r="F112" s="12" t="n">
+        <f aca="false">_xlfn.STDEV.P(B112:D112)</f>
+        <v>20.0753421522613</v>
+      </c>
+      <c r="G112" s="13" t="n">
+        <f aca="false">F112/E112</f>
+        <v>0.134114186059439</v>
+      </c>
+    </row>
+    <row r="113" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A113" s="12" t="s">
+        <v>118</v>
+      </c>
+      <c r="B113" s="9" t="n">
+        <v>181.105072463768</v>
+      </c>
+      <c r="C113" s="9" t="n">
+        <v>148.333333333333</v>
+      </c>
+      <c r="D113" s="10" t="n">
+        <v>143.333333333333</v>
+      </c>
+      <c r="E113" s="12" t="n">
+        <f aca="false">AVERAGE(B113:D113)</f>
+        <v>157.590579710145</v>
+      </c>
+      <c r="F113" s="12" t="n">
+        <f aca="false">_xlfn.STDEV.P(B113:D113)</f>
+        <v>16.7520849865552</v>
+      </c>
+      <c r="G113" s="13" t="n">
+        <f aca="false">F113/E113</f>
+        <v>0.106301309490499</v>
+      </c>
+    </row>
+    <row r="114" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A114" s="8" t="s">
+        <v>119</v>
+      </c>
+      <c r="B114" s="9" t="n">
+        <v>32.554580912047</v>
+      </c>
+      <c r="C114" s="9" t="n">
+        <v>35.0535797366133</v>
+      </c>
+      <c r="D114" s="10" t="n">
+        <v>34.5102949680361</v>
+      </c>
+      <c r="E114" s="8" t="n">
+        <f aca="false">AVERAGE(B114:D114)</f>
+        <v>34.0394852055655</v>
+      </c>
+      <c r="F114" s="8" t="n">
+        <f aca="false">_xlfn.STDEV.P(B114:D114)</f>
+        <v>1.07315583075467</v>
+      </c>
+      <c r="G114" s="11" t="n">
+        <f aca="false">F114/E114</f>
+        <v>0.0315267937888559</v>
+      </c>
+    </row>
+    <row r="115" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A115" s="12" t="s">
+        <v>120</v>
+      </c>
+      <c r="B115" s="9" t="n">
+        <v>227.504025764895</v>
+      </c>
+      <c r="C115" s="9" t="n">
+        <v>201.799242424243</v>
+      </c>
+      <c r="D115" s="10" t="n">
+        <v>173.333333333333</v>
+      </c>
+      <c r="E115" s="12" t="n">
+        <f aca="false">AVERAGE(B115:D115)</f>
+        <v>200.878867174157</v>
+      </c>
+      <c r="F115" s="12" t="n">
+        <f aca="false">_xlfn.STDEV.P(B115:D115)</f>
+        <v>22.1246664393605</v>
+      </c>
+      <c r="G115" s="13" t="n">
+        <f aca="false">F115/E115</f>
+        <v>0.110139342931374</v>
+      </c>
+    </row>
+    <row r="116" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A116" s="12" t="s">
+        <v>121</v>
+      </c>
+      <c r="B116" s="9" t="n">
+        <v>191.111111111111</v>
+      </c>
+      <c r="C116" s="9" t="n">
+        <v>159.444444444444</v>
+      </c>
+      <c r="D116" s="10" t="n">
+        <v>158.148148148148</v>
+      </c>
+      <c r="E116" s="12" t="n">
+        <f aca="false">AVERAGE(B116:D116)</f>
+        <v>169.567901234568</v>
+      </c>
+      <c r="F116" s="12" t="n">
+        <f aca="false">_xlfn.STDEV.P(B116:D116)</f>
+        <v>15.2425394835318</v>
+      </c>
+      <c r="G116" s="13" t="n">
+        <f aca="false">F116/E116</f>
+        <v>0.0898904767503514</v>
+      </c>
+    </row>
+    <row r="117" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A117" s="12" t="s">
+        <v>110</v>
+      </c>
+      <c r="B117" s="9" t="n">
+        <v>190.03421900161</v>
+      </c>
+      <c r="C117" s="9" t="n">
+        <v>159.351851851852</v>
+      </c>
+      <c r="D117" s="10" t="n">
+        <v>143.888888888889</v>
+      </c>
+      <c r="E117" s="12" t="n">
+        <f aca="false">AVERAGE(B117:D117)</f>
+        <v>164.424986580784</v>
+      </c>
+      <c r="F117" s="12" t="n">
+        <f aca="false">_xlfn.STDEV.P(B117:D117)</f>
+        <v>19.1772503205653</v>
+      </c>
+      <c r="G117" s="13" t="n">
+        <f aca="false">F117/E117</f>
+        <v>0.116632214600445</v>
+      </c>
+    </row>
+    <row r="118" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A118" s="12" t="s">
+        <v>122</v>
+      </c>
+      <c r="B118" s="9" t="n">
+        <v>192.962962962963</v>
+      </c>
+      <c r="C118" s="9" t="n">
+        <v>151.944444444444</v>
+      </c>
+      <c r="D118" s="10" t="n">
+        <v>145.092592592593</v>
+      </c>
+      <c r="E118" s="12" t="n">
+        <f aca="false">AVERAGE(B118:D118)</f>
+        <v>163.333333333333</v>
+      </c>
+      <c r="F118" s="12" t="n">
+        <f aca="false">_xlfn.STDEV.P(B118:D118)</f>
+        <v>21.13722123714</v>
+      </c>
+      <c r="G118" s="13" t="n">
+        <f aca="false">F118/E118</f>
+        <v>0.129411558594734</v>
+      </c>
+    </row>
+    <row r="119" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A119" s="12" t="s">
+        <v>123</v>
+      </c>
+      <c r="B119" s="9" t="n">
+        <v>171.542553191489</v>
+      </c>
+      <c r="C119" s="9" t="n">
+        <v>152.264492753623</v>
+      </c>
+      <c r="D119" s="10" t="n">
+        <v>130.878045020043</v>
+      </c>
+      <c r="E119" s="12" t="n">
+        <f aca="false">AVERAGE(B119:D119)</f>
+        <v>151.561696988385</v>
+      </c>
+      <c r="F119" s="12" t="n">
+        <f aca="false">_xlfn.STDEV.P(B119:D119)</f>
+        <v>16.6086523158288</v>
+      </c>
+      <c r="G119" s="13" t="n">
+        <f aca="false">F119/E119</f>
+        <v>0.109583441237806</v>
+      </c>
+    </row>
+    <row r="120" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A120" s="8" t="s">
+        <v>124</v>
+      </c>
+      <c r="B120" s="9" t="n">
+        <v>15.3050420271285</v>
+      </c>
+      <c r="C120" s="9" t="n">
+        <v>15.1781787182302</v>
+      </c>
+      <c r="D120" s="10" t="n">
+        <v>14.144547979728</v>
+      </c>
+      <c r="E120" s="8" t="n">
+        <f aca="false">AVERAGE(B120:D120)</f>
+        <v>14.8759229083622</v>
+      </c>
+      <c r="F120" s="8" t="n">
+        <f aca="false">_xlfn.STDEV.P(B120:D120)</f>
+        <v>0.519747079172311</v>
+      </c>
+      <c r="G120" s="11" t="n">
+        <f aca="false">F120/E120</f>
+        <v>0.0349388123596786</v>
+      </c>
+    </row>
+    <row r="121" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A121" s="12" t="s">
+        <v>125</v>
+      </c>
+      <c r="B121" s="9" t="n">
+        <v>172.010869565217</v>
+      </c>
+      <c r="C121" s="9" t="n">
+        <v>153.148148148148</v>
+      </c>
+      <c r="D121" s="10" t="n">
+        <v>122.777777777778</v>
+      </c>
+      <c r="E121" s="12" t="n">
+        <f aca="false">AVERAGE(B121:D121)</f>
+        <v>149.312265163714</v>
+      </c>
+      <c r="F121" s="12" t="n">
+        <f aca="false">_xlfn.STDEV.P(B121:D121)</f>
+        <v>20.2815158940403</v>
+      </c>
+      <c r="G121" s="13" t="n">
+        <f aca="false">F121/E121</f>
+        <v>0.135832886011089</v>
+      </c>
+    </row>
+    <row r="122" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A122" s="12" t="s">
+        <v>126</v>
+      </c>
+      <c r="B122" s="9" t="n">
+        <v>168.840579710145</v>
+      </c>
+      <c r="C122" s="9" t="n">
+        <v>133.695652173913</v>
+      </c>
+      <c r="D122" s="10" t="n">
+        <v>120.386473429952</v>
+      </c>
+      <c r="E122" s="12" t="n">
+        <f aca="false">AVERAGE(B122:D122)</f>
+        <v>140.97423510467</v>
+      </c>
+      <c r="F122" s="12" t="n">
+        <f aca="false">_xlfn.STDEV.P(B122:D122)</f>
+        <v>20.4398863493741</v>
+      </c>
+      <c r="G122" s="13" t="n">
+        <f aca="false">F122/E122</f>
+        <v>0.144990227002814</v>
+      </c>
+    </row>
+    <row r="123" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A123" s="12" t="s">
+        <v>127</v>
+      </c>
+      <c r="B123" s="9" t="n">
+        <v>178.623188405797</v>
+      </c>
+      <c r="C123" s="9" t="n">
+        <v>138.586956521739</v>
+      </c>
+      <c r="D123" s="10" t="n">
+        <v>112.210144927536</v>
+      </c>
+      <c r="E123" s="12" t="n">
+        <f aca="false">AVERAGE(B123:D123)</f>
+        <v>143.140096618357</v>
+      </c>
+      <c r="F123" s="12" t="n">
+        <f aca="false">_xlfn.STDEV.P(B123:D123)</f>
+        <v>27.3034967182583</v>
+      </c>
+      <c r="G123" s="13" t="n">
+        <f aca="false">F123/E123</f>
+        <v>0.190746669614562</v>
+      </c>
+    </row>
+    <row r="124" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A124" s="12" t="s">
+        <v>128</v>
+      </c>
+      <c r="B124" s="9" t="n">
+        <v>167.553191489362</v>
+      </c>
+      <c r="C124" s="9" t="n">
+        <v>136.829324699352</v>
+      </c>
+      <c r="D124" s="10" t="n">
+        <v>110.47833795868</v>
+      </c>
+      <c r="E124" s="12" t="n">
+        <f aca="false">AVERAGE(B124:D124)</f>
+        <v>138.286951382465</v>
+      </c>
+      <c r="F124" s="12" t="n">
+        <f aca="false">_xlfn.STDEV.P(B124:D124)</f>
+        <v>23.3234964938461</v>
+      </c>
+      <c r="G124" s="13" t="n">
+        <f aca="false">F124/E124</f>
+        <v>0.168660139374536</v>
+      </c>
+    </row>
+    <row r="125" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A125" s="12" t="s">
+        <v>129</v>
+      </c>
+      <c r="B125" s="9" t="n">
+        <v>169.47463768116</v>
+      </c>
+      <c r="C125" s="9" t="n">
+        <v>139.321658615137</v>
+      </c>
+      <c r="D125" s="10" t="n">
+        <v>118.792517006803</v>
+      </c>
+      <c r="E125" s="12" t="n">
+        <f aca="false">AVERAGE(B125:D125)</f>
+        <v>142.529604434366</v>
+      </c>
+      <c r="F125" s="12" t="n">
+        <f aca="false">_xlfn.STDEV.P(B125:D125)</f>
+        <v>20.8148588961003</v>
+      </c>
+      <c r="G125" s="13" t="n">
+        <f aca="false">F125/E125</f>
+        <v>0.146038845604777</v>
+      </c>
+    </row>
+    <row r="126" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A126" s="12" t="s">
+        <v>130</v>
+      </c>
+      <c r="B126" s="9" t="n">
+        <v>194.235104669887</v>
+      </c>
+      <c r="C126" s="9" t="n">
+        <v>154.166666666667</v>
+      </c>
+      <c r="D126" s="10" t="n">
+        <v>156.944444444444</v>
+      </c>
+      <c r="E126" s="12" t="n">
+        <f aca="false">AVERAGE(B126:D126)</f>
+        <v>168.448738593666</v>
+      </c>
+      <c r="F126" s="12" t="n">
+        <f aca="false">_xlfn.STDEV.P(B126:D126)</f>
+        <v>18.2689448501795</v>
+      </c>
+      <c r="G126" s="13" t="n">
+        <f aca="false">F126/E126</f>
+        <v>0.108454031788555</v>
+      </c>
+    </row>
+    <row r="127" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A127" s="12" t="s">
+        <v>131</v>
+      </c>
+      <c r="B127" s="9" t="n">
+        <v>249.192834138486</v>
+      </c>
+      <c r="C127" s="9" t="n">
+        <v>222.916666666667</v>
+      </c>
+      <c r="D127" s="10" t="n">
+        <v>196.111111111111</v>
+      </c>
+      <c r="E127" s="12" t="n">
+        <f aca="false">AVERAGE(B127:D127)</f>
+        <v>222.740203972088</v>
+      </c>
+      <c r="F127" s="12" t="n">
+        <f aca="false">_xlfn.STDEV.P(B127:D127)</f>
+        <v>21.6708819109986</v>
+      </c>
+      <c r="G127" s="13" t="n">
+        <f aca="false">F127/E127</f>
+        <v>0.0972921884982842</v>
+      </c>
+    </row>
+    <row r="128" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A128" s="12" t="s">
+        <v>132</v>
+      </c>
+      <c r="B128" s="9" t="n">
+        <v>209.555152979066</v>
+      </c>
+      <c r="C128" s="9" t="n">
+        <v>160.740740740741</v>
+      </c>
+      <c r="D128" s="10" t="n">
+        <v>163.703703703704</v>
+      </c>
+      <c r="E128" s="12" t="n">
+        <f aca="false">AVERAGE(B128:D128)</f>
+        <v>177.999865807837</v>
+      </c>
+      <c r="F128" s="12" t="n">
+        <f aca="false">_xlfn.STDEV.P(B128:D128)</f>
+        <v>22.3457214208004</v>
+      </c>
+      <c r="G128" s="13" t="n">
+        <f aca="false">F128/E128</f>
+        <v>0.125537855432566</v>
+      </c>
+    </row>
+    <row r="129" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A129" s="12" t="s">
+        <v>133</v>
+      </c>
+      <c r="B129" s="9" t="n">
+        <v>189.907407407407</v>
+      </c>
+      <c r="C129" s="9" t="n">
+        <v>160.925925925926</v>
+      </c>
+      <c r="D129" s="10" t="n">
+        <v>147.407407407407</v>
+      </c>
+      <c r="E129" s="12" t="n">
+        <f aca="false">AVERAGE(B129:D129)</f>
+        <v>166.08024691358</v>
+      </c>
+      <c r="F129" s="12" t="n">
+        <f aca="false">_xlfn.STDEV.P(B129:D129)</f>
+        <v>17.7292182311728</v>
+      </c>
+      <c r="G129" s="13" t="n">
+        <f aca="false">F129/E129</f>
+        <v>0.106750914456421</v>
+      </c>
+    </row>
+    <row r="130" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A130" s="8" t="s">
+        <v>134</v>
+      </c>
+      <c r="B130" s="9" t="n">
+        <v>18.044331488043</v>
+      </c>
+      <c r="C130" s="9" t="n">
+        <v>17.0265791186689</v>
+      </c>
+      <c r="D130" s="10" t="n">
+        <v>18.735215130452</v>
+      </c>
+      <c r="E130" s="8" t="n">
+        <f aca="false">AVERAGE(B130:D130)</f>
+        <v>17.9353752457213</v>
+      </c>
+      <c r="F130" s="8" t="n">
+        <f aca="false">_xlfn.STDEV.P(B130:D130)</f>
+        <v>0.701789546918529</v>
+      </c>
+      <c r="G130" s="11" t="n">
+        <f aca="false">F130/E130</f>
+        <v>0.0391287908562687</v>
+      </c>
+    </row>
+    <row r="131" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A131" s="12" t="s">
+        <v>135</v>
+      </c>
+      <c r="B131" s="9" t="n">
+        <v>174.537037037037</v>
+      </c>
+      <c r="C131" s="9" t="n">
+        <v>140.740740740741</v>
+      </c>
+      <c r="D131" s="10" t="n">
+        <v>137.777777777778</v>
+      </c>
+      <c r="E131" s="12" t="n">
+        <f aca="false">AVERAGE(B131:D131)</f>
+        <v>151.018518518519</v>
+      </c>
+      <c r="F131" s="12" t="n">
+        <f aca="false">_xlfn.STDEV.P(B131:D131)</f>
+        <v>16.674038150358</v>
+      </c>
+      <c r="G131" s="13" t="n">
+        <f aca="false">F131/E131</f>
+        <v>0.110410553049581</v>
+      </c>
+    </row>
+    <row r="132" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A132" s="12" t="s">
+        <v>136</v>
+      </c>
+      <c r="B132" s="9" t="n">
+        <v>173.550724637681</v>
+      </c>
+      <c r="C132" s="9" t="n">
+        <v>151.018518518519</v>
+      </c>
+      <c r="D132" s="10" t="n">
+        <v>138.287037037037</v>
+      </c>
+      <c r="E132" s="12" t="n">
+        <f aca="false">AVERAGE(B132:D132)</f>
+        <v>154.285426731079</v>
+      </c>
+      <c r="F132" s="12" t="n">
+        <f aca="false">_xlfn.STDEV.P(B132:D132)</f>
+        <v>14.580499139854</v>
+      </c>
+      <c r="G132" s="13" t="n">
+        <f aca="false">F132/E132</f>
+        <v>0.0945034112992927</v>
+      </c>
+    </row>
+    <row r="133" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A133" s="8" t="s">
+        <v>137</v>
+      </c>
+      <c r="B133" s="9" t="n">
+        <v>14.9164941326236</v>
+      </c>
+      <c r="C133" s="9" t="n">
+        <v>8.89181354486749</v>
+      </c>
+      <c r="D133" s="10" t="n">
+        <v>12.4872525408</v>
+      </c>
+      <c r="E133" s="8" t="n">
+        <f aca="false">AVERAGE(B133:D133)</f>
+        <v>12.0985200727637</v>
+      </c>
+      <c r="F133" s="8" t="n">
+        <f aca="false">_xlfn.STDEV.P(B133:D133)</f>
+        <v>2.47487760571449</v>
+      </c>
+      <c r="G133" s="11" t="n">
+        <f aca="false">F133/E133</f>
+        <v>0.204560358690973</v>
+      </c>
+    </row>
+    <row r="134" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A134" s="8" t="s">
+        <v>138</v>
+      </c>
+      <c r="B134" s="9" t="n">
+        <v>24.0835858516652</v>
+      </c>
+      <c r="C134" s="9" t="n">
+        <v>25.3853071985561</v>
+      </c>
+      <c r="D134" s="10" t="n">
+        <v>25.3105258738766</v>
+      </c>
+      <c r="E134" s="8" t="n">
+        <f aca="false">AVERAGE(B134:D134)</f>
+        <v>24.9264729746993</v>
+      </c>
+      <c r="F134" s="8" t="n">
+        <f aca="false">_xlfn.STDEV.P(B134:D134)</f>
+        <v>0.596792587232054</v>
+      </c>
+      <c r="G134" s="11" t="n">
+        <f aca="false">F134/E134</f>
+        <v>0.0239421192014533</v>
+      </c>
+    </row>
+    <row r="135" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A135" s="8" t="s">
+        <v>139</v>
+      </c>
+      <c r="B135" s="9" t="n">
+        <v>10.8854188327726</v>
+      </c>
+      <c r="C135" s="9" t="n">
+        <v>13.2089406514928</v>
+      </c>
+      <c r="D135" s="10" t="n">
+        <v>11.197136856498</v>
+      </c>
+      <c r="E135" s="8" t="n">
+        <f aca="false">AVERAGE(B135:D135)</f>
+        <v>11.7638321135878</v>
+      </c>
+      <c r="F135" s="8" t="n">
+        <f aca="false">_xlfn.STDEV.P(B135:D135)</f>
+        <v>1.02973978794751</v>
+      </c>
+      <c r="G135" s="11" t="n">
+        <f aca="false">F135/E135</f>
+        <v>0.0875343831843801</v>
+      </c>
+    </row>
+    <row r="136" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A136" s="8" t="s">
+        <v>140</v>
+      </c>
+      <c r="B136" s="9" t="n">
+        <v>8.27260318092898</v>
+      </c>
+      <c r="C136" s="9" t="n">
+        <v>0.834117077063385</v>
+      </c>
+      <c r="D136" s="10" t="n">
+        <v>9.60264875798</v>
+      </c>
+      <c r="E136" s="8" t="n">
+        <f aca="false">AVERAGE(B136:D136)</f>
+        <v>6.23645633865746</v>
+      </c>
+      <c r="F136" s="8" t="n">
+        <f aca="false">_xlfn.STDEV.P(B136:D136)</f>
+        <v>3.85842864667979</v>
+      </c>
+      <c r="G136" s="11" t="n">
+        <f aca="false">F136/E136</f>
+        <v>0.618689274350056</v>
+      </c>
+    </row>
+    <row r="137" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A137" s="8" t="s">
+        <v>141</v>
+      </c>
+      <c r="B137" s="9" t="n">
+        <v>9.86264050430498</v>
+      </c>
+      <c r="C137" s="9" t="n">
+        <v>1.94857690631655</v>
+      </c>
+      <c r="D137" s="10" t="n">
+        <v>4.76068633150205</v>
+      </c>
+      <c r="E137" s="8" t="n">
+        <f aca="false">AVERAGE(B137:D137)</f>
+        <v>5.52396791404119</v>
+      </c>
+      <c r="F137" s="8" t="n">
+        <f aca="false">_xlfn.STDEV.P(B137:D137)</f>
+        <v>3.27567293228267</v>
+      </c>
+      <c r="G137" s="11" t="n">
+        <f aca="false">F137/E137</f>
+        <v>0.592992751452509</v>
+      </c>
+    </row>
+    <row r="138" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A138" s="8" t="s">
+        <v>142</v>
+      </c>
+      <c r="B138" s="9" t="n">
+        <v>42.8349148118676</v>
+      </c>
+      <c r="C138" s="9" t="n">
+        <v>41.7999903566233</v>
+      </c>
+      <c r="D138" s="10" t="n">
+        <v>42.5845583824447</v>
+      </c>
+      <c r="E138" s="8" t="n">
+        <f aca="false">AVERAGE(B138:D138)</f>
+        <v>42.4064878503119</v>
+      </c>
+      <c r="F138" s="8" t="n">
+        <f aca="false">_xlfn.STDEV.P(B138:D138)</f>
+        <v>0.440869589808013</v>
+      </c>
+      <c r="G138" s="11" t="n">
+        <f aca="false">F138/E138</f>
+        <v>0.0103962768943331</v>
+      </c>
+    </row>
+    <row r="139" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A139" s="8" t="s">
+        <v>143</v>
+      </c>
+      <c r="B139" s="9" t="n">
+        <v>54.7822423725505</v>
+      </c>
+      <c r="C139" s="9" t="n">
+        <v>48.4891845104465</v>
+      </c>
+      <c r="D139" s="10" t="n">
+        <v>61.2841869794251</v>
+      </c>
+      <c r="E139" s="8" t="n">
+        <f aca="false">AVERAGE(B139:D139)</f>
+        <v>54.851871287474</v>
+      </c>
+      <c r="F139" s="8" t="n">
+        <f aca="false">_xlfn.STDEV.P(B139:D139)</f>
+        <v>5.22376991483078</v>
+      </c>
+      <c r="G139" s="11" t="n">
+        <f aca="false">F139/E139</f>
+        <v>0.0952341240548284</v>
+      </c>
+    </row>
+    <row r="140" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A140" s="12" t="s">
+        <v>144</v>
+      </c>
+      <c r="B140" s="9" t="n">
+        <v>193.611111111111</v>
+      </c>
+      <c r="C140" s="9" t="n">
+        <v>154.166666666667</v>
+      </c>
+      <c r="D140" s="10" t="n">
+        <v>157.183977455717</v>
+      </c>
+      <c r="E140" s="12" t="n">
+        <f aca="false">AVERAGE(B140:D140)</f>
+        <v>168.320585077831</v>
+      </c>
+      <c r="F140" s="12" t="n">
+        <f aca="false">_xlfn.STDEV.P(B140:D140)</f>
+        <v>17.9254766813312</v>
+      </c>
+      <c r="G140" s="13" t="n">
+        <f aca="false">F140/E140</f>
+        <v>0.106496045466112</v>
+      </c>
+    </row>
+    <row r="141" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A141" s="8" t="s">
+        <v>145</v>
+      </c>
+      <c r="B141" s="9" t="n">
+        <v>7.28629193057134</v>
+      </c>
+      <c r="C141" s="9" t="n">
+        <v>4.83759318322454</v>
+      </c>
+      <c r="D141" s="10" t="n">
+        <v>12.77858509808</v>
+      </c>
+      <c r="E141" s="8" t="n">
+        <f aca="false">AVERAGE(B141:D141)</f>
+        <v>8.30082340395864</v>
+      </c>
+      <c r="F141" s="8" t="n">
+        <f aca="false">_xlfn.STDEV.P(B141:D141)</f>
+        <v>3.32032064022138</v>
+      </c>
+      <c r="G141" s="11" t="n">
+        <f aca="false">F141/E141</f>
+        <v>0.399998949337716</v>
+      </c>
+    </row>
+    <row r="142" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A142" s="8" t="s">
+        <v>146</v>
+      </c>
+      <c r="B142" s="9" t="n">
+        <v>9.86048003547952</v>
+      </c>
+      <c r="C142" s="9" t="n">
+        <v>10.2861953478096</v>
+      </c>
+      <c r="D142" s="10" t="n">
+        <v>6.13023890638036</v>
+      </c>
+      <c r="E142" s="8" t="n">
+        <f aca="false">AVERAGE(B142:D142)</f>
+        <v>8.75897142988982</v>
+      </c>
+      <c r="F142" s="8" t="n">
+        <f aca="false">_xlfn.STDEV.P(B142:D142)</f>
+        <v>1.86690195991565</v>
+      </c>
+      <c r="G142" s="11" t="n">
+        <f aca="false">F142/E142</f>
+        <v>0.213141688480098</v>
+      </c>
+    </row>
+    <row r="143" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A143" s="8" t="s">
+        <v>147</v>
+      </c>
+      <c r="B143" s="9" t="n">
+        <v>6.67368871010621</v>
+      </c>
+      <c r="C143" s="9" t="n">
+        <v>6.67782213641337</v>
+      </c>
+      <c r="D143" s="10" t="n">
+        <v>3.98723873915508</v>
+      </c>
+      <c r="E143" s="8" t="n">
+        <f aca="false">AVERAGE(B143:D143)</f>
+        <v>5.77958319522489</v>
+      </c>
+      <c r="F143" s="8" t="n">
+        <f aca="false">_xlfn.STDEV.P(B143:D143)</f>
+        <v>1.26738004250406</v>
+      </c>
+      <c r="G143" s="11" t="n">
+        <f aca="false">F143/E143</f>
+        <v>0.219285716580942</v>
+      </c>
+    </row>
+    <row r="144" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A144" s="8" t="s">
+        <v>148</v>
+      </c>
+      <c r="B144" s="9" t="n">
+        <v>8.10189629380619</v>
+      </c>
+      <c r="C144" s="9" t="n">
+        <v>5.19470528011957</v>
+      </c>
+      <c r="D144" s="10" t="n">
+        <v>6.08393613684449</v>
+      </c>
+      <c r="E144" s="8" t="n">
+        <f aca="false">AVERAGE(B144:D144)</f>
+        <v>6.46017923692341</v>
+      </c>
+      <c r="F144" s="8" t="n">
+        <f aca="false">_xlfn.STDEV.P(B144:D144)</f>
+        <v>1.21630836284302</v>
+      </c>
+      <c r="G144" s="11" t="n">
+        <f aca="false">F144/E144</f>
+        <v>0.188277804413098</v>
+      </c>
+    </row>
+    <row r="145" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A145" s="8" t="s">
+        <v>149</v>
+      </c>
+      <c r="B145" s="9" t="n">
+        <v>7.83784345138453</v>
+      </c>
+      <c r="C145" s="9" t="n">
+        <v>12.2247966927098</v>
+      </c>
+      <c r="D145" s="10" t="n">
+        <v>4.97683930015598</v>
+      </c>
+      <c r="E145" s="8" t="n">
+        <f aca="false">AVERAGE(B145:D145)</f>
+        <v>8.34649314808343</v>
+      </c>
+      <c r="F145" s="8" t="n">
+        <f aca="false">_xlfn.STDEV.P(B145:D145)</f>
+        <v>2.9807454298696</v>
+      </c>
+      <c r="G145" s="11" t="n">
+        <f aca="false">F145/E145</f>
+        <v>0.357125486954249</v>
+      </c>
+    </row>
+    <row r="146" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A146" s="8" t="s">
+        <v>150</v>
+      </c>
+      <c r="B146" s="9" t="n">
+        <v>8.73626603160058</v>
+      </c>
+      <c r="C146" s="9" t="n">
+        <v>1.88665949583112</v>
+      </c>
+      <c r="D146" s="10" t="n">
+        <v>6.35310692819812</v>
+      </c>
+      <c r="E146" s="8" t="n">
+        <f aca="false">AVERAGE(B146:D146)</f>
+        <v>5.65867748520994</v>
+      </c>
+      <c r="F146" s="8" t="n">
+        <f aca="false">_xlfn.STDEV.P(B146:D146)</f>
+        <v>2.83912564148197</v>
+      </c>
+      <c r="G146" s="11" t="n">
+        <f aca="false">F146/E146</f>
+        <v>0.501729538200857</v>
+      </c>
+    </row>
+    <row r="147" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A147" s="8" t="s">
+        <v>151</v>
+      </c>
+      <c r="B147" s="9" t="n">
+        <v>7.41234211029952</v>
+      </c>
+      <c r="C147" s="9" t="n">
+        <v>6.2807530913698</v>
+      </c>
+      <c r="D147" s="10" t="n">
+        <v>5.58923273028524</v>
+      </c>
+      <c r="E147" s="8" t="n">
+        <f aca="false">AVERAGE(B147:D147)</f>
+        <v>6.42744264398485</v>
+      </c>
+      <c r="F147" s="8" t="n">
+        <f aca="false">_xlfn.STDEV.P(B147:D147)</f>
+        <v>0.751474249507287</v>
+      </c>
+      <c r="G147" s="11" t="n">
+        <f aca="false">F147/E147</f>
+        <v>0.11691652358976</v>
+      </c>
+    </row>
+    <row r="148" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A148" s="8" t="s">
+        <v>152</v>
+      </c>
+      <c r="B148" s="9" t="n">
+        <v>32.9300161271777</v>
+      </c>
+      <c r="C148" s="9" t="n">
+        <v>34.424820758338</v>
+      </c>
+      <c r="D148" s="10" t="n">
+        <v>30.8856296674051</v>
+      </c>
+      <c r="E148" s="8" t="n">
+        <f aca="false">AVERAGE(B148:D148)</f>
+        <v>32.7468221843069</v>
+      </c>
+      <c r="F148" s="8" t="n">
+        <f aca="false">_xlfn.STDEV.P(B148:D148)</f>
+        <v>1.45066385034881</v>
+      </c>
+      <c r="G148" s="11" t="n">
+        <f aca="false">F148/E148</f>
+        <v>0.0442993778811307</v>
+      </c>
+    </row>
+    <row r="149" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A149" s="8" t="s">
+        <v>153</v>
+      </c>
+      <c r="B149" s="9" t="n">
+        <v>23.9431494963436</v>
+      </c>
+      <c r="C149" s="9" t="n">
+        <v>27.1253594218736</v>
+      </c>
+      <c r="D149" s="10" t="n">
+        <v>24.981477248295</v>
+      </c>
+      <c r="E149" s="8" t="n">
+        <f aca="false">AVERAGE(B149:D149)</f>
+        <v>25.3499953888374</v>
+      </c>
+      <c r="F149" s="8" t="n">
+        <f aca="false">_xlfn.STDEV.P(B149:D149)</f>
+        <v>1.32500797921297</v>
+      </c>
+      <c r="G149" s="11" t="n">
+        <f aca="false">F149/E149</f>
+        <v>0.0522685688454375</v>
+      </c>
+    </row>
+    <row r="150" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A150" s="8" t="s">
+        <v>154</v>
+      </c>
+      <c r="B150" s="9" t="n">
+        <v>20.2240523232664</v>
+      </c>
+      <c r="C150" s="9" t="n">
+        <v>16.7204648334039</v>
+      </c>
+      <c r="D150" s="10" t="n">
+        <v>17.4796042110412</v>
+      </c>
+      <c r="E150" s="8" t="n">
+        <f aca="false">AVERAGE(B150:D150)</f>
+        <v>18.1413737892372</v>
+      </c>
+      <c r="F150" s="8" t="n">
+        <f aca="false">_xlfn.STDEV.P(B150:D150)</f>
+        <v>1.50493312271113</v>
+      </c>
+      <c r="G150" s="11" t="n">
+        <f aca="false">F150/E150</f>
+        <v>0.0829558521970351</v>
+      </c>
+    </row>
+    <row r="151" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A151" s="8" t="s">
+        <v>155</v>
+      </c>
+      <c r="B151" s="9" t="n">
+        <v>23.9251196466903</v>
+      </c>
+      <c r="C151" s="9" t="n">
+        <v>26.1303711487192</v>
+      </c>
+      <c r="D151" s="10" t="n">
+        <v>21.5507488750554</v>
+      </c>
+      <c r="E151" s="8" t="n">
+        <f aca="false">AVERAGE(B151:D151)</f>
+        <v>23.8687465568216</v>
+      </c>
+      <c r="F151" s="8" t="n">
+        <f aca="false">_xlfn.STDEV.P(B151:D151)</f>
+        <v>1.87004785790906</v>
+      </c>
+      <c r="G151" s="11" t="n">
+        <f aca="false">F151/E151</f>
+        <v>0.0783471328692209</v>
+      </c>
+    </row>
+    <row r="152" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A152" s="8" t="s">
+        <v>156</v>
+      </c>
+      <c r="B152" s="9" t="n">
+        <v>18.5687819778795</v>
+      </c>
+      <c r="C152" s="9" t="n">
+        <v>16.7802787477398</v>
+      </c>
+      <c r="D152" s="10" t="n">
+        <v>16.6837770608205</v>
+      </c>
+      <c r="E152" s="8" t="n">
+        <f aca="false">AVERAGE(B152:D152)</f>
+        <v>17.3442792621466</v>
+      </c>
+      <c r="F152" s="8" t="n">
+        <f aca="false">_xlfn.STDEV.P(B152:D152)</f>
+        <v>0.866749990682626</v>
+      </c>
+      <c r="G152" s="11" t="n">
+        <f aca="false">F152/E152</f>
+        <v>0.0499732492531001</v>
+      </c>
+    </row>
+    <row r="153" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A153" s="8" t="s">
+        <v>157</v>
+      </c>
+      <c r="B153" s="9" t="n">
+        <v>32.5627470976544</v>
+      </c>
+      <c r="C153" s="9" t="n">
+        <v>32.4810464297102</v>
+      </c>
+      <c r="D153" s="10" t="n">
+        <v>37.2604972092554</v>
+      </c>
+      <c r="E153" s="8" t="n">
+        <f aca="false">AVERAGE(B153:D153)</f>
+        <v>34.10143024554</v>
+      </c>
+      <c r="F153" s="8" t="n">
+        <f aca="false">_xlfn.STDEV.P(B153:D153)</f>
+        <v>2.2340466737461</v>
+      </c>
+      <c r="G153" s="11" t="n">
+        <f aca="false">F153/E153</f>
+        <v>0.0655118174710072</v>
+      </c>
+    </row>
+    <row r="154" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A154" s="12" t="s">
+        <v>158</v>
+      </c>
+      <c r="B154" s="9" t="n">
+        <v>174.45652173913</v>
+      </c>
+      <c r="C154" s="9" t="n">
+        <v>149.275362318841</v>
+      </c>
+      <c r="D154" s="10" t="n">
+        <v>137.952898550725</v>
+      </c>
+      <c r="E154" s="12" t="n">
+        <f aca="false">AVERAGE(B154:D154)</f>
+        <v>153.894927536232</v>
+      </c>
+      <c r="F154" s="12" t="n">
+        <f aca="false">_xlfn.STDEV.P(B154:D154)</f>
+        <v>15.2563410547567</v>
+      </c>
+      <c r="G154" s="13" t="n">
+        <f aca="false">F154/E154</f>
+        <v>0.0991347882545695</v>
+      </c>
+    </row>
+    <row r="155" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A155" s="8" t="s">
+        <v>159</v>
+      </c>
+      <c r="B155" s="9" t="n">
+        <v>6.86813760989834</v>
+      </c>
+      <c r="C155" s="9" t="n">
+        <v>13.8944626465417</v>
+      </c>
+      <c r="D155" s="10" t="n">
+        <v>8.54527902962364</v>
+      </c>
+      <c r="E155" s="8" t="n">
+        <f aca="false">AVERAGE(B155:D155)</f>
+        <v>9.76929309535455</v>
+      </c>
+      <c r="F155" s="8" t="n">
+        <f aca="false">_xlfn.STDEV.P(B155:D155)</f>
+        <v>2.99621635900687</v>
+      </c>
+      <c r="G155" s="11" t="n">
+        <f aca="false">F155/E155</f>
+        <v>0.306697355659399</v>
+      </c>
+    </row>
+    <row r="156" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A156" s="8" t="s">
+        <v>160</v>
+      </c>
+      <c r="B156" s="9" t="n">
+        <v>18.5268315647832</v>
+      </c>
+      <c r="C156" s="9" t="n">
+        <v>19.1986789166099</v>
+      </c>
+      <c r="D156" s="10" t="n">
+        <v>17.9379767978045</v>
+      </c>
+      <c r="E156" s="8" t="n">
+        <f aca="false">AVERAGE(B156:D156)</f>
+        <v>18.5544957597325</v>
+      </c>
+      <c r="F156" s="8" t="n">
+        <f aca="false">_xlfn.STDEV.P(B156:D156)</f>
+        <v>0.515051090573711</v>
+      </c>
+      <c r="G156" s="11" t="n">
+        <f aca="false">F156/E156</f>
+        <v>0.0277588298406626</v>
+      </c>
+    </row>
+    <row r="157" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A157" s="8" t="s">
+        <v>161</v>
+      </c>
+      <c r="B157" s="9" t="n">
+        <v>9.09643143326738</v>
+      </c>
+      <c r="C157" s="9" t="n">
+        <v>6.00492778887895</v>
+      </c>
+      <c r="D157" s="10" t="n">
+        <v>11.3024145426557</v>
+      </c>
+      <c r="E157" s="8" t="n">
+        <f aca="false">AVERAGE(B157:D157)</f>
+        <v>8.80125792160069</v>
+      </c>
+      <c r="F157" s="8" t="n">
+        <f aca="false">_xlfn.STDEV.P(B157:D157)</f>
+        <v>2.17273821526392</v>
+      </c>
+      <c r="G157" s="11" t="n">
+        <f aca="false">F157/E157</f>
+        <v>0.246866781387173</v>
+      </c>
+    </row>
+    <row r="158" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A158" s="8" t="s">
+        <v>162</v>
+      </c>
+      <c r="B158" s="9" t="n">
+        <v>29.5972903261458</v>
+      </c>
+      <c r="C158" s="9" t="n">
+        <v>33.5815359776345</v>
+      </c>
+      <c r="D158" s="10" t="n">
+        <v>29.4813369264482</v>
+      </c>
+      <c r="E158" s="8" t="n">
+        <f aca="false">AVERAGE(B158:D158)</f>
+        <v>30.8867210767428</v>
+      </c>
+      <c r="F158" s="8" t="n">
+        <f aca="false">_xlfn.STDEV.P(B158:D158)</f>
+        <v>1.90610979226909</v>
+      </c>
+      <c r="G158" s="11" t="n">
+        <f aca="false">F158/E158</f>
+        <v>0.0617129214698143</v>
+      </c>
+    </row>
+    <row r="159" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A159" s="8" t="s">
+        <v>163</v>
+      </c>
+      <c r="B159" s="9" t="n">
+        <v>9.28670125139555</v>
+      </c>
+      <c r="C159" s="9" t="n">
+        <v>13.9690834720088</v>
+      </c>
+      <c r="D159" s="10" t="n">
+        <v>12.3462986423805</v>
+      </c>
+      <c r="E159" s="8" t="n">
+        <f aca="false">AVERAGE(B159:D159)</f>
+        <v>11.8673611219283</v>
+      </c>
+      <c r="F159" s="8" t="n">
+        <f aca="false">_xlfn.STDEV.P(B159:D159)</f>
+        <v>1.94134174843952</v>
+      </c>
+      <c r="G159" s="11" t="n">
+        <f aca="false">F159/E159</f>
+        <v>0.163586641418736</v>
+      </c>
+    </row>
+    <row r="160" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A160" s="8" t="s">
+        <v>164</v>
+      </c>
+      <c r="B160" s="9" t="n">
+        <v>37.4155454051136</v>
+      </c>
+      <c r="C160" s="9" t="n">
+        <v>38.8768861282253</v>
+      </c>
+      <c r="D160" s="10" t="n">
+        <v>30.7437581131955</v>
+      </c>
+      <c r="E160" s="8" t="n">
+        <f aca="false">AVERAGE(B160:D160)</f>
+        <v>35.6787298821781</v>
+      </c>
+      <c r="F160" s="8" t="n">
+        <f aca="false">_xlfn.STDEV.P(B160:D160)</f>
+        <v>3.54018257040963</v>
+      </c>
+      <c r="G160" s="11" t="n">
+        <f aca="false">F160/E160</f>
+        <v>0.0992238956403541</v>
+      </c>
+    </row>
+    <row r="161" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A161" s="8" t="s">
+        <v>165</v>
+      </c>
+      <c r="B161" s="9" t="n">
+        <v>18.5268502180949</v>
+      </c>
+      <c r="C161" s="9" t="n">
+        <v>18.4269706128353</v>
+      </c>
+      <c r="D161" s="10" t="n">
+        <v>15.6213419757535</v>
+      </c>
+      <c r="E161" s="8" t="n">
+        <f aca="false">AVERAGE(B161:D161)</f>
+        <v>17.5250542688945</v>
+      </c>
+      <c r="F161" s="8" t="n">
+        <f aca="false">_xlfn.STDEV.P(B161:D161)</f>
+        <v>1.34674530014129</v>
+      </c>
+      <c r="G161" s="11" t="n">
+        <f aca="false">F161/E161</f>
+        <v>0.0768468547644755</v>
+      </c>
+    </row>
+    <row r="162" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A162" s="8" t="s">
+        <v>166</v>
+      </c>
+      <c r="B162" s="9" t="n">
+        <v>18.3384464652781</v>
+      </c>
+      <c r="C162" s="9" t="n">
+        <v>17.2321660005887</v>
+      </c>
+      <c r="D162" s="10" t="n">
+        <v>16.49139465073</v>
+      </c>
+      <c r="E162" s="8" t="n">
+        <f aca="false">AVERAGE(B162:D162)</f>
+        <v>17.354002372199</v>
+      </c>
+      <c r="F162" s="8" t="n">
+        <f aca="false">_xlfn.STDEV.P(B162:D162)</f>
+        <v>0.758961210028418</v>
+      </c>
+      <c r="G162" s="11" t="n">
+        <f aca="false">F162/E162</f>
+        <v>0.0437340731982538</v>
+      </c>
+    </row>
+    <row r="163" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A163" s="8" t="s">
+        <v>167</v>
+      </c>
+      <c r="B163" s="9" t="n">
+        <v>22.7565229328065</v>
+      </c>
+      <c r="C163" s="9" t="n">
+        <v>22.864821173959</v>
+      </c>
+      <c r="D163" s="10" t="n">
+        <v>22.6831942884134</v>
+      </c>
+      <c r="E163" s="8" t="n">
+        <f aca="false">AVERAGE(B163:D163)</f>
+        <v>22.7681794650596</v>
+      </c>
+      <c r="F163" s="8" t="n">
+        <f aca="false">_xlfn.STDEV.P(B163:D163)</f>
+        <v>0.0746055737255366</v>
+      </c>
+      <c r="G163" s="11" t="n">
+        <f aca="false">F163/E163</f>
+        <v>0.0032767474378014</v>
+      </c>
+    </row>
+    <row r="164" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A164" s="8" t="s">
+        <v>168</v>
+      </c>
+      <c r="B164" s="9" t="n">
+        <v>18.8819155478954</v>
+      </c>
+      <c r="C164" s="9" t="n">
+        <v>17.7616959911274</v>
+      </c>
+      <c r="D164" s="10" t="n">
+        <v>21.011195654297</v>
+      </c>
+      <c r="E164" s="8" t="n">
+        <f aca="false">AVERAGE(B164:D164)</f>
+        <v>19.2182690644399</v>
+      </c>
+      <c r="F164" s="8" t="n">
+        <f aca="false">_xlfn.STDEV.P(B164:D164)</f>
+        <v>1.34775425091857</v>
+      </c>
+      <c r="G164" s="11" t="n">
+        <f aca="false">F164/E164</f>
+        <v>0.0701288053778138</v>
+      </c>
+    </row>
+    <row r="165" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A165" s="12" t="s">
+        <v>169</v>
+      </c>
+      <c r="B165" s="9" t="n">
+        <v>180.107153869874</v>
+      </c>
+      <c r="C165" s="9" t="n">
+        <v>149.63768115942</v>
+      </c>
+      <c r="D165" s="10" t="n">
+        <v>144.655797101449</v>
+      </c>
+      <c r="E165" s="12" t="n">
+        <f aca="false">AVERAGE(B165:D165)</f>
+        <v>158.133544043581</v>
+      </c>
+      <c r="F165" s="12" t="n">
+        <f aca="false">_xlfn.STDEV.P(B165:D165)</f>
+        <v>15.6702358797471</v>
+      </c>
+      <c r="G165" s="13" t="n">
+        <f aca="false">F165/E165</f>
+        <v>0.0990949515140725</v>
+      </c>
+    </row>
+    <row r="166" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A166" s="8" t="s">
+        <v>170</v>
+      </c>
+      <c r="B166" s="9" t="n">
+        <v>15.0450845578124</v>
+      </c>
+      <c r="C166" s="9" t="n">
+        <v>15.0744444288284</v>
+      </c>
+      <c r="D166" s="10" t="n">
+        <v>14.3868384447297</v>
+      </c>
+      <c r="E166" s="8" t="n">
+        <f aca="false">AVERAGE(B166:D166)</f>
+        <v>14.8354558104568</v>
+      </c>
+      <c r="F166" s="8" t="n">
+        <f aca="false">_xlfn.STDEV.P(B166:D166)</f>
+        <v>0.317446747377113</v>
+      </c>
+      <c r="G166" s="11" t="n">
+        <f aca="false">F166/E166</f>
+        <v>0.0213978425356746</v>
+      </c>
+    </row>
+    <row r="167" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A167" s="12" t="s">
+        <v>171</v>
+      </c>
+      <c r="B167" s="9" t="n">
+        <v>174.468085106383</v>
+      </c>
+      <c r="C167" s="9" t="n">
+        <v>160.904255319149</v>
+      </c>
+      <c r="D167" s="10" t="n">
+        <v>159.057971014493</v>
+      </c>
+      <c r="E167" s="12" t="n">
+        <f aca="false">AVERAGE(B167:D167)</f>
+        <v>164.810103813342</v>
+      </c>
+      <c r="F167" s="12" t="n">
+        <f aca="false">_xlfn.STDEV.P(B167:D167)</f>
+        <v>6.87069348396793</v>
+      </c>
+      <c r="G167" s="13" t="n">
+        <f aca="false">F167/E167</f>
+        <v>0.0416885453318411</v>
+      </c>
+    </row>
+    <row r="168" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A168" s="8" t="s">
+        <v>172</v>
+      </c>
+      <c r="B168" s="9" t="n">
+        <v>19.4365957183667</v>
+      </c>
+      <c r="C168" s="9" t="n">
+        <v>21.3222286910409</v>
+      </c>
+      <c r="D168" s="10" t="n">
+        <v>22.4652226552811</v>
+      </c>
+      <c r="E168" s="8" t="n">
+        <f aca="false">AVERAGE(B168:D168)</f>
+        <v>21.0746823548963</v>
+      </c>
+      <c r="F168" s="8" t="n">
+        <f aca="false">_xlfn.STDEV.P(B168:D168)</f>
+        <v>1.24876063149425</v>
+      </c>
+      <c r="G168" s="11" t="n">
+        <f aca="false">F168/E168</f>
+        <v>0.0592540665840272</v>
+      </c>
+    </row>
+    <row r="169" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A169" s="12" t="s">
+        <v>173</v>
+      </c>
+      <c r="B169" s="9" t="n">
+        <v>176.811594202899</v>
+      </c>
+      <c r="C169" s="9" t="n">
+        <v>146.851851851852</v>
+      </c>
+      <c r="D169" s="10" t="n">
+        <v>133.152173913044</v>
+      </c>
+      <c r="E169" s="12" t="n">
+        <f aca="false">AVERAGE(B169:D169)</f>
+        <v>152.271873322598</v>
+      </c>
+      <c r="F169" s="12" t="n">
+        <f aca="false">_xlfn.STDEV.P(B169:D169)</f>
+        <v>18.2312683700113</v>
+      </c>
+      <c r="G169" s="13" t="n">
+        <f aca="false">F169/E169</f>
+        <v>0.119728404019744</v>
+      </c>
+    </row>
+    <row r="170" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A170" s="8" t="s">
+        <v>174</v>
+      </c>
+      <c r="B170" s="9" t="n">
+        <v>31.4829379174821</v>
+      </c>
+      <c r="C170" s="9" t="n">
+        <v>33.1457528144587</v>
+      </c>
+      <c r="D170" s="10" t="n">
+        <v>30.0678983018156</v>
+      </c>
+      <c r="E170" s="8" t="n">
+        <f aca="false">AVERAGE(B170:D170)</f>
+        <v>31.5655296779188</v>
+      </c>
+      <c r="F170" s="8" t="n">
+        <f aca="false">_xlfn.STDEV.P(B170:D170)</f>
+        <v>1.25788530198332</v>
+      </c>
+      <c r="G170" s="11" t="n">
+        <f aca="false">F170/E170</f>
+        <v>0.0398499665558679</v>
+      </c>
+    </row>
+    <row r="171" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A171" s="8" t="s">
+        <v>175</v>
+      </c>
+      <c r="B171" s="9" t="n">
+        <v>15.9205922152832</v>
+      </c>
+      <c r="C171" s="9" t="n">
+        <v>15.4342831612585</v>
+      </c>
+      <c r="D171" s="10" t="n">
+        <v>12.8416001111707</v>
+      </c>
+      <c r="E171" s="8" t="n">
+        <f aca="false">AVERAGE(B171:D171)</f>
+        <v>14.7321584959042</v>
+      </c>
+      <c r="F171" s="8" t="n">
+        <f aca="false">_xlfn.STDEV.P(B171:D171)</f>
+        <v>1.35148865541448</v>
+      </c>
+      <c r="G171" s="11" t="n">
+        <f aca="false">F171/E171</f>
+        <v>0.0917373143786241</v>
+      </c>
+    </row>
+    <row r="172" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A172" s="8" t="s">
+        <v>176</v>
+      </c>
+      <c r="B172" s="9" t="n">
+        <v>30.420189403978</v>
+      </c>
+      <c r="C172" s="9" t="n">
+        <v>26.1399867385722</v>
+      </c>
+      <c r="D172" s="10" t="n">
+        <v>21.9406602177351</v>
+      </c>
+      <c r="E172" s="8" t="n">
+        <f aca="false">AVERAGE(B172:D172)</f>
+        <v>26.1669454534284</v>
+      </c>
+      <c r="F172" s="8" t="n">
+        <f aca="false">_xlfn.STDEV.P(B172:D172)</f>
+        <v>3.46180577967783</v>
+      </c>
+      <c r="G172" s="11" t="n">
+        <f aca="false">F172/E172</f>
+        <v>0.132296900524331</v>
+      </c>
+    </row>
+    <row r="173" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A173" s="8" t="s">
+        <v>177</v>
+      </c>
+      <c r="B173" s="9" t="n">
+        <v>17.4809129025168</v>
+      </c>
+      <c r="C173" s="9" t="n">
+        <v>17.1518160868072</v>
+      </c>
+      <c r="D173" s="10" t="n">
+        <v>15.3244907937877</v>
+      </c>
+      <c r="E173" s="8" t="n">
+        <f aca="false">AVERAGE(B173:D173)</f>
+        <v>16.6524065943706</v>
+      </c>
+      <c r="F173" s="8" t="n">
+        <f aca="false">_xlfn.STDEV.P(B173:D173)</f>
+        <v>0.948541497460123</v>
+      </c>
+      <c r="G173" s="11" t="n">
+        <f aca="false">F173/E173</f>
+        <v>0.05696122611976</v>
+      </c>
+    </row>
+    <row r="174" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A174" s="8" t="s">
+        <v>178</v>
+      </c>
+      <c r="B174" s="9" t="n">
+        <v>46.3297773519986</v>
+      </c>
+      <c r="C174" s="9" t="n">
+        <v>43.3297493473021</v>
+      </c>
+      <c r="D174" s="10" t="n">
+        <v>48.6683443476077</v>
+      </c>
+      <c r="E174" s="8" t="n">
+        <f aca="false">AVERAGE(B174:D174)</f>
+        <v>46.1092903489695</v>
+      </c>
+      <c r="F174" s="8" t="n">
+        <f aca="false">_xlfn.STDEV.P(B174:D174)</f>
+        <v>2.18504157598896</v>
+      </c>
+      <c r="G174" s="11" t="n">
+        <f aca="false">F174/E174</f>
+        <v>0.0473883150109639</v>
+      </c>
+    </row>
+    <row r="175" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A175" s="8" t="s">
+        <v>179</v>
+      </c>
+      <c r="B175" s="9" t="n">
+        <v>25.6212522181895</v>
+      </c>
+      <c r="C175" s="9" t="n">
+        <v>28.1265976688357</v>
+      </c>
+      <c r="D175" s="10" t="n">
+        <v>24.8050732128362</v>
+      </c>
+      <c r="E175" s="8" t="n">
+        <f aca="false">AVERAGE(B175:D175)</f>
+        <v>26.1843076999538</v>
+      </c>
+      <c r="F175" s="8" t="n">
+        <f aca="false">_xlfn.STDEV.P(B175:D175)</f>
+        <v>1.4132479812143</v>
+      </c>
+      <c r="G175" s="11" t="n">
+        <f aca="false">F175/E175</f>
+        <v>0.0539730894323698</v>
+      </c>
+    </row>
+    <row r="176" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A176" s="8" t="s">
+        <v>180</v>
+      </c>
+      <c r="B176" s="9" t="n">
+        <v>20.1315290430884</v>
+      </c>
+      <c r="C176" s="9" t="n">
+        <v>19.3266602237379</v>
+      </c>
+      <c r="D176" s="10" t="n">
+        <v>18.9525089118372</v>
+      </c>
+      <c r="E176" s="8" t="n">
+        <f aca="false">AVERAGE(B176:D176)</f>
+        <v>19.4702327262212</v>
+      </c>
+      <c r="F176" s="8" t="n">
+        <f aca="false">_xlfn.STDEV.P(B176:D176)</f>
+        <v>0.491922700618622</v>
+      </c>
+      <c r="G176" s="11" t="n">
+        <f aca="false">F176/E176</f>
+        <v>0.0252653734311113</v>
+      </c>
+    </row>
+    <row r="177" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A177" s="8" t="s">
+        <v>181</v>
+      </c>
+      <c r="B177" s="9" t="n">
+        <v>19.8671062814573</v>
+      </c>
+      <c r="C177" s="9" t="n">
+        <v>17.0430149215157</v>
+      </c>
+      <c r="D177" s="10" t="n">
+        <v>18.9982721409592</v>
+      </c>
+      <c r="E177" s="8" t="n">
+        <f aca="false">AVERAGE(B177:D177)</f>
+        <v>18.6361311146441</v>
+      </c>
+      <c r="F177" s="8" t="n">
+        <f aca="false">_xlfn.STDEV.P(B177:D177)</f>
+        <v>1.18102571084899</v>
+      </c>
+      <c r="G177" s="11" t="n">
+        <f aca="false">F177/E177</f>
+        <v>0.0633729020032998</v>
+      </c>
+    </row>
+    <row r="178" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A178" s="8" t="s">
+        <v>182</v>
+      </c>
+      <c r="B178" s="9" t="n">
+        <v>21.0068734898088</v>
+      </c>
+      <c r="C178" s="9" t="n">
+        <v>20.2095713790577</v>
+      </c>
+      <c r="D178" s="10" t="n">
+        <v>20.3868681042213</v>
+      </c>
+      <c r="E178" s="8" t="n">
+        <f aca="false">AVERAGE(B178:D178)</f>
+        <v>20.5344376576959</v>
+      </c>
+      <c r="F178" s="8" t="n">
+        <f aca="false">_xlfn.STDEV.P(B178:D178)</f>
+        <v>0.341814027200541</v>
+      </c>
+      <c r="G178" s="11" t="n">
+        <f aca="false">F178/E178</f>
+        <v>0.016645891789125</v>
+      </c>
+    </row>
+    <row r="179" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A179" s="8" t="s">
+        <v>183</v>
+      </c>
+      <c r="B179" s="9" t="n">
+        <v>19.6826103529755</v>
+      </c>
+      <c r="C179" s="9" t="n">
+        <v>18.3514596057298</v>
+      </c>
+      <c r="D179" s="10" t="n">
+        <v>18.3986363756362</v>
+      </c>
+      <c r="E179" s="8" t="n">
+        <f aca="false">AVERAGE(B179:D179)</f>
+        <v>18.8109021114472</v>
+      </c>
+      <c r="F179" s="8" t="n">
+        <f aca="false">_xlfn.STDEV.P(B179:D179)</f>
+        <v>0.616691633187934</v>
+      </c>
+      <c r="G179" s="11" t="n">
+        <f aca="false">F179/E179</f>
+        <v>0.0327837351730544</v>
+      </c>
+    </row>
+    <row r="180" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A180" s="12" t="s">
+        <v>184</v>
+      </c>
+      <c r="B180" s="9" t="n">
+        <v>208.888888888889</v>
+      </c>
+      <c r="C180" s="9" t="n">
+        <v>173.796296296296</v>
+      </c>
+      <c r="D180" s="10" t="n">
+        <v>160.462962962963</v>
+      </c>
+      <c r="E180" s="12" t="n">
+        <f aca="false">AVERAGE(B180:D180)</f>
+        <v>181.049382716049</v>
+      </c>
+      <c r="F180" s="12" t="n">
+        <f aca="false">_xlfn.STDEV.P(B180:D180)</f>
+        <v>20.424218016938</v>
+      </c>
+      <c r="G180" s="13" t="n">
+        <f aca="false">F180/E180</f>
+        <v>0.112810205207772</v>
       </c>
     </row>
   </sheetData>

</xml_diff>